<commit_message>
new images and changes to excel for key and image mapping
</commit_message>
<xml_diff>
--- a/prep/StreamdeckIconInputKeyMapping.xlsx
+++ b/prep/StreamdeckIconInputKeyMapping.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irene\src\biz.dfch.PhoneTap\prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9263FA0F-73FE-4C8F-A5DC-691F1CD741F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30632FBB-4119-437C-8C2A-935C9722D40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{4419FAFA-D280-4090-97B7-CB07F6B7BE60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$129</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="138">
   <si>
     <t>States</t>
   </si>
@@ -146,9 +149,6 @@
     <t>ic_fluent_speaker_2_48_regular.svg</t>
   </si>
   <si>
-    <t>ic_fluent_speaker_off_48_regular.svg</t>
-  </si>
-  <si>
     <t xml:space="preserve">        HELP = InputEventMap.KEY_ASTERISK</t>
   </si>
   <si>
@@ -158,21 +158,6 @@
     <t>        SKIP_DEVICE = InputEventMap.KEY_2</t>
   </si>
   <si>
-    <t>ic_fluent_phone_checkmark_20_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_phone_dismiss_24_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_keyboard_24_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_dismiss_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_speaker_box_24_regular.svg</t>
-  </si>
-  <si>
     <t>        FORMAT_DEVICE = InputEventMap.KEY_6</t>
   </si>
   <si>
@@ -188,18 +173,6 @@
     <t>ic_fluent_usb_stick_24_regular.svg</t>
   </si>
   <si>
-    <t>ic_fluent_pen_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_broom_32_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_arrow_autofit_up_24_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_arrow_autofit_down_24_regular.svg</t>
-  </si>
-  <si>
     <t>        START_RECORDING_MX0 = InputEventMap.KEY_1</t>
   </si>
   <si>
@@ -456,6 +429,30 @@
   </si>
   <si>
     <t>ic_fluent_local_language_28_regular.svg</t>
+  </si>
+  <si>
+    <t>ic_fluent_home_48_regular.svg</t>
+  </si>
+  <si>
+    <t>ic_fluent_eraser_24_regular.svg</t>
+  </si>
+  <si>
+    <t>ic_fluent_search_48_regular.svg</t>
+  </si>
+  <si>
+    <t>ic_fluent_skip_forward_tab_24_regular.svg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        SCREEN = InputEventMap.KEY_ASTERISK</t>
+  </si>
+  <si>
+    <t>ic_fluent_database_warning_20_regular.svg</t>
+  </si>
+  <si>
+    <t>ic_fluent_database_checkmark_24_regular.svg</t>
+  </si>
+  <si>
+    <t>ic_fluent_database_arrow_down_20_regular.svg</t>
   </si>
 </sst>
 </file>
@@ -842,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47861C0B-96C3-4FC0-B828-7FD785B358D7}">
-  <dimension ref="A1:I128"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -952,7 +949,7 @@
         <v>menu</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F47" si="3">"KEY_" &amp; CHOOSE(
+        <f t="shared" ref="F3:F48" si="3">"KEY_" &amp; CHOOSE(
     D3+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
@@ -1047,7 +1044,7 @@
         <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>133</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -1078,7 +1075,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -1112,10 +1109,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1146,10 +1143,10 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>133</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -1180,7 +1177,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -1214,10 +1211,10 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -1248,10 +1245,10 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>133</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -1282,7 +1279,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1316,10 +1313,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -1350,10 +1347,10 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
       <c r="D15">
         <v>6</v>
@@ -1384,7 +1381,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -1418,10 +1415,10 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -1452,10 +1449,10 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
       <c r="D18">
         <v>6</v>
@@ -1486,7 +1483,7 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -1520,10 +1517,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="D20">
         <v>5</v>
@@ -1554,10 +1551,10 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
       <c r="D21">
         <v>6</v>
@@ -1588,7 +1585,7 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -1622,10 +1619,10 @@
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>132</v>
       </c>
       <c r="D23">
         <v>5</v>
@@ -1656,10 +1653,10 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
       <c r="D24">
         <v>6</v>
@@ -1690,7 +1687,7 @@
         <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -1732,10 +1729,10 @@
         <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>132</v>
       </c>
       <c r="D26">
         <v>5</v>
@@ -1766,10 +1763,10 @@
         <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
       <c r="D27">
         <v>6</v>
@@ -1800,10 +1797,10 @@
         <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>135</v>
       </c>
       <c r="D28">
         <v>10</v>
@@ -1834,10 +1831,10 @@
         <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>52</v>
+        <v>136</v>
       </c>
       <c r="D29">
         <v>11</v>
@@ -1868,10 +1865,10 @@
         <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>137</v>
       </c>
       <c r="D30">
         <v>12</v>
@@ -1902,10 +1899,10 @@
         <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="D31">
         <v>13</v>
@@ -1936,7 +1933,7 @@
         <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -1970,16 +1967,16 @@
         <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>132</v>
       </c>
       <c r="D33">
         <v>5</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" ref="E33:E39" si="9">LOWER(
+        <f t="shared" ref="E33:E40" si="9">LOWER(
   TRIM(
     SUBSTITUTE(
       LEFT(B33, FIND(" = InputEventMap", B33) - 1),
@@ -1995,15 +1992,15 @@
         <v>KEY_05</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" ref="G33:G39" si="10">_xlfn.CONCAT(A33, "-", F33, "-", E33, ".png")</f>
+        <f t="shared" ref="G33:G40" si="10">_xlfn.CONCAT(A33, "-", F33, "-", E33, ".png")</f>
         <v>InitialiseRc2-KEY_05-detect_device.png</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" ref="H33:H39" si="11">MID(B33, FIND("InputEventMap", B33), LEN(B33))</f>
+        <f t="shared" ref="H33:H40" si="11">MID(B33, FIND("InputEventMap", B33), LEN(B33))</f>
         <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I33" t="str">
-        <f t="shared" ref="I33:I39" si="12">_xlfn.CONCAT("StreamdeckInput.", F33, ": ", H33, ",")</f>
+        <f t="shared" ref="I33:I40" si="12">_xlfn.CONCAT("StreamdeckInput.", F33, ": ", H33, ",")</f>
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
@@ -2012,10 +2009,10 @@
         <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
       <c r="D34">
         <v>6</v>
@@ -2046,10 +2043,10 @@
         <v>19</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>50</v>
+        <v>135</v>
       </c>
       <c r="D35">
         <v>10</v>
@@ -2080,10 +2077,10 @@
         <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>52</v>
+        <v>136</v>
       </c>
       <c r="D36">
         <v>11</v>
@@ -2114,10 +2111,10 @@
         <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>53</v>
+        <v>137</v>
       </c>
       <c r="D37">
         <v>12</v>
@@ -2148,10 +2145,10 @@
         <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="D38">
         <v>13</v>
@@ -2182,33 +2179,44 @@
         <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>134</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
+        <v>130</v>
       </c>
       <c r="D39">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="9"/>
-        <v>help</v>
+        <f t="shared" ref="E39" si="13">LOWER(
+  TRIM(
+    SUBSTITUTE(
+      LEFT(B39, FIND(" = InputEventMap", B39) - 1),
+      CHAR(160),
+      " "
+    )
+  )
+)</f>
+        <v>screen</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="3"/>
-        <v>KEY_04</v>
+        <f t="shared" ref="F39" si="14">"KEY_" &amp; CHOOSE(
+    D39+1,
+    "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
+)</f>
+        <v>KEY_00</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="10"/>
-        <v>Main-KEY_04-help.png</v>
+        <f t="shared" ref="G39" si="15">_xlfn.CONCAT(A39, "-", F39, "-", E39, ".png")</f>
+        <v>Main-KEY_00-screen.png</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="H39" si="16">MID(B39, FIND("InputEventMap", B39), LEN(B39))</f>
         <v>InputEventMap.KEY_ASTERISK</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" si="12"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
+        <f t="shared" ref="I39" si="17">_xlfn.CONCAT("StreamdeckInput.", F39, ": ", H39, ",")</f>
+        <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
@@ -2216,19 +2224,53 @@
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="9"/>
+        <v>help</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="3"/>
+        <v>KEY_04</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="10"/>
+        <v>Main-KEY_04-help.png</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="11"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="12"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41">
         <v>5</v>
       </c>
-      <c r="E40" t="str">
-        <f t="shared" ref="E40:E47" si="13">LOWER(
+      <c r="E41" t="str">
+        <f t="shared" ref="E41:E48" si="18">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B40, FIND(" = InputEventMap", B40) - 1),
+      LEFT(B41, FIND(" = InputEventMap", B41) - 1),
       CHAR(160),
       " "
     )
@@ -2236,55 +2278,21 @@
 )</f>
         <v>start_recording_mx0</v>
       </c>
-      <c r="F40" t="str">
+      <c r="F41" t="str">
         <f t="shared" si="3"/>
         <v>KEY_05</v>
       </c>
-      <c r="G40" t="str">
-        <f t="shared" ref="G40:G45" si="14">_xlfn.CONCAT(A40, "-", F40, "-", E40, ".png")</f>
+      <c r="G41" t="str">
+        <f t="shared" ref="G41:G46" si="19">_xlfn.CONCAT(A41, "-", F41, "-", E41, ".png")</f>
         <v>Main-KEY_05-start_recording_mx0.png</v>
       </c>
-      <c r="H40" t="str">
-        <f t="shared" ref="H40:H45" si="15">MID(B40, FIND("InputEventMap", B40), LEN(B40))</f>
+      <c r="H41" t="str">
+        <f t="shared" ref="H41:H46" si="20">MID(B41, FIND("InputEventMap", B41), LEN(B41))</f>
         <v>InputEventMap.KEY_1</v>
       </c>
-      <c r="I40" t="str">
-        <f t="shared" ref="I40:I45" si="16">_xlfn.CONCAT("StreamdeckInput.", F40, ": ", H40, ",")</f>
+      <c r="I41" t="str">
+        <f t="shared" ref="I41:I46" si="21">_xlfn.CONCAT("StreamdeckInput.", F41, ": ", H41, ",")</f>
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" t="s">
-        <v>60</v>
-      </c>
-      <c r="D41">
-        <v>6</v>
-      </c>
-      <c r="E41" t="str">
-        <f t="shared" si="13"/>
-        <v>start_recording_mx1</v>
-      </c>
-      <c r="F41" t="str">
-        <f t="shared" si="3"/>
-        <v>KEY_06</v>
-      </c>
-      <c r="G41" t="str">
-        <f t="shared" si="14"/>
-        <v>Main-KEY_06-start_recording_mx1.png</v>
-      </c>
-      <c r="H41" t="str">
-        <f t="shared" si="15"/>
-        <v>InputEventMap.KEY_2</v>
-      </c>
-      <c r="I41" t="str">
-        <f t="shared" si="16"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
@@ -2292,33 +2300,33 @@
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D42">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="13"/>
-        <v>start_recording_mx2</v>
+        <f t="shared" si="18"/>
+        <v>start_recording_mx1</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="3"/>
-        <v>KEY_07</v>
+        <v>KEY_06</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="14"/>
-        <v>Main-KEY_07-start_recording_mx2.png</v>
+        <f t="shared" si="19"/>
+        <v>Main-KEY_06-start_recording_mx1.png</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="15"/>
-        <v>InputEventMap.KEY_3</v>
+        <f t="shared" si="20"/>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I42" t="str">
-        <f t="shared" si="16"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
+        <f t="shared" si="21"/>
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
@@ -2326,33 +2334,33 @@
         <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D43">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="13"/>
-        <v>start_playback</v>
+        <f t="shared" si="18"/>
+        <v>start_recording_mx2</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="3"/>
-        <v>KEY_0A</v>
+        <v>KEY_07</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="14"/>
-        <v>Main-KEY_0A-start_playback.png</v>
+        <f t="shared" si="19"/>
+        <v>Main-KEY_07-start_recording_mx2.png</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="15"/>
-        <v>InputEventMap.KEY_4</v>
+        <f t="shared" si="20"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I43" t="str">
-        <f t="shared" si="16"/>
-        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_4,</v>
+        <f t="shared" si="21"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
@@ -2360,33 +2368,33 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="D44">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="13"/>
-        <v>menu</v>
+        <f t="shared" si="18"/>
+        <v>start_playback</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="3"/>
-        <v>KEY_09</v>
+        <v>KEY_0A</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="14"/>
-        <v>Main-KEY_09-menu.png</v>
+        <f t="shared" si="19"/>
+        <v>Main-KEY_0A-start_playback.png</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="15"/>
-        <v>InputEventMap.KEY_5</v>
+        <f t="shared" si="20"/>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I44" t="str">
-        <f t="shared" si="16"/>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
+        <f t="shared" si="21"/>
+        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_4,</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
@@ -2394,33 +2402,33 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
       <c r="D45">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="13"/>
-        <v>set_name</v>
+        <f t="shared" si="18"/>
+        <v>menu</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="3"/>
-        <v>KEY_0B</v>
+        <v>KEY_09</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="14"/>
-        <v>Main-KEY_0B-set_name.png</v>
+        <f t="shared" si="19"/>
+        <v>Main-KEY_09-menu.png</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="15"/>
-        <v>InputEventMap.KEY_6</v>
+        <f t="shared" si="20"/>
+        <v>InputEventMap.KEY_5</v>
       </c>
       <c r="I45" t="str">
-        <f t="shared" si="16"/>
-        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_6,</v>
+        <f t="shared" si="21"/>
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
@@ -2428,67 +2436,67 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D46">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E46" t="str">
-        <f t="shared" si="13"/>
-        <v>stop_system</v>
+        <f t="shared" si="18"/>
+        <v>set_name</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="3"/>
-        <v>KEY_0E</v>
+        <v>KEY_0B</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" ref="G46:G47" si="17">_xlfn.CONCAT(A46, "-", F46, "-", E46, ".png")</f>
-        <v>Main-KEY_0E-stop_system.png</v>
+        <f t="shared" si="19"/>
+        <v>Main-KEY_0B-set_name.png</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" ref="H46:H47" si="18">MID(B46, FIND("InputEventMap", B46), LEN(B46))</f>
-        <v>InputEventMap.KEY_9</v>
+        <f t="shared" si="20"/>
+        <v>InputEventMap.KEY_6</v>
       </c>
       <c r="I46" t="str">
-        <f t="shared" ref="I46:I47" si="19">_xlfn.CONCAT("StreamdeckInput.", F46, ": ", H46, ",")</f>
-        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_9,</v>
+        <f t="shared" si="21"/>
+        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_6,</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="C47" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="D47">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="13"/>
-        <v>help</v>
+        <f t="shared" si="18"/>
+        <v>stop_system</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="3"/>
-        <v>KEY_04</v>
+        <v>KEY_0E</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="17"/>
-        <v>OnRecord-KEY_04-help.png</v>
+        <f t="shared" ref="G47:G48" si="22">_xlfn.CONCAT(A47, "-", F47, "-", E47, ".png")</f>
+        <v>Main-KEY_0E-stop_system.png</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="18"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
+        <f t="shared" ref="H47:H48" si="23">MID(B47, FIND("InputEventMap", B47), LEN(B47))</f>
+        <v>InputEventMap.KEY_9</v>
       </c>
       <c r="I47" t="str">
-        <f t="shared" si="19"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
+        <f t="shared" ref="I47:I48" si="24">_xlfn.CONCAT("StreamdeckInput.", F47, ": ", H47, ",")</f>
+        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_9,</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
@@ -2496,19 +2504,53 @@
         <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="D48">
+        <v>4</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="18"/>
+        <v>help</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="3"/>
+        <v>KEY_04</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="22"/>
+        <v>OnRecord-KEY_04-help.png</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="23"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="24"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49">
         <v>6</v>
       </c>
-      <c r="E48" t="str">
-        <f t="shared" ref="E48:E51" si="20">LOWER(
+      <c r="E49" t="str">
+        <f t="shared" ref="E49:E52" si="25">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B48, FIND(" = InputEventMap", B48) - 1),
+      LEFT(B49, FIND(" = InputEventMap", B49) - 1),
       CHAR(160),
       " "
     )
@@ -2516,58 +2558,24 @@
 )</f>
         <v>stop_recording</v>
       </c>
-      <c r="F48" t="str">
-        <f t="shared" ref="F48:F51" si="21">"KEY_" &amp; CHOOSE(
-    D48+1,
+      <c r="F49" t="str">
+        <f t="shared" ref="F49:F52" si="26">"KEY_" &amp; CHOOSE(
+    D49+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_06</v>
       </c>
-      <c r="G48" t="str">
-        <f t="shared" ref="G48:G51" si="22">_xlfn.CONCAT(A48, "-", F48, "-", E48, ".png")</f>
+      <c r="G49" t="str">
+        <f t="shared" ref="G49:G52" si="27">_xlfn.CONCAT(A49, "-", F49, "-", E49, ".png")</f>
         <v>OnRecord-KEY_06-stop_recording.png</v>
       </c>
-      <c r="H48" t="str">
-        <f t="shared" ref="H48:H51" si="23">MID(B48, FIND("InputEventMap", B48), LEN(B48))</f>
+      <c r="H49" t="str">
+        <f t="shared" ref="H49:H52" si="28">MID(B49, FIND("InputEventMap", B49), LEN(B49))</f>
         <v>InputEventMap.KEY_1</v>
       </c>
-      <c r="I48" t="str">
-        <f t="shared" ref="I48:I51" si="24">_xlfn.CONCAT("StreamdeckInput.", F48, ": ", H48, ",")</f>
+      <c r="I49" t="str">
+        <f t="shared" ref="I49:I52" si="29">_xlfn.CONCAT("StreamdeckInput.", F49, ": ", H49, ",")</f>
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_1,</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
-        <v>20</v>
-      </c>
-      <c r="B49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C49" t="s">
-        <v>69</v>
-      </c>
-      <c r="D49">
-        <v>5</v>
-      </c>
-      <c r="E49" t="str">
-        <f t="shared" si="20"/>
-        <v>set_cue</v>
-      </c>
-      <c r="F49" t="str">
-        <f t="shared" si="21"/>
-        <v>KEY_05</v>
-      </c>
-      <c r="G49" t="str">
-        <f t="shared" si="22"/>
-        <v>OnRecord-KEY_05-set_cue.png</v>
-      </c>
-      <c r="H49" t="str">
-        <f t="shared" si="23"/>
-        <v>InputEventMap.KEY_2</v>
-      </c>
-      <c r="I49" t="str">
-        <f t="shared" si="24"/>
-        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.45">
@@ -2575,33 +2583,33 @@
         <v>20</v>
       </c>
       <c r="B50" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C50" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D50">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" si="20"/>
-        <v>toggle_mute</v>
+        <f t="shared" si="25"/>
+        <v>set_cue</v>
       </c>
       <c r="F50" t="str">
-        <f t="shared" si="21"/>
-        <v>KEY_07</v>
+        <f t="shared" si="26"/>
+        <v>KEY_05</v>
       </c>
       <c r="G50" t="str">
-        <f t="shared" si="22"/>
-        <v>OnRecord-KEY_07-toggle_mute.png</v>
+        <f t="shared" si="27"/>
+        <v>OnRecord-KEY_05-set_cue.png</v>
       </c>
       <c r="H50" t="str">
-        <f t="shared" si="23"/>
-        <v>InputEventMap.KEY_3</v>
+        <f t="shared" si="28"/>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I50" t="str">
-        <f t="shared" si="24"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
+        <f t="shared" si="29"/>
+        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.45">
@@ -2609,53 +2617,87 @@
         <v>20</v>
       </c>
       <c r="B51" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C51" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D51">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="20"/>
-        <v>show_status</v>
+        <f t="shared" si="25"/>
+        <v>toggle_mute</v>
       </c>
       <c r="F51" t="str">
-        <f t="shared" si="21"/>
-        <v>KEY_0A</v>
+        <f t="shared" si="26"/>
+        <v>KEY_07</v>
       </c>
       <c r="G51" t="str">
-        <f t="shared" si="22"/>
-        <v>OnRecord-KEY_0A-show_status.png</v>
+        <f t="shared" si="27"/>
+        <v>OnRecord-KEY_07-toggle_mute.png</v>
       </c>
       <c r="H51" t="str">
-        <f t="shared" si="23"/>
-        <v>InputEventMap.KEY_4</v>
+        <f t="shared" si="28"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I51" t="str">
-        <f t="shared" si="24"/>
-        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_4,</v>
+        <f t="shared" si="29"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" t="s">
+        <v>57</v>
+      </c>
+      <c r="C52" t="s">
+        <v>61</v>
+      </c>
+      <c r="D52">
+        <v>10</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="25"/>
+        <v>show_status</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="26"/>
+        <v>KEY_0A</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="27"/>
+        <v>OnRecord-KEY_0A-show_status.png</v>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" si="28"/>
+        <v>InputEventMap.KEY_4</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="29"/>
+        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_4,</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
         <v>31</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>6</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>4</v>
       </c>
-      <c r="D52">
+      <c r="D53">
         <v>4</v>
       </c>
-      <c r="E52" t="str">
-        <f t="shared" ref="E52:E113" si="25">LOWER(
+      <c r="E53" t="str">
+        <f t="shared" ref="E53:E114" si="30">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B52, FIND(" = InputEventMap", B52) - 1),
+      LEFT(B53, FIND(" = InputEventMap", B53) - 1),
       CHAR(160),
       " "
     )
@@ -2663,58 +2705,24 @@
 )</f>
         <v>help</v>
       </c>
-      <c r="F52" t="str">
-        <f t="shared" ref="F52:F113" si="26">"KEY_" &amp; CHOOSE(
-    D52+1,
+      <c r="F53" t="str">
+        <f t="shared" ref="F53:F114" si="31">"KEY_" &amp; CHOOSE(
+    D53+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_04</v>
       </c>
-      <c r="G52" t="str">
-        <f t="shared" ref="G52:G113" si="27">_xlfn.CONCAT(A52, "-", F52, "-", E52, ".png")</f>
+      <c r="G53" t="str">
+        <f t="shared" ref="G53:G114" si="32">_xlfn.CONCAT(A53, "-", F53, "-", E53, ".png")</f>
         <v>PlaybackPaused-KEY_04-help.png</v>
       </c>
-      <c r="H52" t="str">
-        <f t="shared" ref="H52:H113" si="28">MID(B52, FIND("InputEventMap", B52), LEN(B52))</f>
+      <c r="H53" t="str">
+        <f t="shared" ref="H53:H114" si="33">MID(B53, FIND("InputEventMap", B53), LEN(B53))</f>
         <v>InputEventMap.KEY_ASTERISK</v>
       </c>
-      <c r="I52" t="str">
-        <f t="shared" ref="I52:I113" si="29">_xlfn.CONCAT("StreamdeckInput.", F52, ": ", H52, ",")</f>
+      <c r="I53" t="str">
+        <f t="shared" ref="I53:I114" si="34">_xlfn.CONCAT("StreamdeckInput.", F53, ": ", H53, ",")</f>
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
-        <v>31</v>
-      </c>
-      <c r="B53" t="s">
-        <v>72</v>
-      </c>
-      <c r="C53" t="s">
-        <v>61</v>
-      </c>
-      <c r="D53">
-        <v>5</v>
-      </c>
-      <c r="E53" t="str">
-        <f t="shared" si="25"/>
-        <v>pause_resume</v>
-      </c>
-      <c r="F53" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_05</v>
-      </c>
-      <c r="G53" t="str">
-        <f t="shared" si="27"/>
-        <v>PlaybackPaused-KEY_05-pause_resume.png</v>
-      </c>
-      <c r="H53" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_0</v>
-      </c>
-      <c r="I53" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_0,</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.45">
@@ -2722,67 +2730,67 @@
         <v>31</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="C54" t="s">
+        <v>51</v>
+      </c>
+      <c r="D54">
         <v>5</v>
       </c>
-      <c r="D54">
-        <v>9</v>
-      </c>
       <c r="E54" t="str">
-        <f t="shared" si="25"/>
-        <v>menu</v>
+        <f t="shared" si="30"/>
+        <v>pause_resume</v>
       </c>
       <c r="F54" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_09</v>
+        <f t="shared" si="31"/>
+        <v>KEY_05</v>
       </c>
       <c r="G54" t="str">
-        <f t="shared" si="27"/>
-        <v>PlaybackPaused-KEY_09-menu.png</v>
+        <f t="shared" si="32"/>
+        <v>PlaybackPaused-KEY_05-pause_resume.png</v>
       </c>
       <c r="H54" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_5</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_0</v>
       </c>
       <c r="I54" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_0,</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D55">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" si="25"/>
-        <v>help</v>
+        <f t="shared" si="30"/>
+        <v>menu</v>
       </c>
       <c r="F55" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_04</v>
+        <f t="shared" si="31"/>
+        <v>KEY_09</v>
       </c>
       <c r="G55" t="str">
-        <f t="shared" si="27"/>
-        <v>Playback-KEY_04-help.png</v>
+        <f t="shared" si="32"/>
+        <v>PlaybackPaused-KEY_09-menu.png</v>
       </c>
       <c r="H55" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_5</v>
       </c>
       <c r="I55" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.45">
@@ -2790,33 +2798,33 @@
         <v>30</v>
       </c>
       <c r="B56" t="s">
-        <v>72</v>
+        <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="D56">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" si="25"/>
-        <v>pause_resume</v>
+        <f t="shared" si="30"/>
+        <v>help</v>
       </c>
       <c r="F56" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_07</v>
+        <f t="shared" si="31"/>
+        <v>KEY_04</v>
       </c>
       <c r="G56" t="str">
-        <f t="shared" si="27"/>
-        <v>Playback-KEY_07-pause_resume.png</v>
+        <f t="shared" si="32"/>
+        <v>Playback-KEY_04-help.png</v>
       </c>
       <c r="H56" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_0</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
       </c>
       <c r="I56" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_0,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
@@ -2824,33 +2832,33 @@
         <v>30</v>
       </c>
       <c r="B57" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C57" t="s">
-        <v>114</v>
+        <v>51</v>
       </c>
       <c r="D57">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="25"/>
-        <v>jump_clip_end</v>
+        <f t="shared" si="30"/>
+        <v>pause_resume</v>
       </c>
       <c r="F57" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0B</v>
+        <f t="shared" si="31"/>
+        <v>KEY_07</v>
       </c>
       <c r="G57" t="str">
-        <f t="shared" si="27"/>
-        <v>Playback-KEY_0B-jump_clip_end.png</v>
+        <f t="shared" si="32"/>
+        <v>Playback-KEY_07-pause_resume.png</v>
       </c>
       <c r="H57" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_1</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_0</v>
       </c>
       <c r="I57" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_0,</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.45">
@@ -2858,33 +2866,33 @@
         <v>30</v>
       </c>
       <c r="B58" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C58" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D58">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="25"/>
-        <v>seek_next</v>
+        <f t="shared" si="30"/>
+        <v>jump_clip_end</v>
       </c>
       <c r="F58" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0C</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0B</v>
       </c>
       <c r="G58" t="str">
-        <f t="shared" si="27"/>
-        <v>Playback-KEY_0C-seek_next.png</v>
+        <f t="shared" si="32"/>
+        <v>Playback-KEY_0B-jump_clip_end.png</v>
       </c>
       <c r="H58" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_2</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I58" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.45">
@@ -2892,33 +2900,33 @@
         <v>30</v>
       </c>
       <c r="B59" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C59" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D59">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="25"/>
-        <v>jump_cue_next</v>
+        <f t="shared" si="30"/>
+        <v>seek_next</v>
       </c>
       <c r="F59" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0D</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0C</v>
       </c>
       <c r="G59" t="str">
-        <f t="shared" si="27"/>
-        <v>Playback-KEY_0D-jump_cue_next.png</v>
+        <f t="shared" si="32"/>
+        <v>Playback-KEY_0C-seek_next.png</v>
       </c>
       <c r="H59" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_3</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I59" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
@@ -2926,33 +2934,33 @@
         <v>30</v>
       </c>
       <c r="B60" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C60" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="D60">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E60" t="str">
-        <f t="shared" si="25"/>
-        <v>jump_clip_previous</v>
+        <f t="shared" si="30"/>
+        <v>jump_cue_next</v>
       </c>
       <c r="F60" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_06</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0D</v>
       </c>
       <c r="G60" t="str">
-        <f t="shared" si="27"/>
-        <v>Playback-KEY_06-jump_clip_previous.png</v>
+        <f t="shared" si="32"/>
+        <v>Playback-KEY_0D-jump_cue_next.png</v>
       </c>
       <c r="H60" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_4</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I60" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.45">
@@ -2960,33 +2968,33 @@
         <v>30</v>
       </c>
       <c r="B61" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="C61" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="D61">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E61" t="str">
-        <f t="shared" si="25"/>
-        <v>menu</v>
+        <f t="shared" si="30"/>
+        <v>jump_clip_previous</v>
       </c>
       <c r="F61" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_09</v>
+        <f t="shared" si="31"/>
+        <v>KEY_06</v>
       </c>
       <c r="G61" t="str">
-        <f t="shared" si="27"/>
-        <v>Playback-KEY_09-menu.png</v>
+        <f t="shared" si="32"/>
+        <v>Playback-KEY_06-jump_clip_previous.png</v>
       </c>
       <c r="H61" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_5</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I61" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.45">
@@ -2994,33 +3002,33 @@
         <v>30</v>
       </c>
       <c r="B62" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="C62" t="s">
-        <v>117</v>
+        <v>5</v>
       </c>
       <c r="D62">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E62" t="str">
-        <f t="shared" si="25"/>
-        <v>jump_clip_next</v>
+        <f t="shared" si="30"/>
+        <v>menu</v>
       </c>
       <c r="F62" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_08</v>
+        <f t="shared" si="31"/>
+        <v>KEY_09</v>
       </c>
       <c r="G62" t="str">
-        <f t="shared" si="27"/>
-        <v>Playback-KEY_08-jump_clip_next.png</v>
+        <f t="shared" si="32"/>
+        <v>Playback-KEY_09-menu.png</v>
       </c>
       <c r="H62" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_6</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_5</v>
       </c>
       <c r="I62" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.45">
@@ -3028,33 +3036,33 @@
         <v>30</v>
       </c>
       <c r="B63" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C63" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D63">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E63" t="str">
-        <f t="shared" si="25"/>
-        <v>jump_clip_start</v>
+        <f t="shared" si="30"/>
+        <v>jump_clip_next</v>
       </c>
       <c r="F63" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_02</v>
+        <f t="shared" si="31"/>
+        <v>KEY_08</v>
       </c>
       <c r="G63" t="str">
-        <f t="shared" si="27"/>
-        <v>Playback-KEY_02-jump_clip_start.png</v>
+        <f t="shared" si="32"/>
+        <v>Playback-KEY_08-jump_clip_next.png</v>
       </c>
       <c r="H63" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_7</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_6</v>
       </c>
       <c r="I63" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_7,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.45">
@@ -3062,33 +3070,33 @@
         <v>30</v>
       </c>
       <c r="B64" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C64" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D64">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E64" t="str">
-        <f t="shared" si="25"/>
-        <v>seek_previous</v>
+        <f t="shared" si="30"/>
+        <v>jump_clip_start</v>
       </c>
       <c r="F64" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_03</v>
+        <f t="shared" si="31"/>
+        <v>KEY_02</v>
       </c>
       <c r="G64" t="str">
-        <f t="shared" si="27"/>
-        <v>Playback-KEY_03-seek_previous.png</v>
+        <f t="shared" si="32"/>
+        <v>Playback-KEY_02-jump_clip_start.png</v>
       </c>
       <c r="H64" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_8</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_7</v>
       </c>
       <c r="I64" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_8,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_7,</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.45">
@@ -3096,67 +3104,67 @@
         <v>30</v>
       </c>
       <c r="B65" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C65" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D65">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E65" t="str">
-        <f t="shared" si="25"/>
-        <v>jump_cue_previous</v>
+        <f t="shared" si="30"/>
+        <v>seek_previous</v>
       </c>
       <c r="F65" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_04</v>
+        <f t="shared" si="31"/>
+        <v>KEY_03</v>
       </c>
       <c r="G65" t="str">
-        <f t="shared" si="27"/>
-        <v>Playback-KEY_04-jump_cue_previous.png</v>
+        <f t="shared" si="32"/>
+        <v>Playback-KEY_03-seek_previous.png</v>
       </c>
       <c r="H65" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_9</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_8</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_9,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_8,</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B66" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="C66" t="s">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="D66">
         <v>4</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" si="25"/>
-        <v>help</v>
+        <f t="shared" si="30"/>
+        <v>jump_cue_previous</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>KEY_04</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" si="27"/>
-        <v>SelectLanguage-KEY_04-help.png</v>
+        <f t="shared" si="32"/>
+        <v>Playback-KEY_04-jump_cue_previous.png</v>
       </c>
       <c r="H66" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_9</v>
       </c>
       <c r="I66" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_9,</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
@@ -3164,33 +3172,33 @@
         <v>26</v>
       </c>
       <c r="B67" t="s">
-        <v>81</v>
+        <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>121</v>
+        <v>4</v>
       </c>
       <c r="D67">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" si="25"/>
-        <v>select_english</v>
+        <f t="shared" si="30"/>
+        <v>help</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_05</v>
+        <f t="shared" si="31"/>
+        <v>KEY_04</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" si="27"/>
-        <v>SelectLanguage-KEY_05-select_english.png</v>
+        <f t="shared" si="32"/>
+        <v>SelectLanguage-KEY_04-help.png</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_1</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.45">
@@ -3198,33 +3206,33 @@
         <v>26</v>
       </c>
       <c r="B68" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C68" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D68">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="25"/>
-        <v>select_german</v>
+        <f t="shared" si="30"/>
+        <v>select_english</v>
       </c>
       <c r="F68" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_06</v>
+        <f t="shared" si="31"/>
+        <v>KEY_05</v>
       </c>
       <c r="G68" t="str">
-        <f t="shared" si="27"/>
-        <v>SelectLanguage-KEY_06-select_german.png</v>
+        <f t="shared" si="32"/>
+        <v>SelectLanguage-KEY_05-select_english.png</v>
       </c>
       <c r="H68" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_2</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I68" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.45">
@@ -3232,33 +3240,33 @@
         <v>26</v>
       </c>
       <c r="B69" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C69" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="D69">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="25"/>
-        <v>select_french</v>
+        <f t="shared" si="30"/>
+        <v>select_german</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_07</v>
+        <f t="shared" si="31"/>
+        <v>KEY_06</v>
       </c>
       <c r="G69" t="str">
-        <f t="shared" si="27"/>
-        <v>SelectLanguage-KEY_07-select_french.png</v>
+        <f t="shared" si="32"/>
+        <v>SelectLanguage-KEY_06-select_german.png</v>
       </c>
       <c r="H69" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_3</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I69" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.45">
@@ -3266,67 +3274,67 @@
         <v>26</v>
       </c>
       <c r="B70" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C70" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D70">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="25"/>
-        <v>select_italian</v>
+        <f t="shared" si="30"/>
+        <v>select_french</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_08</v>
+        <f t="shared" si="31"/>
+        <v>KEY_07</v>
       </c>
       <c r="G70" t="str">
-        <f t="shared" si="27"/>
-        <v>SelectLanguage-KEY_08-select_italian.png</v>
+        <f t="shared" si="32"/>
+        <v>SelectLanguage-KEY_07-select_french.png</v>
       </c>
       <c r="H70" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_4</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I70" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_4,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B71" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="C71" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
       <c r="D71">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E71" t="str">
-        <f t="shared" si="25"/>
-        <v>help</v>
+        <f t="shared" si="30"/>
+        <v>select_italian</v>
       </c>
       <c r="F71" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_04</v>
+        <f t="shared" si="31"/>
+        <v>KEY_08</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" si="27"/>
-        <v>SetDate-KEY_04-help.png</v>
+        <f t="shared" si="32"/>
+        <v>SelectLanguage-KEY_08-select_italian.png</v>
       </c>
       <c r="H71" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I71" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_4,</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.45">
@@ -3334,33 +3342,33 @@
         <v>27</v>
       </c>
       <c r="B72" t="s">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>125</v>
+        <v>4</v>
       </c>
       <c r="D72">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E72" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_0</v>
+        <f t="shared" si="30"/>
+        <v>help</v>
       </c>
       <c r="F72" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0A</v>
+        <f t="shared" si="31"/>
+        <v>KEY_04</v>
       </c>
       <c r="G72" t="str">
-        <f t="shared" si="27"/>
-        <v>SetDate-KEY_0A-digit_0.png</v>
+        <f t="shared" si="32"/>
+        <v>SetDate-KEY_04-help.png</v>
       </c>
       <c r="H72" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_0</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
       </c>
       <c r="I72" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.45">
@@ -3368,33 +3376,33 @@
         <v>27</v>
       </c>
       <c r="B73" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C73" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D73">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E73" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_1</v>
+        <f t="shared" si="30"/>
+        <v>digit_0</v>
       </c>
       <c r="F73" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0B</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0A</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="27"/>
-        <v>SetDate-KEY_0B-digit_1.png</v>
+        <f t="shared" si="32"/>
+        <v>SetDate-KEY_0A-digit_0.png</v>
       </c>
       <c r="H73" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_1</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_0</v>
       </c>
       <c r="I73" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.45">
@@ -3402,33 +3410,33 @@
         <v>27</v>
       </c>
       <c r="B74" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C74" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D74">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E74" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_2</v>
+        <f t="shared" si="30"/>
+        <v>digit_1</v>
       </c>
       <c r="F74" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0C</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0B</v>
       </c>
       <c r="G74" t="str">
-        <f t="shared" si="27"/>
-        <v>SetDate-KEY_0C-digit_2.png</v>
+        <f t="shared" si="32"/>
+        <v>SetDate-KEY_0B-digit_1.png</v>
       </c>
       <c r="H74" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_2</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I74" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.45">
@@ -3436,33 +3444,33 @@
         <v>27</v>
       </c>
       <c r="B75" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C75" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D75">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E75" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_3</v>
+        <f t="shared" si="30"/>
+        <v>digit_2</v>
       </c>
       <c r="F75" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0D</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0C</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" si="27"/>
-        <v>SetDate-KEY_0D-digit_3.png</v>
+        <f t="shared" si="32"/>
+        <v>SetDate-KEY_0C-digit_2.png</v>
       </c>
       <c r="H75" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_3</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I75" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
@@ -3470,33 +3478,33 @@
         <v>27</v>
       </c>
       <c r="B76" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C76" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="D76">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E76" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_4</v>
+        <f t="shared" si="30"/>
+        <v>digit_3</v>
       </c>
       <c r="F76" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_06</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0D</v>
       </c>
       <c r="G76" t="str">
-        <f t="shared" si="27"/>
-        <v>SetDate-KEY_06-digit_4.png</v>
+        <f t="shared" si="32"/>
+        <v>SetDate-KEY_0D-digit_3.png</v>
       </c>
       <c r="H76" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_4</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I76" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.45">
@@ -3504,33 +3512,33 @@
         <v>27</v>
       </c>
       <c r="B77" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C77" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="D77">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E77" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_5</v>
+        <f t="shared" si="30"/>
+        <v>digit_4</v>
       </c>
       <c r="F77" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_07</v>
+        <f t="shared" si="31"/>
+        <v>KEY_06</v>
       </c>
       <c r="G77" t="str">
-        <f t="shared" si="27"/>
-        <v>SetDate-KEY_07-digit_5.png</v>
+        <f t="shared" si="32"/>
+        <v>SetDate-KEY_06-digit_4.png</v>
       </c>
       <c r="H77" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_5</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I77" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.45">
@@ -3538,33 +3546,33 @@
         <v>27</v>
       </c>
       <c r="B78" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C78" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="D78">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E78" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_6</v>
+        <f t="shared" si="30"/>
+        <v>digit_5</v>
       </c>
       <c r="F78" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_08</v>
+        <f t="shared" si="31"/>
+        <v>KEY_07</v>
       </c>
       <c r="G78" t="str">
-        <f t="shared" si="27"/>
-        <v>SetDate-KEY_08-digit_6.png</v>
+        <f t="shared" si="32"/>
+        <v>SetDate-KEY_07-digit_5.png</v>
       </c>
       <c r="H78" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_6</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_5</v>
       </c>
       <c r="I78" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.45">
@@ -3572,33 +3580,33 @@
         <v>27</v>
       </c>
       <c r="B79" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C79" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D79">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E79" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_7</v>
+        <f t="shared" si="30"/>
+        <v>digit_6</v>
       </c>
       <c r="F79" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_02</v>
+        <f t="shared" si="31"/>
+        <v>KEY_08</v>
       </c>
       <c r="G79" t="str">
-        <f t="shared" si="27"/>
-        <v>SetDate-KEY_02-digit_7.png</v>
+        <f t="shared" si="32"/>
+        <v>SetDate-KEY_08-digit_6.png</v>
       </c>
       <c r="H79" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_7</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_6</v>
       </c>
       <c r="I79" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_7,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.45">
@@ -3606,33 +3614,33 @@
         <v>27</v>
       </c>
       <c r="B80" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C80" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D80">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E80" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_8</v>
+        <f t="shared" si="30"/>
+        <v>digit_7</v>
       </c>
       <c r="F80" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_03</v>
+        <f t="shared" si="31"/>
+        <v>KEY_02</v>
       </c>
       <c r="G80" t="str">
-        <f t="shared" si="27"/>
-        <v>SetDate-KEY_03-digit_8.png</v>
+        <f t="shared" si="32"/>
+        <v>SetDate-KEY_02-digit_7.png</v>
       </c>
       <c r="H80" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_8</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_7</v>
       </c>
       <c r="I80" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_8,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_7,</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.45">
@@ -3640,33 +3648,33 @@
         <v>27</v>
       </c>
       <c r="B81" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C81" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D81">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E81" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_9</v>
+        <f t="shared" si="30"/>
+        <v>digit_8</v>
       </c>
       <c r="F81" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_04</v>
+        <f t="shared" si="31"/>
+        <v>KEY_03</v>
       </c>
       <c r="G81" t="str">
-        <f t="shared" si="27"/>
-        <v>SetDate-KEY_04-digit_9.png</v>
+        <f t="shared" si="32"/>
+        <v>SetDate-KEY_03-digit_8.png</v>
       </c>
       <c r="H81" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_9</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_8</v>
       </c>
       <c r="I81" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_9,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_8,</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.45">
@@ -3674,33 +3682,33 @@
         <v>27</v>
       </c>
       <c r="B82" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C82" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D82">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E82" t="str">
-        <f t="shared" si="25"/>
-        <v>back_space</v>
+        <f t="shared" si="30"/>
+        <v>digit_9</v>
       </c>
       <c r="F82" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_05</v>
+        <f t="shared" si="31"/>
+        <v>KEY_04</v>
       </c>
       <c r="G82" t="str">
-        <f t="shared" si="27"/>
-        <v>SetDate-KEY_05-back_space.png</v>
+        <f t="shared" si="32"/>
+        <v>SetDate-KEY_04-digit_9.png</v>
       </c>
       <c r="H82" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_BACKSPACE</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_9</v>
       </c>
       <c r="I82" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_9,</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.45">
@@ -3708,33 +3716,33 @@
         <v>27</v>
       </c>
       <c r="B83" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C83" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D83">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E83" t="str">
-        <f t="shared" si="25"/>
-        <v>enter</v>
+        <f t="shared" si="30"/>
+        <v>back_space</v>
       </c>
       <c r="F83" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0E</v>
+        <f t="shared" si="31"/>
+        <v>KEY_05</v>
       </c>
       <c r="G83" t="str">
-        <f t="shared" si="27"/>
-        <v>SetDate-KEY_0E-enter.png</v>
+        <f t="shared" si="32"/>
+        <v>SetDate-KEY_05-back_space.png</v>
       </c>
       <c r="H83" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_ENTER</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_BACKSPACE</v>
       </c>
       <c r="I83" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.45">
@@ -3742,67 +3750,67 @@
         <v>27</v>
       </c>
       <c r="B84" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C84" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="D84">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E84" t="str">
-        <f t="shared" si="25"/>
-        <v>jump_next</v>
+        <f t="shared" si="30"/>
+        <v>enter</v>
       </c>
       <c r="F84" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_09</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0E</v>
       </c>
       <c r="G84" t="str">
-        <f t="shared" si="27"/>
-        <v>SetDate-KEY_09-jump_next.png</v>
+        <f t="shared" si="32"/>
+        <v>SetDate-KEY_0E-enter.png</v>
       </c>
       <c r="H84" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_TAB</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_ENTER</v>
       </c>
       <c r="I84" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B85" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="C85" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D85">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E85" t="str">
-        <f t="shared" si="25"/>
-        <v>help</v>
+        <f t="shared" si="30"/>
+        <v>jump_next</v>
       </c>
       <c r="F85" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_04</v>
+        <f t="shared" si="31"/>
+        <v>KEY_09</v>
       </c>
       <c r="G85" t="str">
-        <f t="shared" si="27"/>
-        <v>SetName-KEY_04-help.png</v>
+        <f t="shared" si="32"/>
+        <v>SetDate-KEY_09-jump_next.png</v>
       </c>
       <c r="H85" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_TAB</v>
       </c>
       <c r="I85" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.45">
@@ -3810,33 +3818,33 @@
         <v>29</v>
       </c>
       <c r="B86" t="s">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="C86" t="s">
-        <v>125</v>
+        <v>4</v>
       </c>
       <c r="D86">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E86" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_0</v>
+        <f t="shared" si="30"/>
+        <v>help</v>
       </c>
       <c r="F86" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0A</v>
+        <f t="shared" si="31"/>
+        <v>KEY_04</v>
       </c>
       <c r="G86" t="str">
-        <f t="shared" si="27"/>
-        <v>SetName-KEY_0A-digit_0.png</v>
+        <f t="shared" si="32"/>
+        <v>SetName-KEY_04-help.png</v>
       </c>
       <c r="H86" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_0</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
       </c>
       <c r="I86" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.45">
@@ -3844,33 +3852,33 @@
         <v>29</v>
       </c>
       <c r="B87" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C87" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D87">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E87" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_1</v>
+        <f t="shared" si="30"/>
+        <v>digit_0</v>
       </c>
       <c r="F87" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0B</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0A</v>
       </c>
       <c r="G87" t="str">
-        <f t="shared" si="27"/>
-        <v>SetName-KEY_0B-digit_1.png</v>
+        <f t="shared" si="32"/>
+        <v>SetName-KEY_0A-digit_0.png</v>
       </c>
       <c r="H87" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_1</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_0</v>
       </c>
       <c r="I87" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.45">
@@ -3878,33 +3886,33 @@
         <v>29</v>
       </c>
       <c r="B88" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C88" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D88">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E88" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_2</v>
+        <f t="shared" si="30"/>
+        <v>digit_1</v>
       </c>
       <c r="F88" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0C</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0B</v>
       </c>
       <c r="G88" t="str">
-        <f t="shared" si="27"/>
-        <v>SetName-KEY_0C-digit_2.png</v>
+        <f t="shared" si="32"/>
+        <v>SetName-KEY_0B-digit_1.png</v>
       </c>
       <c r="H88" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_2</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I88" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.45">
@@ -3912,33 +3920,33 @@
         <v>29</v>
       </c>
       <c r="B89" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C89" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D89">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E89" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_3</v>
+        <f t="shared" si="30"/>
+        <v>digit_2</v>
       </c>
       <c r="F89" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0D</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0C</v>
       </c>
       <c r="G89" t="str">
-        <f t="shared" si="27"/>
-        <v>SetName-KEY_0D-digit_3.png</v>
+        <f t="shared" si="32"/>
+        <v>SetName-KEY_0C-digit_2.png</v>
       </c>
       <c r="H89" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_3</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I89" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.45">
@@ -3946,33 +3954,33 @@
         <v>29</v>
       </c>
       <c r="B90" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C90" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="D90">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E90" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_4</v>
+        <f t="shared" si="30"/>
+        <v>digit_3</v>
       </c>
       <c r="F90" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_06</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0D</v>
       </c>
       <c r="G90" t="str">
-        <f t="shared" si="27"/>
-        <v>SetName-KEY_06-digit_4.png</v>
+        <f t="shared" si="32"/>
+        <v>SetName-KEY_0D-digit_3.png</v>
       </c>
       <c r="H90" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_4</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I90" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.45">
@@ -3980,33 +3988,33 @@
         <v>29</v>
       </c>
       <c r="B91" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C91" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="D91">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E91" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_5</v>
+        <f t="shared" si="30"/>
+        <v>digit_4</v>
       </c>
       <c r="F91" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_07</v>
+        <f t="shared" si="31"/>
+        <v>KEY_06</v>
       </c>
       <c r="G91" t="str">
-        <f t="shared" si="27"/>
-        <v>SetName-KEY_07-digit_5.png</v>
+        <f t="shared" si="32"/>
+        <v>SetName-KEY_06-digit_4.png</v>
       </c>
       <c r="H91" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_5</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I91" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.45">
@@ -4014,33 +4022,33 @@
         <v>29</v>
       </c>
       <c r="B92" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C92" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="D92">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E92" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_6</v>
+        <f t="shared" si="30"/>
+        <v>digit_5</v>
       </c>
       <c r="F92" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_08</v>
+        <f t="shared" si="31"/>
+        <v>KEY_07</v>
       </c>
       <c r="G92" t="str">
-        <f t="shared" si="27"/>
-        <v>SetName-KEY_08-digit_6.png</v>
+        <f t="shared" si="32"/>
+        <v>SetName-KEY_07-digit_5.png</v>
       </c>
       <c r="H92" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_6</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_5</v>
       </c>
       <c r="I92" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.45">
@@ -4048,33 +4056,33 @@
         <v>29</v>
       </c>
       <c r="B93" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C93" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D93">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E93" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_7</v>
+        <f t="shared" si="30"/>
+        <v>digit_6</v>
       </c>
       <c r="F93" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_02</v>
+        <f t="shared" si="31"/>
+        <v>KEY_08</v>
       </c>
       <c r="G93" t="str">
-        <f t="shared" si="27"/>
-        <v>SetName-KEY_02-digit_7.png</v>
+        <f t="shared" si="32"/>
+        <v>SetName-KEY_08-digit_6.png</v>
       </c>
       <c r="H93" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_7</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_6</v>
       </c>
       <c r="I93" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_7,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.45">
@@ -4082,33 +4090,33 @@
         <v>29</v>
       </c>
       <c r="B94" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C94" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D94">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E94" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_8</v>
+        <f t="shared" si="30"/>
+        <v>digit_7</v>
       </c>
       <c r="F94" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_03</v>
+        <f t="shared" si="31"/>
+        <v>KEY_02</v>
       </c>
       <c r="G94" t="str">
-        <f t="shared" si="27"/>
-        <v>SetName-KEY_03-digit_8.png</v>
+        <f t="shared" si="32"/>
+        <v>SetName-KEY_02-digit_7.png</v>
       </c>
       <c r="H94" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_8</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_7</v>
       </c>
       <c r="I94" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_8,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_7,</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.45">
@@ -4116,33 +4124,33 @@
         <v>29</v>
       </c>
       <c r="B95" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C95" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D95">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E95" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_9</v>
+        <f t="shared" si="30"/>
+        <v>digit_8</v>
       </c>
       <c r="F95" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_04</v>
+        <f t="shared" si="31"/>
+        <v>KEY_03</v>
       </c>
       <c r="G95" t="str">
-        <f t="shared" si="27"/>
-        <v>SetName-KEY_04-digit_9.png</v>
+        <f t="shared" si="32"/>
+        <v>SetName-KEY_03-digit_8.png</v>
       </c>
       <c r="H95" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_9</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_8</v>
       </c>
       <c r="I95" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_9,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_8,</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.45">
@@ -4150,33 +4158,33 @@
         <v>29</v>
       </c>
       <c r="B96" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C96" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D96">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E96" t="str">
-        <f t="shared" si="25"/>
-        <v>back_space</v>
+        <f t="shared" si="30"/>
+        <v>digit_9</v>
       </c>
       <c r="F96" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_05</v>
+        <f t="shared" si="31"/>
+        <v>KEY_04</v>
       </c>
       <c r="G96" t="str">
-        <f t="shared" si="27"/>
-        <v>SetName-KEY_05-back_space.png</v>
+        <f t="shared" si="32"/>
+        <v>SetName-KEY_04-digit_9.png</v>
       </c>
       <c r="H96" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_BACKSPACE</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_9</v>
       </c>
       <c r="I96" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_9,</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.45">
@@ -4184,33 +4192,33 @@
         <v>29</v>
       </c>
       <c r="B97" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C97" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D97">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E97" t="str">
-        <f t="shared" si="25"/>
-        <v>enter</v>
+        <f t="shared" si="30"/>
+        <v>back_space</v>
       </c>
       <c r="F97" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0E</v>
+        <f t="shared" si="31"/>
+        <v>KEY_05</v>
       </c>
       <c r="G97" t="str">
-        <f t="shared" si="27"/>
-        <v>SetName-KEY_0E-enter.png</v>
+        <f t="shared" si="32"/>
+        <v>SetName-KEY_05-back_space.png</v>
       </c>
       <c r="H97" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_ENTER</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_BACKSPACE</v>
       </c>
       <c r="I97" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.45">
@@ -4218,67 +4226,67 @@
         <v>29</v>
       </c>
       <c r="B98" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C98" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="D98">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E98" t="str">
-        <f t="shared" si="25"/>
-        <v>jump_next</v>
+        <f t="shared" si="30"/>
+        <v>enter</v>
       </c>
       <c r="F98" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_09</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0E</v>
       </c>
       <c r="G98" t="str">
-        <f t="shared" si="27"/>
-        <v>SetName-KEY_09-jump_next.png</v>
+        <f t="shared" si="32"/>
+        <v>SetName-KEY_0E-enter.png</v>
       </c>
       <c r="H98" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_TAB</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_ENTER</v>
       </c>
       <c r="I98" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B99" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="C99" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D99">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E99" t="str">
-        <f t="shared" si="25"/>
-        <v>help</v>
+        <f t="shared" si="30"/>
+        <v>jump_next</v>
       </c>
       <c r="F99" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_04</v>
+        <f t="shared" si="31"/>
+        <v>KEY_09</v>
       </c>
       <c r="G99" t="str">
-        <f t="shared" si="27"/>
-        <v>SetTime-KEY_04-help.png</v>
+        <f t="shared" si="32"/>
+        <v>SetName-KEY_09-jump_next.png</v>
       </c>
       <c r="H99" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_TAB</v>
       </c>
       <c r="I99" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.45">
@@ -4286,33 +4294,33 @@
         <v>28</v>
       </c>
       <c r="B100" t="s">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="C100" t="s">
-        <v>125</v>
+        <v>4</v>
       </c>
       <c r="D100">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E100" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_0</v>
+        <f t="shared" si="30"/>
+        <v>help</v>
       </c>
       <c r="F100" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0A</v>
+        <f t="shared" si="31"/>
+        <v>KEY_04</v>
       </c>
       <c r="G100" t="str">
-        <f t="shared" si="27"/>
-        <v>SetTime-KEY_0A-digit_0.png</v>
+        <f t="shared" si="32"/>
+        <v>SetTime-KEY_04-help.png</v>
       </c>
       <c r="H100" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_0</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
       </c>
       <c r="I100" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.45">
@@ -4320,33 +4328,33 @@
         <v>28</v>
       </c>
       <c r="B101" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C101" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D101">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E101" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_1</v>
+        <f t="shared" si="30"/>
+        <v>digit_0</v>
       </c>
       <c r="F101" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0B</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0A</v>
       </c>
       <c r="G101" t="str">
-        <f t="shared" si="27"/>
-        <v>SetTime-KEY_0B-digit_1.png</v>
+        <f t="shared" si="32"/>
+        <v>SetTime-KEY_0A-digit_0.png</v>
       </c>
       <c r="H101" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_1</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_0</v>
       </c>
       <c r="I101" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.45">
@@ -4354,33 +4362,33 @@
         <v>28</v>
       </c>
       <c r="B102" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C102" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D102">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E102" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_2</v>
+        <f t="shared" si="30"/>
+        <v>digit_1</v>
       </c>
       <c r="F102" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0C</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0B</v>
       </c>
       <c r="G102" t="str">
-        <f t="shared" si="27"/>
-        <v>SetTime-KEY_0C-digit_2.png</v>
+        <f t="shared" si="32"/>
+        <v>SetTime-KEY_0B-digit_1.png</v>
       </c>
       <c r="H102" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_2</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I102" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.45">
@@ -4388,33 +4396,33 @@
         <v>28</v>
       </c>
       <c r="B103" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C103" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D103">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E103" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_3</v>
+        <f t="shared" si="30"/>
+        <v>digit_2</v>
       </c>
       <c r="F103" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0D</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0C</v>
       </c>
       <c r="G103" t="str">
-        <f t="shared" si="27"/>
-        <v>SetTime-KEY_0D-digit_3.png</v>
+        <f t="shared" si="32"/>
+        <v>SetTime-KEY_0C-digit_2.png</v>
       </c>
       <c r="H103" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_3</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I103" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.45">
@@ -4422,33 +4430,33 @@
         <v>28</v>
       </c>
       <c r="B104" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C104" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="D104">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E104" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_4</v>
+        <f t="shared" si="30"/>
+        <v>digit_3</v>
       </c>
       <c r="F104" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_06</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0D</v>
       </c>
       <c r="G104" t="str">
-        <f t="shared" si="27"/>
-        <v>SetTime-KEY_06-digit_4.png</v>
+        <f t="shared" si="32"/>
+        <v>SetTime-KEY_0D-digit_3.png</v>
       </c>
       <c r="H104" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_4</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I104" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.45">
@@ -4456,33 +4464,33 @@
         <v>28</v>
       </c>
       <c r="B105" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C105" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="D105">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E105" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_5</v>
+        <f t="shared" si="30"/>
+        <v>digit_4</v>
       </c>
       <c r="F105" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_07</v>
+        <f t="shared" si="31"/>
+        <v>KEY_06</v>
       </c>
       <c r="G105" t="str">
-        <f t="shared" si="27"/>
-        <v>SetTime-KEY_07-digit_5.png</v>
+        <f t="shared" si="32"/>
+        <v>SetTime-KEY_06-digit_4.png</v>
       </c>
       <c r="H105" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_5</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I105" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.45">
@@ -4490,33 +4498,33 @@
         <v>28</v>
       </c>
       <c r="B106" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C106" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="D106">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E106" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_6</v>
+        <f t="shared" si="30"/>
+        <v>digit_5</v>
       </c>
       <c r="F106" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_08</v>
+        <f t="shared" si="31"/>
+        <v>KEY_07</v>
       </c>
       <c r="G106" t="str">
-        <f t="shared" si="27"/>
-        <v>SetTime-KEY_08-digit_6.png</v>
+        <f t="shared" si="32"/>
+        <v>SetTime-KEY_07-digit_5.png</v>
       </c>
       <c r="H106" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_6</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_5</v>
       </c>
       <c r="I106" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.45">
@@ -4524,33 +4532,33 @@
         <v>28</v>
       </c>
       <c r="B107" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C107" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D107">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E107" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_7</v>
+        <f t="shared" si="30"/>
+        <v>digit_6</v>
       </c>
       <c r="F107" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_02</v>
+        <f t="shared" si="31"/>
+        <v>KEY_08</v>
       </c>
       <c r="G107" t="str">
-        <f t="shared" si="27"/>
-        <v>SetTime-KEY_02-digit_7.png</v>
+        <f t="shared" si="32"/>
+        <v>SetTime-KEY_08-digit_6.png</v>
       </c>
       <c r="H107" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_7</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_6</v>
       </c>
       <c r="I107" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_7,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.45">
@@ -4558,33 +4566,33 @@
         <v>28</v>
       </c>
       <c r="B108" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C108" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D108">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E108" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_8</v>
+        <f t="shared" si="30"/>
+        <v>digit_7</v>
       </c>
       <c r="F108" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_03</v>
+        <f t="shared" si="31"/>
+        <v>KEY_02</v>
       </c>
       <c r="G108" t="str">
-        <f t="shared" si="27"/>
-        <v>SetTime-KEY_03-digit_8.png</v>
+        <f t="shared" si="32"/>
+        <v>SetTime-KEY_02-digit_7.png</v>
       </c>
       <c r="H108" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_8</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_7</v>
       </c>
       <c r="I108" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_8,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_7,</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.45">
@@ -4592,33 +4600,33 @@
         <v>28</v>
       </c>
       <c r="B109" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C109" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D109">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E109" t="str">
-        <f t="shared" si="25"/>
-        <v>digit_9</v>
+        <f t="shared" si="30"/>
+        <v>digit_8</v>
       </c>
       <c r="F109" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_04</v>
+        <f t="shared" si="31"/>
+        <v>KEY_03</v>
       </c>
       <c r="G109" t="str">
-        <f t="shared" si="27"/>
-        <v>SetTime-KEY_04-digit_9.png</v>
+        <f t="shared" si="32"/>
+        <v>SetTime-KEY_03-digit_8.png</v>
       </c>
       <c r="H109" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_9</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_8</v>
       </c>
       <c r="I109" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_9,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_8,</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.45">
@@ -4626,33 +4634,33 @@
         <v>28</v>
       </c>
       <c r="B110" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C110" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D110">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E110" t="str">
-        <f t="shared" si="25"/>
-        <v>back_space</v>
+        <f t="shared" si="30"/>
+        <v>digit_9</v>
       </c>
       <c r="F110" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_05</v>
+        <f t="shared" si="31"/>
+        <v>KEY_04</v>
       </c>
       <c r="G110" t="str">
-        <f t="shared" si="27"/>
-        <v>SetTime-KEY_05-back_space.png</v>
+        <f t="shared" si="32"/>
+        <v>SetTime-KEY_04-digit_9.png</v>
       </c>
       <c r="H110" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_BACKSPACE</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_9</v>
       </c>
       <c r="I110" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_9,</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.45">
@@ -4660,33 +4668,33 @@
         <v>28</v>
       </c>
       <c r="B111" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C111" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D111">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E111" t="str">
-        <f t="shared" si="25"/>
-        <v>enter</v>
+        <f t="shared" si="30"/>
+        <v>back_space</v>
       </c>
       <c r="F111" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_0E</v>
+        <f t="shared" si="31"/>
+        <v>KEY_05</v>
       </c>
       <c r="G111" t="str">
-        <f t="shared" si="27"/>
-        <v>SetTime-KEY_0E-enter.png</v>
+        <f t="shared" si="32"/>
+        <v>SetTime-KEY_05-back_space.png</v>
       </c>
       <c r="H111" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_ENTER</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_BACKSPACE</v>
       </c>
       <c r="I111" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.45">
@@ -4694,67 +4702,67 @@
         <v>28</v>
       </c>
       <c r="B112" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C112" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="D112">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E112" t="str">
-        <f t="shared" si="25"/>
-        <v>jump_next</v>
+        <f t="shared" si="30"/>
+        <v>enter</v>
       </c>
       <c r="F112" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_09</v>
+        <f t="shared" si="31"/>
+        <v>KEY_0E</v>
       </c>
       <c r="G112" t="str">
-        <f t="shared" si="27"/>
-        <v>SetTime-KEY_09-jump_next.png</v>
+        <f t="shared" si="32"/>
+        <v>SetTime-KEY_0E-enter.png</v>
       </c>
       <c r="H112" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_TAB</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_ENTER</v>
       </c>
       <c r="I112" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B113" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="C113" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D113">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E113" t="str">
-        <f t="shared" si="25"/>
-        <v>help</v>
+        <f t="shared" si="30"/>
+        <v>jump_next</v>
       </c>
       <c r="F113" t="str">
-        <f t="shared" si="26"/>
-        <v>KEY_04</v>
+        <f t="shared" si="31"/>
+        <v>KEY_09</v>
       </c>
       <c r="G113" t="str">
-        <f t="shared" si="27"/>
-        <v>StorageManagement-KEY_04-help.png</v>
+        <f t="shared" si="32"/>
+        <v>SetTime-KEY_09-jump_next.png</v>
       </c>
       <c r="H113" t="str">
-        <f t="shared" si="28"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_TAB</v>
       </c>
       <c r="I113" t="str">
-        <f t="shared" si="29"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.45">
@@ -4762,19 +4770,53 @@
         <v>32</v>
       </c>
       <c r="B114" t="s">
+        <v>6</v>
+      </c>
+      <c r="C114" t="s">
+        <v>4</v>
+      </c>
+      <c r="D114">
+        <v>4</v>
+      </c>
+      <c r="E114" t="str">
+        <f t="shared" si="30"/>
+        <v>help</v>
+      </c>
+      <c r="F114" t="str">
+        <f t="shared" si="31"/>
+        <v>KEY_04</v>
+      </c>
+      <c r="G114" t="str">
+        <f t="shared" si="32"/>
+        <v>StorageManagement-KEY_04-help.png</v>
+      </c>
+      <c r="H114" t="str">
+        <f t="shared" si="33"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
+      </c>
+      <c r="I114" t="str">
+        <f t="shared" si="34"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A115" t="s">
+        <v>32</v>
+      </c>
+      <c r="B115" t="s">
         <v>7</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C115" t="s">
         <v>5</v>
       </c>
-      <c r="D114">
+      <c r="D115">
         <v>9</v>
       </c>
-      <c r="E114" t="str">
-        <f t="shared" ref="E114:E128" si="30">LOWER(
+      <c r="E115" t="str">
+        <f t="shared" ref="E115:E129" si="35">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B114, FIND(" = InputEventMap", B114) - 1),
+      LEFT(B115, FIND(" = InputEventMap", B115) - 1),
       CHAR(160),
       " "
     )
@@ -4782,58 +4824,24 @@
 )</f>
         <v>menu</v>
       </c>
-      <c r="F114" t="str">
-        <f t="shared" ref="F114:F128" si="31">"KEY_" &amp; CHOOSE(
-    D114+1,
+      <c r="F115" t="str">
+        <f t="shared" ref="F115:F129" si="36">"KEY_" &amp; CHOOSE(
+    D115+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_09</v>
       </c>
-      <c r="G114" t="str">
-        <f t="shared" ref="G114:G128" si="32">_xlfn.CONCAT(A114, "-", F114, "-", E114, ".png")</f>
+      <c r="G115" t="str">
+        <f t="shared" ref="G115:G129" si="37">_xlfn.CONCAT(A115, "-", F115, "-", E115, ".png")</f>
         <v>StorageManagement-KEY_09-menu.png</v>
       </c>
-      <c r="H114" t="str">
-        <f t="shared" ref="H114:H128" si="33">MID(B114, FIND("InputEventMap", B114), LEN(B114))</f>
+      <c r="H115" t="str">
+        <f t="shared" ref="H115:H129" si="38">MID(B115, FIND("InputEventMap", B115), LEN(B115))</f>
         <v>InputEventMap.KEY_5</v>
       </c>
-      <c r="I114" t="str">
-        <f t="shared" ref="I114:I128" si="34">_xlfn.CONCAT("StreamdeckInput.", F114, ": ", H114, ",")</f>
+      <c r="I115" t="str">
+        <f t="shared" ref="I115:I129" si="39">_xlfn.CONCAT("StreamdeckInput.", F115, ": ", H115, ",")</f>
         <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A115" t="s">
-        <v>32</v>
-      </c>
-      <c r="B115" t="s">
-        <v>98</v>
-      </c>
-      <c r="C115" t="s">
-        <v>135</v>
-      </c>
-      <c r="D115">
-        <v>5</v>
-      </c>
-      <c r="E115" t="str">
-        <f t="shared" si="30"/>
-        <v>disconnect_storage</v>
-      </c>
-      <c r="F115" t="str">
-        <f t="shared" si="31"/>
-        <v>KEY_05</v>
-      </c>
-      <c r="G115" t="str">
-        <f t="shared" si="32"/>
-        <v>StorageManagement-KEY_05-disconnect_storage.png</v>
-      </c>
-      <c r="H115" t="str">
-        <f t="shared" si="33"/>
-        <v>InputEventMap.KEY_0</v>
-      </c>
-      <c r="I115" t="str">
-        <f t="shared" si="34"/>
-        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_0,</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.45">
@@ -4841,33 +4849,33 @@
         <v>32</v>
       </c>
       <c r="B116" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C116" t="s">
-        <v>49</v>
+        <v>125</v>
       </c>
       <c r="D116">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E116" t="str">
-        <f t="shared" si="30"/>
-        <v>detect_rc1</v>
+        <f t="shared" si="35"/>
+        <v>disconnect_storage</v>
       </c>
       <c r="F116" t="str">
-        <f t="shared" si="31"/>
-        <v>KEY_02</v>
+        <f t="shared" si="36"/>
+        <v>KEY_05</v>
       </c>
       <c r="G116" t="str">
-        <f t="shared" si="32"/>
-        <v>StorageManagement-KEY_02-detect_rc1.png</v>
+        <f t="shared" si="37"/>
+        <v>StorageManagement-KEY_05-disconnect_storage.png</v>
       </c>
       <c r="H116" t="str">
-        <f t="shared" si="33"/>
-        <v>InputEventMap.KEY_1</v>
+        <f t="shared" si="38"/>
+        <v>InputEventMap.KEY_0</v>
       </c>
       <c r="I116" t="str">
-        <f t="shared" si="34"/>
-        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_1,</v>
+        <f t="shared" si="39"/>
+        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_0,</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.45">
@@ -4875,33 +4883,33 @@
         <v>32</v>
       </c>
       <c r="B117" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C117" t="s">
-        <v>49</v>
+        <v>132</v>
       </c>
       <c r="D117">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E117" t="str">
-        <f t="shared" si="30"/>
-        <v>detect_rc2</v>
+        <f t="shared" si="35"/>
+        <v>detect_rc1</v>
       </c>
       <c r="F117" t="str">
-        <f t="shared" si="31"/>
-        <v>KEY_03</v>
+        <f t="shared" si="36"/>
+        <v>KEY_02</v>
       </c>
       <c r="G117" t="str">
-        <f t="shared" si="32"/>
-        <v>StorageManagement-KEY_03-detect_rc2.png</v>
+        <f t="shared" si="37"/>
+        <v>StorageManagement-KEY_02-detect_rc1.png</v>
       </c>
       <c r="H117" t="str">
-        <f t="shared" si="33"/>
-        <v>InputEventMap.KEY_3</v>
+        <f t="shared" si="38"/>
+        <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I117" t="str">
-        <f t="shared" si="34"/>
-        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_3,</v>
+        <f t="shared" si="39"/>
+        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_1,</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.45">
@@ -4909,33 +4917,33 @@
         <v>32</v>
       </c>
       <c r="B118" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C118" t="s">
-        <v>50</v>
+        <v>132</v>
       </c>
       <c r="D118">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E118" t="str">
-        <f t="shared" si="30"/>
-        <v>format_rc1</v>
+        <f t="shared" si="35"/>
+        <v>detect_rc2</v>
       </c>
       <c r="F118" t="str">
-        <f t="shared" si="31"/>
-        <v>KEY_06</v>
+        <f t="shared" si="36"/>
+        <v>KEY_03</v>
       </c>
       <c r="G118" t="str">
-        <f t="shared" si="32"/>
-        <v>StorageManagement-KEY_06-format_rc1.png</v>
+        <f t="shared" si="37"/>
+        <v>StorageManagement-KEY_03-detect_rc2.png</v>
       </c>
       <c r="H118" t="str">
-        <f t="shared" si="33"/>
-        <v>InputEventMap.KEY_4</v>
+        <f t="shared" si="38"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I118" t="str">
-        <f t="shared" si="34"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
+        <f t="shared" si="39"/>
+        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_3,</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.45">
@@ -4943,33 +4951,33 @@
         <v>32</v>
       </c>
       <c r="B119" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C119" t="s">
-        <v>50</v>
+        <v>135</v>
       </c>
       <c r="D119">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E119" t="str">
-        <f t="shared" si="30"/>
-        <v>format_rc2</v>
+        <f t="shared" si="35"/>
+        <v>format_rc1</v>
       </c>
       <c r="F119" t="str">
-        <f t="shared" si="31"/>
-        <v>KEY_07</v>
+        <f t="shared" si="36"/>
+        <v>KEY_06</v>
       </c>
       <c r="G119" t="str">
-        <f t="shared" si="32"/>
-        <v>StorageManagement-KEY_07-format_rc2.png</v>
+        <f t="shared" si="37"/>
+        <v>StorageManagement-KEY_06-format_rc1.png</v>
       </c>
       <c r="H119" t="str">
-        <f t="shared" si="33"/>
-        <v>InputEventMap.KEY_6</v>
+        <f t="shared" si="38"/>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I119" t="str">
-        <f t="shared" si="34"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_6,</v>
+        <f t="shared" si="39"/>
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.45">
@@ -4977,33 +4985,33 @@
         <v>32</v>
       </c>
       <c r="B120" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C120" t="s">
-        <v>51</v>
+        <v>135</v>
       </c>
       <c r="D120">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E120" t="str">
-        <f t="shared" si="30"/>
-        <v>clean_rc1</v>
+        <f t="shared" si="35"/>
+        <v>format_rc2</v>
       </c>
       <c r="F120" t="str">
-        <f t="shared" si="31"/>
-        <v>KEY_0B</v>
+        <f t="shared" si="36"/>
+        <v>KEY_07</v>
       </c>
       <c r="G120" t="str">
-        <f t="shared" si="32"/>
-        <v>StorageManagement-KEY_0B-clean_rc1.png</v>
+        <f t="shared" si="37"/>
+        <v>StorageManagement-KEY_07-format_rc2.png</v>
       </c>
       <c r="H120" t="str">
-        <f t="shared" si="33"/>
-        <v>InputEventMap.KEY_7</v>
+        <f t="shared" si="38"/>
+        <v>InputEventMap.KEY_6</v>
       </c>
       <c r="I120" t="str">
-        <f t="shared" si="34"/>
-        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_7,</v>
+        <f t="shared" si="39"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_6,</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.45">
@@ -5011,67 +5019,67 @@
         <v>32</v>
       </c>
       <c r="B121" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C121" t="s">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="D121">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E121" t="str">
-        <f t="shared" si="30"/>
-        <v>clean_rc2</v>
+        <f t="shared" si="35"/>
+        <v>clean_rc1</v>
       </c>
       <c r="F121" t="str">
-        <f t="shared" si="31"/>
-        <v>KEY_0C</v>
+        <f t="shared" si="36"/>
+        <v>KEY_0B</v>
       </c>
       <c r="G121" t="str">
-        <f t="shared" si="32"/>
-        <v>StorageManagement-KEY_0C-clean_rc2.png</v>
+        <f t="shared" si="37"/>
+        <v>StorageManagement-KEY_0B-clean_rc1.png</v>
       </c>
       <c r="H121" t="str">
-        <f t="shared" si="33"/>
-        <v>InputEventMap.KEY_9</v>
+        <f t="shared" si="38"/>
+        <v>InputEventMap.KEY_7</v>
       </c>
       <c r="I121" t="str">
-        <f t="shared" si="34"/>
-        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_9,</v>
+        <f t="shared" si="39"/>
+        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_7,</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B122" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="C122" t="s">
-        <v>4</v>
+        <v>131</v>
       </c>
       <c r="D122">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E122" t="str">
-        <f t="shared" si="30"/>
-        <v>help</v>
+        <f t="shared" si="35"/>
+        <v>clean_rc2</v>
       </c>
       <c r="F122" t="str">
-        <f t="shared" si="31"/>
-        <v>KEY_04</v>
+        <f t="shared" si="36"/>
+        <v>KEY_0C</v>
       </c>
       <c r="G122" t="str">
-        <f t="shared" si="32"/>
-        <v>System-KEY_04-help.png</v>
+        <f t="shared" si="37"/>
+        <v>StorageManagement-KEY_0C-clean_rc2.png</v>
       </c>
       <c r="H122" t="str">
-        <f t="shared" si="33"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
+        <f t="shared" si="38"/>
+        <v>InputEventMap.KEY_9</v>
       </c>
       <c r="I122" t="str">
-        <f t="shared" si="34"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
+        <f t="shared" si="39"/>
+        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_9,</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.45">
@@ -5079,33 +5087,33 @@
         <v>10</v>
       </c>
       <c r="B123" t="s">
-        <v>105</v>
+        <v>6</v>
       </c>
       <c r="C123" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D123">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E123" t="str">
-        <f t="shared" si="30"/>
-        <v>select_main</v>
+        <f t="shared" si="35"/>
+        <v>help</v>
       </c>
       <c r="F123" t="str">
-        <f t="shared" si="31"/>
-        <v>KEY_09</v>
+        <f t="shared" si="36"/>
+        <v>KEY_04</v>
       </c>
       <c r="G123" t="str">
-        <f t="shared" si="32"/>
-        <v>System-KEY_09-select_main.png</v>
+        <f t="shared" si="37"/>
+        <v>System-KEY_04-help.png</v>
       </c>
       <c r="H123" t="str">
-        <f t="shared" si="33"/>
-        <v>InputEventMap.KEY_1</v>
+        <f t="shared" si="38"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
       </c>
       <c r="I123" t="str">
-        <f t="shared" si="34"/>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_1,</v>
+        <f t="shared" si="39"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.45">
@@ -5113,33 +5121,33 @@
         <v>10</v>
       </c>
       <c r="B124" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C124" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D124">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E124" t="str">
-        <f t="shared" si="30"/>
-        <v>select_language</v>
+        <f t="shared" si="35"/>
+        <v>select_main</v>
       </c>
       <c r="F124" t="str">
-        <f t="shared" si="31"/>
-        <v>KEY_06</v>
+        <f t="shared" si="36"/>
+        <v>KEY_09</v>
       </c>
       <c r="G124" t="str">
-        <f t="shared" si="32"/>
-        <v>System-KEY_06-select_language.png</v>
+        <f t="shared" si="37"/>
+        <v>System-KEY_09-select_main.png</v>
       </c>
       <c r="H124" t="str">
-        <f t="shared" si="33"/>
-        <v>InputEventMap.KEY_2</v>
+        <f t="shared" si="38"/>
+        <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I124" t="str">
-        <f t="shared" si="34"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
+        <f t="shared" si="39"/>
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_1,</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.45">
@@ -5147,33 +5155,33 @@
         <v>10</v>
       </c>
       <c r="B125" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C125" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="D125">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E125" t="str">
-        <f t="shared" si="30"/>
-        <v>select_storage</v>
+        <f t="shared" si="35"/>
+        <v>select_language</v>
       </c>
       <c r="F125" t="str">
-        <f t="shared" si="31"/>
-        <v>KEY_07</v>
+        <f t="shared" si="36"/>
+        <v>KEY_06</v>
       </c>
       <c r="G125" t="str">
-        <f t="shared" si="32"/>
-        <v>System-KEY_07-select_storage.png</v>
+        <f t="shared" si="37"/>
+        <v>System-KEY_06-select_language.png</v>
       </c>
       <c r="H125" t="str">
-        <f t="shared" si="33"/>
-        <v>InputEventMap.KEY_3</v>
+        <f t="shared" si="38"/>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I125" t="str">
-        <f t="shared" si="34"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
+        <f t="shared" si="39"/>
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.45">
@@ -5181,33 +5189,33 @@
         <v>10</v>
       </c>
       <c r="B126" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C126" t="s">
-        <v>138</v>
+        <v>43</v>
       </c>
       <c r="D126">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E126" t="str">
-        <f t="shared" si="30"/>
-        <v>set_date</v>
+        <f t="shared" si="35"/>
+        <v>select_storage</v>
       </c>
       <c r="F126" t="str">
-        <f t="shared" si="31"/>
-        <v>KEY_0B</v>
+        <f t="shared" si="36"/>
+        <v>KEY_07</v>
       </c>
       <c r="G126" t="str">
-        <f t="shared" si="32"/>
-        <v>System-KEY_0B-set_date.png</v>
+        <f t="shared" si="37"/>
+        <v>System-KEY_07-select_storage.png</v>
       </c>
       <c r="H126" t="str">
-        <f t="shared" si="33"/>
-        <v>InputEventMap.KEY_4</v>
+        <f t="shared" si="38"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I126" t="str">
-        <f t="shared" si="34"/>
-        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_4,</v>
+        <f t="shared" si="39"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.45">
@@ -5215,33 +5223,33 @@
         <v>10</v>
       </c>
       <c r="B127" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C127" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D127">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E127" t="str">
-        <f t="shared" si="30"/>
-        <v>set_time</v>
+        <f t="shared" si="35"/>
+        <v>set_date</v>
       </c>
       <c r="F127" t="str">
-        <f t="shared" si="31"/>
-        <v>KEY_0C</v>
+        <f t="shared" si="36"/>
+        <v>KEY_0B</v>
       </c>
       <c r="G127" t="str">
-        <f t="shared" si="32"/>
-        <v>System-KEY_0C-set_time.png</v>
+        <f t="shared" si="37"/>
+        <v>System-KEY_0B-set_date.png</v>
       </c>
       <c r="H127" t="str">
-        <f t="shared" si="33"/>
-        <v>InputEventMap.KEY_6</v>
+        <f t="shared" si="38"/>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I127" t="str">
-        <f t="shared" si="34"/>
-        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_6,</v>
+        <f t="shared" si="39"/>
+        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_4,</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.45">
@@ -5249,36 +5257,71 @@
         <v>10</v>
       </c>
       <c r="B128" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="C128" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D128">
+        <v>12</v>
+      </c>
+      <c r="E128" t="str">
+        <f t="shared" si="35"/>
+        <v>set_time</v>
+      </c>
+      <c r="F128" t="str">
+        <f t="shared" si="36"/>
+        <v>KEY_0C</v>
+      </c>
+      <c r="G128" t="str">
+        <f t="shared" si="37"/>
+        <v>System-KEY_0C-set_time.png</v>
+      </c>
+      <c r="H128" t="str">
+        <f t="shared" si="38"/>
+        <v>InputEventMap.KEY_6</v>
+      </c>
+      <c r="I128" t="str">
+        <f t="shared" si="39"/>
+        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_6,</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A129" t="s">
+        <v>10</v>
+      </c>
+      <c r="B129" t="s">
+        <v>49</v>
+      </c>
+      <c r="C129" t="s">
+        <v>127</v>
+      </c>
+      <c r="D129">
         <v>14</v>
       </c>
-      <c r="E128" t="str">
-        <f t="shared" si="30"/>
+      <c r="E129" t="str">
+        <f t="shared" si="35"/>
         <v>stop_system</v>
       </c>
-      <c r="F128" t="str">
-        <f t="shared" si="31"/>
+      <c r="F129" t="str">
+        <f t="shared" si="36"/>
         <v>KEY_0E</v>
       </c>
-      <c r="G128" t="str">
-        <f t="shared" si="32"/>
+      <c r="G129" t="str">
+        <f t="shared" si="37"/>
         <v>System-KEY_0E-stop_system.png</v>
       </c>
-      <c r="H128" t="str">
-        <f t="shared" si="33"/>
+      <c r="H129" t="str">
+        <f t="shared" si="38"/>
         <v>InputEventMap.KEY_9</v>
       </c>
-      <c r="I128" t="str">
-        <f t="shared" si="34"/>
+      <c r="I129" t="str">
+        <f t="shared" si="39"/>
         <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_9,</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I129" xr:uid="{47861C0B-96C3-4FC0-B828-7FD785B358D7}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Changes to excel with key and image mapping, new images, images in png
</commit_message>
<xml_diff>
--- a/prep/StreamdeckIconInputKeyMapping.xlsx
+++ b/prep/StreamdeckIconInputKeyMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irene\src\biz.dfch.PhoneTap\prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30632FBB-4119-437C-8C2A-935C9722D40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3317F6EA-04A1-47F0-957B-8D7830A6251B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{4419FAFA-D280-4090-97B7-CB07F6B7BE60}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="137">
   <si>
     <t>States</t>
   </si>
@@ -53,12 +53,6 @@
     <t>StreamdeckKey</t>
   </si>
   <si>
-    <t>ic_fluent_lightbulb_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_settings_48_regular.svg</t>
-  </si>
-  <si>
     <t>        HELP = InputEventMap.KEY_ASTERISK</t>
   </si>
   <si>
@@ -146,9 +140,6 @@
     <t>        SKIP_AUDIO = InputEventMap.KEY_2</t>
   </si>
   <si>
-    <t>ic_fluent_speaker_2_48_regular.svg</t>
-  </si>
-  <si>
     <t xml:space="preserve">        HELP = InputEventMap.KEY_ASTERISK</t>
   </si>
   <si>
@@ -200,9 +191,6 @@
     <t>ic_fluent_text_edit_style_character_a_32_regular.svg</t>
   </si>
   <si>
-    <t>ic_fluent_arrow_exit_48_regular.svg</t>
-  </si>
-  <si>
     <t>        STOP_RECORDING = InputEventMap.KEY_1</t>
   </si>
   <si>
@@ -428,31 +416,40 @@
     <t>ic_fluent_calendar_edit_32_regular.svg</t>
   </si>
   <si>
-    <t>ic_fluent_local_language_28_regular.svg</t>
-  </si>
-  <si>
     <t>ic_fluent_home_48_regular.svg</t>
   </si>
   <si>
     <t>ic_fluent_eraser_24_regular.svg</t>
   </si>
   <si>
-    <t>ic_fluent_search_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_skip_forward_tab_24_regular.svg</t>
-  </si>
-  <si>
     <t xml:space="preserve">        SCREEN = InputEventMap.KEY_ASTERISK</t>
   </si>
   <si>
-    <t>ic_fluent_database_warning_20_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_database_checkmark_24_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_database_arrow_down_20_regular.svg</t>
+    <t>ic_fluent_globe_48_regular.svg</t>
+  </si>
+  <si>
+    <t>ic_fluent_lightbulb_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_settings_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_speaker_2_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_skip_forward_tab_24_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_search_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_database_warning_20_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_database_checkmark_24_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_database_arrow_down_20_regular.png</t>
   </si>
 </sst>
 </file>
@@ -841,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47861C0B-96C3-4FC0-B828-7FD785B358D7}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -868,33 +865,33 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D2">
         <v>4</v>
@@ -933,13 +930,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="D3">
         <v>9</v>
@@ -970,13 +967,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -1004,13 +1001,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>131</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -1038,13 +1035,13 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -1072,13 +1069,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -1106,13 +1103,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1140,13 +1137,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -1174,13 +1171,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -1208,13 +1205,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -1242,13 +1239,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -1276,13 +1273,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D13">
         <v>4</v>
@@ -1310,13 +1307,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -1344,13 +1341,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D15">
         <v>6</v>
@@ -1378,13 +1375,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -1412,13 +1409,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -1446,13 +1443,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D18">
         <v>6</v>
@@ -1480,13 +1477,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D19">
         <v>4</v>
@@ -1514,13 +1511,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D20">
         <v>5</v>
@@ -1548,13 +1545,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D21">
         <v>6</v>
@@ -1582,13 +1579,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D22">
         <v>4</v>
@@ -1616,13 +1613,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D23">
         <v>5</v>
@@ -1650,13 +1647,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D24">
         <v>6</v>
@@ -1684,13 +1681,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D25">
         <v>4</v>
@@ -1726,13 +1723,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D26">
         <v>5</v>
@@ -1760,13 +1757,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D27">
         <v>6</v>
@@ -1794,13 +1791,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D28">
         <v>10</v>
@@ -1828,13 +1825,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D29">
         <v>11</v>
@@ -1862,13 +1859,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D30">
         <v>12</v>
@@ -1896,13 +1893,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D31">
         <v>13</v>
@@ -1930,13 +1927,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D32">
         <v>4</v>
@@ -1964,13 +1961,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D33">
         <v>5</v>
@@ -2006,13 +2003,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D34">
         <v>6</v>
@@ -2040,13 +2037,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D35">
         <v>10</v>
@@ -2074,13 +2071,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D36">
         <v>11</v>
@@ -2108,13 +2105,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D37">
         <v>12</v>
@@ -2142,13 +2139,13 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D38">
         <v>13</v>
@@ -2176,13 +2173,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C39" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -2221,13 +2218,13 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C40" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D40">
         <v>4</v>
@@ -2255,13 +2252,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D41">
         <v>5</v>
@@ -2297,13 +2294,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D42">
         <v>6</v>
@@ -2331,13 +2328,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D43">
         <v>7</v>
@@ -2365,13 +2362,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D44">
         <v>10</v>
@@ -2399,13 +2396,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="D45">
         <v>9</v>
@@ -2433,13 +2430,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D46">
         <v>11</v>
@@ -2467,13 +2464,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
       <c r="D47">
         <v>14</v>
@@ -2501,13 +2498,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D48">
         <v>4</v>
@@ -2535,13 +2532,13 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" t="s">
         <v>54</v>
-      </c>
-      <c r="C49" t="s">
-        <v>58</v>
       </c>
       <c r="D49">
         <v>6</v>
@@ -2580,13 +2577,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" t="s">
         <v>55</v>
-      </c>
-      <c r="C50" t="s">
-        <v>59</v>
       </c>
       <c r="D50">
         <v>5</v>
@@ -2614,13 +2611,13 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" t="s">
         <v>56</v>
-      </c>
-      <c r="C51" t="s">
-        <v>60</v>
       </c>
       <c r="D51">
         <v>7</v>
@@ -2648,13 +2645,13 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" t="s">
         <v>57</v>
-      </c>
-      <c r="C52" t="s">
-        <v>61</v>
       </c>
       <c r="D52">
         <v>10</v>
@@ -2682,13 +2679,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B53" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D53">
         <v>4</v>
@@ -2727,13 +2724,13 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B54" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C54" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D54">
         <v>5</v>
@@ -2761,13 +2758,13 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>5</v>
+        <v>125</v>
       </c>
       <c r="D55">
         <v>9</v>
@@ -2795,13 +2792,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D56">
         <v>4</v>
@@ -2829,13 +2826,13 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B57" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C57" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D57">
         <v>7</v>
@@ -2863,13 +2860,13 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B58" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C58" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D58">
         <v>11</v>
@@ -2897,13 +2894,13 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C59" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D59">
         <v>12</v>
@@ -2931,13 +2928,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B60" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C60" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D60">
         <v>13</v>
@@ -2965,13 +2962,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B61" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C61" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D61">
         <v>6</v>
@@ -2999,13 +2996,13 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="D62">
         <v>9</v>
@@ -3033,13 +3030,13 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B63" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C63" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D63">
         <v>8</v>
@@ -3067,13 +3064,13 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B64" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C64" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D64">
         <v>2</v>
@@ -3101,13 +3098,13 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B65" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C65" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D65">
         <v>3</v>
@@ -3135,13 +3132,13 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B66" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C66" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D66">
         <v>4</v>
@@ -3169,13 +3166,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D67">
         <v>4</v>
@@ -3203,13 +3200,13 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B68" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C68" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D68">
         <v>5</v>
@@ -3237,13 +3234,13 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B69" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C69" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D69">
         <v>6</v>
@@ -3271,13 +3268,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B70" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C70" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D70">
         <v>7</v>
@@ -3305,13 +3302,13 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B71" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C71" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D71">
         <v>8</v>
@@ -3339,13 +3336,13 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D72">
         <v>4</v>
@@ -3373,13 +3370,13 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B73" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C73" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D73">
         <v>10</v>
@@ -3407,13 +3404,13 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B74" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C74" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D74">
         <v>11</v>
@@ -3441,13 +3438,13 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B75" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D75">
         <v>12</v>
@@ -3475,13 +3472,13 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B76" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C76" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D76">
         <v>13</v>
@@ -3509,13 +3506,13 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B77" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C77" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D77">
         <v>6</v>
@@ -3543,13 +3540,13 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B78" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C78" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D78">
         <v>7</v>
@@ -3577,13 +3574,13 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B79" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C79" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D79">
         <v>8</v>
@@ -3611,13 +3608,13 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B80" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C80" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D80">
         <v>2</v>
@@ -3645,13 +3642,13 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B81" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C81" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D81">
         <v>3</v>
@@ -3679,13 +3676,13 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B82" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D82">
         <v>4</v>
@@ -3713,13 +3710,13 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B83" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C83" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D83">
         <v>5</v>
@@ -3747,13 +3744,13 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B84" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C84" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D84">
         <v>14</v>
@@ -3781,13 +3778,13 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B85" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C85" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D85">
         <v>9</v>
@@ -3815,13 +3812,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B86" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C86" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D86">
         <v>4</v>
@@ -3849,13 +3846,13 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B87" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C87" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D87">
         <v>10</v>
@@ -3883,13 +3880,13 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B88" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C88" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D88">
         <v>11</v>
@@ -3917,13 +3914,13 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B89" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C89" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D89">
         <v>12</v>
@@ -3951,13 +3948,13 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B90" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C90" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D90">
         <v>13</v>
@@ -3985,13 +3982,13 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B91" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C91" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D91">
         <v>6</v>
@@ -4019,13 +4016,13 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B92" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C92" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D92">
         <v>7</v>
@@ -4053,13 +4050,13 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B93" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C93" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D93">
         <v>8</v>
@@ -4087,13 +4084,13 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B94" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C94" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D94">
         <v>2</v>
@@ -4121,13 +4118,13 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B95" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C95" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D95">
         <v>3</v>
@@ -4155,13 +4152,13 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B96" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C96" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D96">
         <v>4</v>
@@ -4189,13 +4186,13 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B97" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C97" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D97">
         <v>5</v>
@@ -4223,13 +4220,13 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B98" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C98" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D98">
         <v>14</v>
@@ -4257,13 +4254,13 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B99" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C99" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D99">
         <v>9</v>
@@ -4291,13 +4288,13 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B100" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C100" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D100">
         <v>4</v>
@@ -4325,13 +4322,13 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B101" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C101" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D101">
         <v>10</v>
@@ -4359,13 +4356,13 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B102" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C102" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D102">
         <v>11</v>
@@ -4393,13 +4390,13 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B103" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C103" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D103">
         <v>12</v>
@@ -4427,13 +4424,13 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B104" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C104" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D104">
         <v>13</v>
@@ -4461,13 +4458,13 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B105" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C105" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D105">
         <v>6</v>
@@ -4495,13 +4492,13 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B106" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C106" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D106">
         <v>7</v>
@@ -4529,13 +4526,13 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B107" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C107" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D107">
         <v>8</v>
@@ -4563,13 +4560,13 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B108" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C108" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D108">
         <v>2</v>
@@ -4597,13 +4594,13 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B109" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C109" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D109">
         <v>3</v>
@@ -4631,13 +4628,13 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B110" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C110" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D110">
         <v>4</v>
@@ -4665,13 +4662,13 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B111" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C111" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D111">
         <v>5</v>
@@ -4699,13 +4696,13 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B112" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C112" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D112">
         <v>14</v>
@@ -4733,13 +4730,13 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B113" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C113" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D113">
         <v>9</v>
@@ -4767,13 +4764,13 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B114" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C114" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D114">
         <v>4</v>
@@ -4801,13 +4798,13 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B115" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="D115">
         <v>9</v>
@@ -4846,13 +4843,13 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B116" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C116" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D116">
         <v>5</v>
@@ -4880,13 +4877,13 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B117" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C117" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D117">
         <v>2</v>
@@ -4914,13 +4911,13 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B118" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C118" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D118">
         <v>3</v>
@@ -4948,13 +4945,13 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B119" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C119" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D119">
         <v>6</v>
@@ -4982,13 +4979,13 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B120" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C120" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D120">
         <v>7</v>
@@ -5016,13 +5013,13 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B121" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C121" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D121">
         <v>11</v>
@@ -5050,13 +5047,13 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B122" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C122" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D122">
         <v>12</v>
@@ -5084,13 +5081,13 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B123" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C123" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D123">
         <v>4</v>
@@ -5118,13 +5115,13 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B124" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C124" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D124">
         <v>9</v>
@@ -5152,13 +5149,13 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B125" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C125" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D125">
         <v>6</v>
@@ -5186,13 +5183,13 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B126" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C126" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D126">
         <v>7</v>
@@ -5220,13 +5217,13 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B127" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C127" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D127">
         <v>11</v>
@@ -5254,13 +5251,13 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B128" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C128" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D128">
         <v>12</v>
@@ -5288,13 +5285,13 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B129" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C129" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D129">
         <v>14</v>

</xml_diff>

<commit_message>
changes to excel key image mapping, new image
</commit_message>
<xml_diff>
--- a/prep/StreamdeckIconInputKeyMapping.xlsx
+++ b/prep/StreamdeckIconInputKeyMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irene\src\biz.dfch.PhoneTap\prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F561F6F-5C5D-4C1A-A34A-68D0A6F77724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E5459F-97C3-4803-AB02-31EE66E51630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{4419FAFA-D280-4090-97B7-CB07F6B7BE60}"/>
   </bookViews>
@@ -317,9 +317,6 @@
     <t>ic_fluent_bookmark_32_regular.svg</t>
   </si>
   <si>
-    <t>ic_fluent_skip_forward_30_48_regular.svg</t>
-  </si>
-  <si>
     <t>ic_fluent_skip_back_10_48_regular.svg</t>
   </si>
   <si>
@@ -516,6 +513,9 @@
   </si>
   <si>
     <t>ic_fluent_next_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_skip_forward_30_48_regular.png</t>
   </si>
 </sst>
 </file>
@@ -904,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47861C0B-96C3-4FC0-B828-7FD785B358D7}">
   <dimension ref="A1:I148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G160" sqref="G160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -954,10 +954,10 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1002,7 +1002,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -1047,7 +1047,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D4">
         <v>9</v>
@@ -1081,10 +1081,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1129,7 +1129,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1163,7 +1163,7 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1197,7 +1197,7 @@
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1228,10 +1228,10 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1276,7 +1276,7 @@
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -1310,7 +1310,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -1344,7 +1344,7 @@
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -1375,10 +1375,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1423,7 +1423,7 @@
         <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -1457,7 +1457,7 @@
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -1491,7 +1491,7 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D16">
         <v>6</v>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1570,7 +1570,7 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -1604,7 +1604,7 @@
         <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D19">
         <v>5</v>
@@ -1638,7 +1638,7 @@
         <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D20">
         <v>6</v>
@@ -1669,10 +1669,10 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1717,7 +1717,7 @@
         <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D22">
         <v>4</v>
@@ -1751,7 +1751,7 @@
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D23">
         <v>5</v>
@@ -1785,7 +1785,7 @@
         <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D24">
         <v>6</v>
@@ -1816,10 +1816,10 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1864,7 +1864,7 @@
         <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D26">
         <v>4</v>
@@ -1898,7 +1898,7 @@
         <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D27">
         <v>5</v>
@@ -1932,7 +1932,7 @@
         <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D28">
         <v>6</v>
@@ -1963,10 +1963,10 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2011,7 +2011,7 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D30">
         <v>4</v>
@@ -2045,7 +2045,7 @@
         <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D31">
         <v>5</v>
@@ -2079,7 +2079,7 @@
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D32">
         <v>6</v>
@@ -2110,10 +2110,10 @@
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2150,7 +2150,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D34">
         <v>4</v>
@@ -2192,7 +2192,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D35">
         <v>5</v>
@@ -2226,7 +2226,7 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D36">
         <v>6</v>
@@ -2260,7 +2260,7 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D37">
         <v>10</v>
@@ -2294,7 +2294,7 @@
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D38">
         <v>11</v>
@@ -2328,7 +2328,7 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D39">
         <v>12</v>
@@ -2362,7 +2362,7 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D40">
         <v>13</v>
@@ -2393,10 +2393,10 @@
         <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -2441,7 +2441,7 @@
         <v>33</v>
       </c>
       <c r="C42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D42">
         <v>4</v>
@@ -2475,7 +2475,7 @@
         <v>34</v>
       </c>
       <c r="C43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D43">
         <v>5</v>
@@ -2517,7 +2517,7 @@
         <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D44">
         <v>6</v>
@@ -2551,7 +2551,7 @@
         <v>36</v>
       </c>
       <c r="C45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D45">
         <v>10</v>
@@ -2585,7 +2585,7 @@
         <v>37</v>
       </c>
       <c r="C46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D46">
         <v>11</v>
@@ -2619,7 +2619,7 @@
         <v>38</v>
       </c>
       <c r="C47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D47">
         <v>12</v>
@@ -2653,7 +2653,7 @@
         <v>39</v>
       </c>
       <c r="C48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D48">
         <v>13</v>
@@ -2684,10 +2684,10 @@
         <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C49" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -2732,7 +2732,7 @@
         <v>33</v>
       </c>
       <c r="C50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D50">
         <v>4</v>
@@ -2766,7 +2766,7 @@
         <v>41</v>
       </c>
       <c r="C51" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D51">
         <v>5</v>
@@ -2808,7 +2808,7 @@
         <v>42</v>
       </c>
       <c r="C52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D52">
         <v>6</v>
@@ -2842,7 +2842,7 @@
         <v>43</v>
       </c>
       <c r="C53" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D53">
         <v>7</v>
@@ -2876,7 +2876,7 @@
         <v>44</v>
       </c>
       <c r="C54" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D54">
         <v>10</v>
@@ -2910,7 +2910,7 @@
         <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D55">
         <v>9</v>
@@ -2944,7 +2944,7 @@
         <v>45</v>
       </c>
       <c r="C56" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D56">
         <v>11</v>
@@ -2978,7 +2978,7 @@
         <v>46</v>
       </c>
       <c r="C57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D57">
         <v>14</v>
@@ -3009,10 +3009,10 @@
         <v>18</v>
       </c>
       <c r="B58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -3057,7 +3057,7 @@
         <v>4</v>
       </c>
       <c r="C59" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D59">
         <v>4</v>
@@ -3091,7 +3091,7 @@
         <v>48</v>
       </c>
       <c r="C60" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D60">
         <v>6</v>
@@ -3136,7 +3136,7 @@
         <v>49</v>
       </c>
       <c r="C61" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D61">
         <v>5</v>
@@ -3170,7 +3170,7 @@
         <v>50</v>
       </c>
       <c r="C62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D62">
         <v>7</v>
@@ -3204,7 +3204,7 @@
         <v>51</v>
       </c>
       <c r="C63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D63">
         <v>10</v>
@@ -3235,10 +3235,10 @@
         <v>29</v>
       </c>
       <c r="B64" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C64" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -3272,7 +3272,7 @@
         <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D65">
         <v>4</v>
@@ -3351,7 +3351,7 @@
         <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D67">
         <v>9</v>
@@ -3382,10 +3382,10 @@
         <v>28</v>
       </c>
       <c r="B68" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C68" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -3430,7 +3430,7 @@
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D69">
         <v>4</v>
@@ -3464,7 +3464,7 @@
         <v>52</v>
       </c>
       <c r="C70" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D70">
         <v>7</v>
@@ -3498,7 +3498,7 @@
         <v>53</v>
       </c>
       <c r="C71" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D71">
         <v>11</v>
@@ -3532,7 +3532,7 @@
         <v>54</v>
       </c>
       <c r="C72" t="s">
-        <v>92</v>
+        <v>158</v>
       </c>
       <c r="D72">
         <v>12</v>
@@ -3600,7 +3600,7 @@
         <v>56</v>
       </c>
       <c r="C74" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D74">
         <v>6</v>
@@ -3634,7 +3634,7 @@
         <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D75">
         <v>9</v>
@@ -3668,7 +3668,7 @@
         <v>57</v>
       </c>
       <c r="C76" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D76">
         <v>8</v>
@@ -3702,7 +3702,7 @@
         <v>58</v>
       </c>
       <c r="C77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D77">
         <v>2</v>
@@ -3736,7 +3736,7 @@
         <v>59</v>
       </c>
       <c r="C78" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D78">
         <v>3</v>
@@ -3801,10 +3801,10 @@
         <v>24</v>
       </c>
       <c r="B80" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C80" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -3849,7 +3849,7 @@
         <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D81">
         <v>4</v>
@@ -3883,7 +3883,7 @@
         <v>61</v>
       </c>
       <c r="C82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D82">
         <v>5</v>
@@ -3917,7 +3917,7 @@
         <v>62</v>
       </c>
       <c r="C83" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D83">
         <v>6</v>
@@ -3951,7 +3951,7 @@
         <v>63</v>
       </c>
       <c r="C84" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D84">
         <v>7</v>
@@ -3985,7 +3985,7 @@
         <v>64</v>
       </c>
       <c r="C85" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D85">
         <v>8</v>
@@ -4016,10 +4016,10 @@
         <v>25</v>
       </c>
       <c r="B86" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C86" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -4064,7 +4064,7 @@
         <v>4</v>
       </c>
       <c r="C87" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D87">
         <v>4</v>
@@ -4098,7 +4098,7 @@
         <v>65</v>
       </c>
       <c r="C88" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D88">
         <v>10</v>
@@ -4132,7 +4132,7 @@
         <v>66</v>
       </c>
       <c r="C89" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D89">
         <v>11</v>
@@ -4166,7 +4166,7 @@
         <v>67</v>
       </c>
       <c r="C90" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D90">
         <v>12</v>
@@ -4200,7 +4200,7 @@
         <v>68</v>
       </c>
       <c r="C91" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D91">
         <v>13</v>
@@ -4234,7 +4234,7 @@
         <v>69</v>
       </c>
       <c r="C92" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D92">
         <v>6</v>
@@ -4268,7 +4268,7 @@
         <v>70</v>
       </c>
       <c r="C93" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D93">
         <v>7</v>
@@ -4302,7 +4302,7 @@
         <v>71</v>
       </c>
       <c r="C94" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D94">
         <v>8</v>
@@ -4336,7 +4336,7 @@
         <v>72</v>
       </c>
       <c r="C95" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D95">
         <v>2</v>
@@ -4370,7 +4370,7 @@
         <v>73</v>
       </c>
       <c r="C96" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D96">
         <v>3</v>
@@ -4404,7 +4404,7 @@
         <v>74</v>
       </c>
       <c r="C97" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D97">
         <v>4</v>
@@ -4438,7 +4438,7 @@
         <v>75</v>
       </c>
       <c r="C98" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D98">
         <v>5</v>
@@ -4472,7 +4472,7 @@
         <v>76</v>
       </c>
       <c r="C99" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D99">
         <v>14</v>
@@ -4506,7 +4506,7 @@
         <v>77</v>
       </c>
       <c r="C100" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D100">
         <v>9</v>
@@ -4537,10 +4537,10 @@
         <v>27</v>
       </c>
       <c r="B101" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C101" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -4585,7 +4585,7 @@
         <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D102">
         <v>4</v>
@@ -4619,7 +4619,7 @@
         <v>65</v>
       </c>
       <c r="C103" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D103">
         <v>10</v>
@@ -4653,7 +4653,7 @@
         <v>66</v>
       </c>
       <c r="C104" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D104">
         <v>11</v>
@@ -4687,7 +4687,7 @@
         <v>67</v>
       </c>
       <c r="C105" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D105">
         <v>12</v>
@@ -4721,7 +4721,7 @@
         <v>68</v>
       </c>
       <c r="C106" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D106">
         <v>13</v>
@@ -4755,7 +4755,7 @@
         <v>69</v>
       </c>
       <c r="C107" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D107">
         <v>6</v>
@@ -4789,7 +4789,7 @@
         <v>70</v>
       </c>
       <c r="C108" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D108">
         <v>7</v>
@@ -4823,7 +4823,7 @@
         <v>71</v>
       </c>
       <c r="C109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D109">
         <v>8</v>
@@ -4857,7 +4857,7 @@
         <v>72</v>
       </c>
       <c r="C110" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D110">
         <v>2</v>
@@ -4891,7 +4891,7 @@
         <v>73</v>
       </c>
       <c r="C111" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D111">
         <v>3</v>
@@ -4925,7 +4925,7 @@
         <v>74</v>
       </c>
       <c r="C112" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D112">
         <v>4</v>
@@ -4959,7 +4959,7 @@
         <v>75</v>
       </c>
       <c r="C113" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D113">
         <v>5</v>
@@ -4993,7 +4993,7 @@
         <v>76</v>
       </c>
       <c r="C114" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D114">
         <v>14</v>
@@ -5027,7 +5027,7 @@
         <v>77</v>
       </c>
       <c r="C115" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D115">
         <v>9</v>
@@ -5058,10 +5058,10 @@
         <v>26</v>
       </c>
       <c r="B116" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C116" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -5106,7 +5106,7 @@
         <v>4</v>
       </c>
       <c r="C117" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D117">
         <v>4</v>
@@ -5140,7 +5140,7 @@
         <v>65</v>
       </c>
       <c r="C118" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D118">
         <v>10</v>
@@ -5174,7 +5174,7 @@
         <v>66</v>
       </c>
       <c r="C119" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D119">
         <v>11</v>
@@ -5208,7 +5208,7 @@
         <v>67</v>
       </c>
       <c r="C120" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D120">
         <v>12</v>
@@ -5242,7 +5242,7 @@
         <v>68</v>
       </c>
       <c r="C121" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D121">
         <v>13</v>
@@ -5276,7 +5276,7 @@
         <v>69</v>
       </c>
       <c r="C122" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D122">
         <v>6</v>
@@ -5310,7 +5310,7 @@
         <v>70</v>
       </c>
       <c r="C123" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D123">
         <v>7</v>
@@ -5344,7 +5344,7 @@
         <v>71</v>
       </c>
       <c r="C124" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D124">
         <v>8</v>
@@ -5378,7 +5378,7 @@
         <v>72</v>
       </c>
       <c r="C125" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D125">
         <v>2</v>
@@ -5412,7 +5412,7 @@
         <v>73</v>
       </c>
       <c r="C126" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D126">
         <v>3</v>
@@ -5446,7 +5446,7 @@
         <v>74</v>
       </c>
       <c r="C127" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D127">
         <v>4</v>
@@ -5480,7 +5480,7 @@
         <v>75</v>
       </c>
       <c r="C128" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D128">
         <v>5</v>
@@ -5514,7 +5514,7 @@
         <v>76</v>
       </c>
       <c r="C129" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D129">
         <v>14</v>
@@ -5548,7 +5548,7 @@
         <v>77</v>
       </c>
       <c r="C130" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D130">
         <v>9</v>
@@ -5579,10 +5579,10 @@
         <v>30</v>
       </c>
       <c r="B131" t="s">
+        <v>128</v>
+      </c>
+      <c r="C131" t="s">
         <v>129</v>
-      </c>
-      <c r="C131" t="s">
-        <v>130</v>
       </c>
       <c r="D131">
         <v>0</v>
@@ -5627,7 +5627,7 @@
         <v>4</v>
       </c>
       <c r="C132" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D132">
         <v>4</v>
@@ -5661,7 +5661,7 @@
         <v>5</v>
       </c>
       <c r="C133" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D133">
         <v>9</v>
@@ -5706,7 +5706,7 @@
         <v>78</v>
       </c>
       <c r="C134" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D134">
         <v>5</v>
@@ -5740,7 +5740,7 @@
         <v>79</v>
       </c>
       <c r="C135" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D135">
         <v>2</v>
@@ -5774,7 +5774,7 @@
         <v>80</v>
       </c>
       <c r="C136" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D136">
         <v>3</v>
@@ -5808,7 +5808,7 @@
         <v>81</v>
       </c>
       <c r="C137" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D137">
         <v>6</v>
@@ -5842,7 +5842,7 @@
         <v>82</v>
       </c>
       <c r="C138" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D138">
         <v>7</v>
@@ -5876,7 +5876,7 @@
         <v>83</v>
       </c>
       <c r="C139" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D139">
         <v>11</v>
@@ -5910,7 +5910,7 @@
         <v>84</v>
       </c>
       <c r="C140" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D140">
         <v>12</v>
@@ -5941,10 +5941,10 @@
         <v>8</v>
       </c>
       <c r="B141" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C141" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D141">
         <v>0</v>
@@ -5989,7 +5989,7 @@
         <v>4</v>
       </c>
       <c r="C142" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D142">
         <v>4</v>
@@ -6023,7 +6023,7 @@
         <v>85</v>
       </c>
       <c r="C143" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D143">
         <v>9</v>
@@ -6057,7 +6057,7 @@
         <v>86</v>
       </c>
       <c r="C144" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D144">
         <v>6</v>
@@ -6125,7 +6125,7 @@
         <v>88</v>
       </c>
       <c r="C146" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D146">
         <v>11</v>
@@ -6159,7 +6159,7 @@
         <v>89</v>
       </c>
       <c r="C147" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D147">
         <v>12</v>
@@ -6193,7 +6193,7 @@
         <v>46</v>
       </c>
       <c r="C148" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D148">
         <v>14</v>

</xml_diff>

<commit_message>
changes to the excel key image mapping, new images
</commit_message>
<xml_diff>
--- a/prep/StreamdeckIconInputKeyMapping.xlsx
+++ b/prep/StreamdeckIconInputKeyMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irene\src\biz.dfch.PhoneTap\prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E5459F-97C3-4803-AB02-31EE66E51630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388EC602-BC47-46BF-8688-C8E179424866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{4419FAFA-D280-4090-97B7-CB07F6B7BE60}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="158">
   <si>
     <t>States</t>
   </si>
@@ -161,9 +161,6 @@
     <t>        CLEAN_DEVICE = InputEventMap.KEY_9</t>
   </si>
   <si>
-    <t>ic_fluent_usb_stick_24_regular.svg</t>
-  </si>
-  <si>
     <t>        START_RECORDING_MX0 = InputEventMap.KEY_1</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
     <t>        STOP_SYSTEM = InputEventMap.KEY_9</t>
   </si>
   <si>
-    <t>ic_fluent_play_48_regular.svg</t>
-  </si>
-  <si>
     <t>        STOP_RECORDING = InputEventMap.KEY_1</t>
   </si>
   <si>
@@ -311,87 +305,9 @@
     <t>        SET_TIME = InputEventMap.KEY_6</t>
   </si>
   <si>
-    <t>ic_fluent_bookmark_multiple_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_bookmark_32_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_skip_back_10_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_previous_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_previous_frame_24_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_next_frame_24_regular.svg</t>
-  </si>
-  <si>
-    <t>it.svg</t>
-  </si>
-  <si>
-    <t>de.svg</t>
-  </si>
-  <si>
-    <t>fr.svg</t>
-  </si>
-  <si>
-    <t>gb.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_backspace_24_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_arrow_enter_left_24_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_number_circle_0_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_number_circle_1_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_number_circle_2_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_number_circle_3_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_number_circle_4_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_number_circle_5_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_number_circle_6_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_number_circle_7_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_number_circle_8_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_number_circle_9_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_plug_disconnected_48_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_time_picker_24_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_calendar_edit_32_regular.svg</t>
-  </si>
-  <si>
     <t xml:space="preserve">        SCREEN = InputEventMap.KEY_ASTERISK</t>
   </si>
   <si>
-    <t>ic_fluent_globe_48_regular.svg</t>
-  </si>
-  <si>
     <t>ic_fluent_lightbulb_48_regular.png</t>
   </si>
   <si>
@@ -428,21 +344,6 @@
     <t>        SCREEN = InputEventMap.KEY_ASTERISK</t>
   </si>
   <si>
-    <t>ic_fluent_usb_stick_24_regular_pink.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_time_picker_24_regular_pink.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_text_edit_style_character_a_32_regular_pink.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_calendar_edit_32_regular_pink.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_globe_48_regular_pink.svg</t>
-  </si>
-  <si>
     <t>ic_fluent_speaker_2_48_regular_pink.png</t>
   </si>
   <si>
@@ -452,12 +353,6 @@
     <t>ic_fluent_phone_48_regular_green.png</t>
   </si>
   <si>
-    <t>ic_fluent_keyboard_tab_24_regular.svg</t>
-  </si>
-  <si>
-    <t>ic_fluent_settings_48_regular_pink.svg</t>
-  </si>
-  <si>
     <t>ic_fluent_power_28_regular.png</t>
   </si>
   <si>
@@ -516,6 +411,108 @@
   </si>
   <si>
     <t>ic_fluent_skip_forward_30_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_skip_forward_bookmark_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_skip_back_bookmark_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_previous_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_next_frame_24_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_previous_frame_24_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_skip_back_10_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_globe_48_regular_pink.png</t>
+  </si>
+  <si>
+    <t>gb.png</t>
+  </si>
+  <si>
+    <t>de.png</t>
+  </si>
+  <si>
+    <t>fr.png</t>
+  </si>
+  <si>
+    <t>it.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_calendar_edit_32_regular_pink.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_number_circle_0_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_number_circle_1_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_number_circle_2_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_number_circle_3_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_number_circle_4_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_number_circle_5_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_number_circle_6_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_number_circle_7_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_number_circle_8_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_number_circle_9_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_backspace_24_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_arrow_enter_left_24_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_keyboard_tab_24_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_text_edit_style_character_a_32_regular_pink.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_time_picker_24_regular_pink.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_usb_stick_24_regular_pink.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_plug_disconnected_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_settings_48_regular_pink.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_globe_48_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_usb_stick_24_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_calendar_edit_32_regular.png</t>
+  </si>
+  <si>
+    <t>ic_fluent_time_picker_24_regular.png</t>
   </si>
 </sst>
 </file>
@@ -545,12 +542,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -565,9 +568,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47861C0B-96C3-4FC0-B828-7FD785B358D7}">
   <dimension ref="A1:I148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G160" sqref="G160"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C150" sqref="C150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -954,10 +958,10 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -981,7 +985,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G2" t="str">
+      <c r="G2" s="2" t="str">
         <f t="shared" ref="G2" si="1">_xlfn.CONCAT(A2, "-", F2, "-", E2, ".png")</f>
         <v>FinalState-KEY_00-screen.png</v>
       </c>
@@ -1002,7 +1006,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -1026,7 +1030,7 @@
 )</f>
         <v>KEY_04</v>
       </c>
-      <c r="G3" t="str">
+      <c r="G3" s="2" t="str">
         <f t="shared" ref="G3:G33" si="4">_xlfn.CONCAT(A3, "-", F3, "-", E3, ".png")</f>
         <v>FinalState-KEY_04-help.png</v>
       </c>
@@ -1047,7 +1051,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="D4">
         <v>9</v>
@@ -1063,7 +1067,7 @@
 )</f>
         <v>KEY_09</v>
       </c>
-      <c r="G4" t="str">
+      <c r="G4" s="2" t="str">
         <f t="shared" si="4"/>
         <v>FinalState-KEY_09-menu.png</v>
       </c>
@@ -1081,10 +1085,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1108,7 +1112,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G5" t="str">
+      <c r="G5" s="2" t="str">
         <f t="shared" ref="G5" si="10">_xlfn.CONCAT(A5, "-", F5, "-", E5, ".png")</f>
         <v>InitialiseAudio-KEY_00-screen.png</v>
       </c>
@@ -1129,7 +1133,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1142,7 +1146,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G6" t="str">
+      <c r="G6" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseAudio-KEY_04-help.png</v>
       </c>
@@ -1163,7 +1167,7 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1176,7 +1180,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G7" t="str">
+      <c r="G7" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseAudio-KEY_05-init_audio.png</v>
       </c>
@@ -1197,7 +1201,7 @@
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1210,7 +1214,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G8" t="str">
+      <c r="G8" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseAudio-KEY_06-skip_audio.png</v>
       </c>
@@ -1228,10 +1232,10 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1255,7 +1259,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G9" t="str">
+      <c r="G9" s="2" t="str">
         <f t="shared" ref="G9" si="15">_xlfn.CONCAT(A9, "-", F9, "-", E9, ".png")</f>
         <v>InitialiseEx1-KEY_00-screen.png</v>
       </c>
@@ -1276,7 +1280,7 @@
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -1289,7 +1293,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G10" t="str">
+      <c r="G10" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseEx1-KEY_04-help.png</v>
       </c>
@@ -1310,7 +1314,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -1323,7 +1327,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G11" t="str">
+      <c r="G11" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseEx1-KEY_05-detect_device.png</v>
       </c>
@@ -1344,7 +1348,7 @@
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -1357,7 +1361,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G12" t="str">
+      <c r="G12" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseEx1-KEY_06-skip_device.png</v>
       </c>
@@ -1375,10 +1379,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1402,7 +1406,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G13" t="str">
+      <c r="G13" s="2" t="str">
         <f t="shared" ref="G13" si="20">_xlfn.CONCAT(A13, "-", F13, "-", E13, ".png")</f>
         <v>InitialiseEx2-KEY_00-screen.png</v>
       </c>
@@ -1423,7 +1427,7 @@
         <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -1436,7 +1440,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G14" t="str">
+      <c r="G14" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseEx2-KEY_04-help.png</v>
       </c>
@@ -1457,7 +1461,7 @@
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -1470,7 +1474,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G15" t="str">
+      <c r="G15" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseEx2-KEY_05-detect_device.png</v>
       </c>
@@ -1491,7 +1495,7 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="D16">
         <v>6</v>
@@ -1504,7 +1508,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G16" t="str">
+      <c r="G16" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseEx2-KEY_06-skip_device.png</v>
       </c>
@@ -1522,10 +1526,10 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="C17" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1549,7 +1553,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G17" t="str">
+      <c r="G17" s="2" t="str">
         <f t="shared" ref="G17" si="25">_xlfn.CONCAT(A17, "-", F17, "-", E17, ".png")</f>
         <v>InitialiseHi1-KEY_00-screen.png</v>
       </c>
@@ -1570,7 +1574,7 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -1583,7 +1587,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G18" t="str">
+      <c r="G18" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi1-KEY_04-help.png</v>
       </c>
@@ -1604,7 +1608,7 @@
         <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="D19">
         <v>5</v>
@@ -1617,7 +1621,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G19" t="str">
+      <c r="G19" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi1-KEY_05-detect_device.png</v>
       </c>
@@ -1638,7 +1642,7 @@
         <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="D20">
         <v>6</v>
@@ -1651,7 +1655,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G20" t="str">
+      <c r="G20" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi1-KEY_06-skip_device.png</v>
       </c>
@@ -1669,10 +1673,10 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="C21" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1696,7 +1700,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G21" t="str">
+      <c r="G21" s="2" t="str">
         <f t="shared" ref="G21" si="30">_xlfn.CONCAT(A21, "-", F21, "-", E21, ".png")</f>
         <v>InitialiseHi2-KEY_00-screen.png</v>
       </c>
@@ -1717,7 +1721,7 @@
         <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D22">
         <v>4</v>
@@ -1730,7 +1734,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G22" t="str">
+      <c r="G22" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi2-KEY_04-help.png</v>
       </c>
@@ -1751,7 +1755,7 @@
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="D23">
         <v>5</v>
@@ -1764,7 +1768,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G23" t="str">
+      <c r="G23" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi2-KEY_05-detect_device.png</v>
       </c>
@@ -1785,7 +1789,7 @@
         <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="D24">
         <v>6</v>
@@ -1798,7 +1802,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G24" t="str">
+      <c r="G24" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi2-KEY_06-skip_device.png</v>
       </c>
@@ -1816,10 +1820,10 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1843,7 +1847,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G25" t="str">
+      <c r="G25" s="2" t="str">
         <f t="shared" ref="G25" si="35">_xlfn.CONCAT(A25, "-", F25, "-", E25, ".png")</f>
         <v>InitialiseHi3-KEY_00-screen.png</v>
       </c>
@@ -1864,7 +1868,7 @@
         <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D26">
         <v>4</v>
@@ -1877,7 +1881,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G26" t="str">
+      <c r="G26" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi3-KEY_04-help.png</v>
       </c>
@@ -1898,7 +1902,7 @@
         <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="D27">
         <v>5</v>
@@ -1911,7 +1915,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G27" t="str">
+      <c r="G27" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi3-KEY_05-detect_device.png</v>
       </c>
@@ -1932,7 +1936,7 @@
         <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="D28">
         <v>6</v>
@@ -1945,7 +1949,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G28" t="str">
+      <c r="G28" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi3-KEY_06-skip_device.png</v>
       </c>
@@ -1963,10 +1967,10 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1990,7 +1994,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G29" t="str">
+      <c r="G29" s="2" t="str">
         <f t="shared" ref="G29" si="40">_xlfn.CONCAT(A29, "-", F29, "-", E29, ".png")</f>
         <v>InitialiseLcl-KEY_00-screen.png</v>
       </c>
@@ -2011,7 +2015,7 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D30">
         <v>4</v>
@@ -2024,7 +2028,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G30" t="str">
+      <c r="G30" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseLcl-KEY_04-help.png</v>
       </c>
@@ -2045,7 +2049,7 @@
         <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="D31">
         <v>5</v>
@@ -2058,7 +2062,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G31" t="str">
+      <c r="G31" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseLcl-KEY_05-detect_device.png</v>
       </c>
@@ -2079,7 +2083,7 @@
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="D32">
         <v>6</v>
@@ -2092,7 +2096,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G32" t="str">
+      <c r="G32" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseLcl-KEY_06-skip_device.png</v>
       </c>
@@ -2110,10 +2114,10 @@
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="C33" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2129,7 +2133,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G33" t="str">
+      <c r="G33" s="2" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseRc1-KEY_00-screen.png</v>
       </c>
@@ -2150,7 +2154,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D34">
         <v>4</v>
@@ -2171,7 +2175,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G34" t="str">
+      <c r="G34" s="2" t="str">
         <f t="shared" ref="G34:G42" si="45">_xlfn.CONCAT(A34, "-", F34, "-", E34, ".png")</f>
         <v>InitialiseRc1-KEY_04-help.png</v>
       </c>
@@ -2192,7 +2196,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="D35">
         <v>5</v>
@@ -2205,7 +2209,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G35" t="str">
+      <c r="G35" s="2" t="str">
         <f t="shared" si="45"/>
         <v>InitialiseRc1-KEY_05-detect_device.png</v>
       </c>
@@ -2226,7 +2230,7 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="D36">
         <v>6</v>
@@ -2239,7 +2243,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G36" t="str">
+      <c r="G36" s="2" t="str">
         <f t="shared" si="45"/>
         <v>InitialiseRc1-KEY_06-skip_device.png</v>
       </c>
@@ -2260,7 +2264,7 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="D37">
         <v>10</v>
@@ -2273,7 +2277,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0A</v>
       </c>
-      <c r="G37" t="str">
+      <c r="G37" s="2" t="str">
         <f t="shared" si="45"/>
         <v>InitialiseRc1-KEY_0A-format_device.png</v>
       </c>
@@ -2294,7 +2298,7 @@
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="D38">
         <v>11</v>
@@ -2307,7 +2311,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0B</v>
       </c>
-      <c r="G38" t="str">
+      <c r="G38" s="2" t="str">
         <f t="shared" si="45"/>
         <v>InitialiseRc1-KEY_0B-mount_device.png</v>
       </c>
@@ -2328,7 +2332,7 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="D39">
         <v>12</v>
@@ -2341,7 +2345,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0C</v>
       </c>
-      <c r="G39" t="str">
+      <c r="G39" s="2" t="str">
         <f t="shared" si="45"/>
         <v>InitialiseRc1-KEY_0C-unmount_device.png</v>
       </c>
@@ -2362,7 +2366,7 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="D40">
         <v>13</v>
@@ -2375,7 +2379,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0D</v>
       </c>
-      <c r="G40" t="str">
+      <c r="G40" s="2" t="str">
         <f t="shared" si="45"/>
         <v>InitialiseRc1-KEY_0D-clean_device.png</v>
       </c>
@@ -2393,10 +2397,10 @@
         <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="C41" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -2420,7 +2424,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G41" t="str">
+      <c r="G41" s="2" t="str">
         <f t="shared" ref="G41" si="50">_xlfn.CONCAT(A41, "-", F41, "-", E41, ".png")</f>
         <v>InitialiseRc2-KEY_00-screen.png</v>
       </c>
@@ -2441,7 +2445,7 @@
         <v>33</v>
       </c>
       <c r="C42" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D42">
         <v>4</v>
@@ -2454,7 +2458,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G42" t="str">
+      <c r="G42" s="2" t="str">
         <f t="shared" si="45"/>
         <v>InitialiseRc2-KEY_04-help.png</v>
       </c>
@@ -2475,7 +2479,7 @@
         <v>34</v>
       </c>
       <c r="C43" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="D43">
         <v>5</v>
@@ -2496,7 +2500,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G43" t="str">
+      <c r="G43" s="2" t="str">
         <f t="shared" ref="G43:G50" si="54">_xlfn.CONCAT(A43, "-", F43, "-", E43, ".png")</f>
         <v>InitialiseRc2-KEY_05-detect_device.png</v>
       </c>
@@ -2517,7 +2521,7 @@
         <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="D44">
         <v>6</v>
@@ -2530,7 +2534,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G44" t="str">
+      <c r="G44" s="2" t="str">
         <f t="shared" si="54"/>
         <v>InitialiseRc2-KEY_06-skip_device.png</v>
       </c>
@@ -2551,7 +2555,7 @@
         <v>36</v>
       </c>
       <c r="C45" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="D45">
         <v>10</v>
@@ -2564,7 +2568,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0A</v>
       </c>
-      <c r="G45" t="str">
+      <c r="G45" s="2" t="str">
         <f t="shared" si="54"/>
         <v>InitialiseRc2-KEY_0A-format_device.png</v>
       </c>
@@ -2585,7 +2589,7 @@
         <v>37</v>
       </c>
       <c r="C46" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="D46">
         <v>11</v>
@@ -2598,7 +2602,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0B</v>
       </c>
-      <c r="G46" t="str">
+      <c r="G46" s="2" t="str">
         <f t="shared" si="54"/>
         <v>InitialiseRc2-KEY_0B-mount_device.png</v>
       </c>
@@ -2619,7 +2623,7 @@
         <v>38</v>
       </c>
       <c r="C47" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="D47">
         <v>12</v>
@@ -2632,7 +2636,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0C</v>
       </c>
-      <c r="G47" t="str">
+      <c r="G47" s="2" t="str">
         <f t="shared" si="54"/>
         <v>InitialiseRc2-KEY_0C-unmount_device.png</v>
       </c>
@@ -2653,7 +2657,7 @@
         <v>39</v>
       </c>
       <c r="C48" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="D48">
         <v>13</v>
@@ -2666,7 +2670,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0D</v>
       </c>
-      <c r="G48" t="str">
+      <c r="G48" s="2" t="str">
         <f t="shared" si="54"/>
         <v>InitialiseRc2-KEY_0D-clean_device.png</v>
       </c>
@@ -2684,10 +2688,10 @@
         <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="C49" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -2711,7 +2715,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G49" t="str">
+      <c r="G49" s="2" t="str">
         <f t="shared" ref="G49" si="59">_xlfn.CONCAT(A49, "-", F49, "-", E49, ".png")</f>
         <v>Main-KEY_00-screen.png</v>
       </c>
@@ -2732,7 +2736,7 @@
         <v>33</v>
       </c>
       <c r="C50" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D50">
         <v>4</v>
@@ -2745,7 +2749,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G50" t="str">
+      <c r="G50" s="2" t="str">
         <f t="shared" si="54"/>
         <v>Main-KEY_04-help.png</v>
       </c>
@@ -2763,10 +2767,10 @@
         <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C51" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="D51">
         <v>5</v>
@@ -2787,7 +2791,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G51" t="str">
+      <c r="G51" s="2" t="str">
         <f t="shared" ref="G51:G56" si="63">_xlfn.CONCAT(A51, "-", F51, "-", E51, ".png")</f>
         <v>Main-KEY_05-start_recording_mx0.png</v>
       </c>
@@ -2805,10 +2809,10 @@
         <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C52" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="D52">
         <v>6</v>
@@ -2821,7 +2825,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G52" t="str">
+      <c r="G52" s="2" t="str">
         <f t="shared" si="63"/>
         <v>Main-KEY_06-start_recording_mx1.png</v>
       </c>
@@ -2839,10 +2843,10 @@
         <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C53" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="D53">
         <v>7</v>
@@ -2855,7 +2859,7 @@
         <f t="shared" si="6"/>
         <v>KEY_07</v>
       </c>
-      <c r="G53" t="str">
+      <c r="G53" s="2" t="str">
         <f t="shared" si="63"/>
         <v>Main-KEY_07-start_recording_mx2.png</v>
       </c>
@@ -2873,10 +2877,10 @@
         <v>7</v>
       </c>
       <c r="B54" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C54" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="D54">
         <v>10</v>
@@ -2889,7 +2893,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0A</v>
       </c>
-      <c r="G54" t="str">
+      <c r="G54" s="2" t="str">
         <f t="shared" si="63"/>
         <v>Main-KEY_0A-start_playback.png</v>
       </c>
@@ -2910,7 +2914,7 @@
         <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="D55">
         <v>9</v>
@@ -2923,7 +2927,7 @@
         <f t="shared" si="6"/>
         <v>KEY_09</v>
       </c>
-      <c r="G55" t="str">
+      <c r="G55" s="2" t="str">
         <f t="shared" si="63"/>
         <v>Main-KEY_09-menu.png</v>
       </c>
@@ -2941,10 +2945,10 @@
         <v>7</v>
       </c>
       <c r="B56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C56" t="s">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="D56">
         <v>11</v>
@@ -2957,7 +2961,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0B</v>
       </c>
-      <c r="G56" t="str">
+      <c r="G56" s="2" t="str">
         <f t="shared" si="63"/>
         <v>Main-KEY_0B-set_name.png</v>
       </c>
@@ -2975,10 +2979,10 @@
         <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C57" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="D57">
         <v>14</v>
@@ -2991,7 +2995,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0E</v>
       </c>
-      <c r="G57" t="str">
+      <c r="G57" s="2" t="str">
         <f t="shared" ref="G57:G59" si="66">_xlfn.CONCAT(A57, "-", F57, "-", E57, ".png")</f>
         <v>Main-KEY_0E-stop_system.png</v>
       </c>
@@ -3009,10 +3013,10 @@
         <v>18</v>
       </c>
       <c r="B58" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="C58" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -3036,7 +3040,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G58" t="str">
+      <c r="G58" s="2" t="str">
         <f t="shared" ref="G58" si="71">_xlfn.CONCAT(A58, "-", F58, "-", E58, ".png")</f>
         <v>OnRecord-KEY_00-screen.png</v>
       </c>
@@ -3057,7 +3061,7 @@
         <v>4</v>
       </c>
       <c r="C59" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D59">
         <v>4</v>
@@ -3070,7 +3074,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G59" t="str">
+      <c r="G59" s="2" t="str">
         <f t="shared" si="66"/>
         <v>OnRecord-KEY_04-help.png</v>
       </c>
@@ -3088,10 +3092,10 @@
         <v>18</v>
       </c>
       <c r="B60" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C60" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="D60">
         <v>6</v>
@@ -3115,7 +3119,7 @@
 )</f>
         <v>KEY_06</v>
       </c>
-      <c r="G60" t="str">
+      <c r="G60" s="2" t="str">
         <f t="shared" ref="G60:G64" si="76">_xlfn.CONCAT(A60, "-", F60, "-", E60, ".png")</f>
         <v>OnRecord-KEY_06-stop_recording.png</v>
       </c>
@@ -3133,10 +3137,10 @@
         <v>18</v>
       </c>
       <c r="B61" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C61" t="s">
-        <v>152</v>
+        <v>117</v>
       </c>
       <c r="D61">
         <v>5</v>
@@ -3149,7 +3153,7 @@
         <f t="shared" si="75"/>
         <v>KEY_05</v>
       </c>
-      <c r="G61" t="str">
+      <c r="G61" s="2" t="str">
         <f t="shared" si="76"/>
         <v>OnRecord-KEY_05-set_cue.png</v>
       </c>
@@ -3167,10 +3171,10 @@
         <v>18</v>
       </c>
       <c r="B62" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C62" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="D62">
         <v>7</v>
@@ -3183,7 +3187,7 @@
         <f t="shared" si="75"/>
         <v>KEY_07</v>
       </c>
-      <c r="G62" t="str">
+      <c r="G62" s="2" t="str">
         <f t="shared" si="76"/>
         <v>OnRecord-KEY_07-toggle_mute.png</v>
       </c>
@@ -3201,10 +3205,10 @@
         <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C63" t="s">
-        <v>154</v>
+        <v>119</v>
       </c>
       <c r="D63">
         <v>10</v>
@@ -3217,7 +3221,7 @@
         <f t="shared" si="75"/>
         <v>KEY_0A</v>
       </c>
-      <c r="G63" t="str">
+      <c r="G63" s="2" t="str">
         <f t="shared" si="76"/>
         <v>OnRecord-KEY_0A-show_status.png</v>
       </c>
@@ -3235,10 +3239,10 @@
         <v>29</v>
       </c>
       <c r="B64" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="C64" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -3251,7 +3255,7 @@
         <f t="shared" si="75"/>
         <v>KEY_00</v>
       </c>
-      <c r="G64" t="str">
+      <c r="G64" s="2" t="str">
         <f t="shared" si="76"/>
         <v>PlaybackPaused-KEY_00-screen.png</v>
       </c>
@@ -3272,7 +3276,7 @@
         <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D65">
         <v>4</v>
@@ -3296,7 +3300,7 @@
 )</f>
         <v>KEY_04</v>
       </c>
-      <c r="G65" t="str">
+      <c r="G65" s="2" t="str">
         <f t="shared" ref="G65:G132" si="81">_xlfn.CONCAT(A65, "-", F65, "-", E65, ".png")</f>
         <v>PlaybackPaused-KEY_04-help.png</v>
       </c>
@@ -3314,10 +3318,10 @@
         <v>29</v>
       </c>
       <c r="B66" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C66" t="s">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="D66">
         <v>5</v>
@@ -3330,7 +3334,7 @@
         <f t="shared" si="80"/>
         <v>KEY_05</v>
       </c>
-      <c r="G66" t="str">
+      <c r="G66" s="2" t="str">
         <f t="shared" si="81"/>
         <v>PlaybackPaused-KEY_05-pause_resume.png</v>
       </c>
@@ -3351,7 +3355,7 @@
         <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="D67">
         <v>9</v>
@@ -3364,7 +3368,7 @@
         <f t="shared" si="80"/>
         <v>KEY_09</v>
       </c>
-      <c r="G67" t="str">
+      <c r="G67" s="2" t="str">
         <f t="shared" si="81"/>
         <v>PlaybackPaused-KEY_09-menu.png</v>
       </c>
@@ -3382,10 +3386,10 @@
         <v>28</v>
       </c>
       <c r="B68" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="C68" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -3409,7 +3413,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G68" t="str">
+      <c r="G68" s="2" t="str">
         <f t="shared" ref="G68" si="86">_xlfn.CONCAT(A68, "-", F68, "-", E68, ".png")</f>
         <v>Playback-KEY_00-screen.png</v>
       </c>
@@ -3430,7 +3434,7 @@
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D69">
         <v>4</v>
@@ -3443,7 +3447,7 @@
         <f t="shared" si="80"/>
         <v>KEY_04</v>
       </c>
-      <c r="G69" t="str">
+      <c r="G69" s="2" t="str">
         <f t="shared" si="81"/>
         <v>Playback-KEY_04-help.png</v>
       </c>
@@ -3461,10 +3465,10 @@
         <v>28</v>
       </c>
       <c r="B70" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C70" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="D70">
         <v>7</v>
@@ -3477,7 +3481,7 @@
         <f t="shared" si="80"/>
         <v>KEY_07</v>
       </c>
-      <c r="G70" t="str">
+      <c r="G70" s="2" t="str">
         <f t="shared" si="81"/>
         <v>Playback-KEY_07-pause_resume.png</v>
       </c>
@@ -3495,10 +3499,10 @@
         <v>28</v>
       </c>
       <c r="B71" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C71" t="s">
-        <v>157</v>
+        <v>122</v>
       </c>
       <c r="D71">
         <v>11</v>
@@ -3511,7 +3515,7 @@
         <f t="shared" si="80"/>
         <v>KEY_0B</v>
       </c>
-      <c r="G71" t="str">
+      <c r="G71" s="2" t="str">
         <f t="shared" si="81"/>
         <v>Playback-KEY_0B-jump_clip_end.png</v>
       </c>
@@ -3529,10 +3533,10 @@
         <v>28</v>
       </c>
       <c r="B72" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C72" t="s">
-        <v>158</v>
+        <v>123</v>
       </c>
       <c r="D72">
         <v>12</v>
@@ -3545,7 +3549,7 @@
         <f t="shared" si="80"/>
         <v>KEY_0C</v>
       </c>
-      <c r="G72" t="str">
+      <c r="G72" s="2" t="str">
         <f t="shared" si="81"/>
         <v>Playback-KEY_0C-seek_next.png</v>
       </c>
@@ -3563,10 +3567,10 @@
         <v>28</v>
       </c>
       <c r="B73" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C73" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="D73">
         <v>13</v>
@@ -3579,7 +3583,7 @@
         <f t="shared" si="80"/>
         <v>KEY_0D</v>
       </c>
-      <c r="G73" t="str">
+      <c r="G73" s="2" t="str">
         <f t="shared" si="81"/>
         <v>Playback-KEY_0D-jump_cue_next.png</v>
       </c>
@@ -3597,10 +3601,10 @@
         <v>28</v>
       </c>
       <c r="B74" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C74" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="D74">
         <v>6</v>
@@ -3634,7 +3638,7 @@
         <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="D75">
         <v>9</v>
@@ -3665,10 +3669,10 @@
         <v>28</v>
       </c>
       <c r="B76" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C76" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="D76">
         <v>8</v>
@@ -3699,10 +3703,10 @@
         <v>28</v>
       </c>
       <c r="B77" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C77" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="D77">
         <v>2</v>
@@ -3733,10 +3737,10 @@
         <v>28</v>
       </c>
       <c r="B78" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C78" t="s">
-        <v>92</v>
+        <v>129</v>
       </c>
       <c r="D78">
         <v>3</v>
@@ -3767,10 +3771,10 @@
         <v>28</v>
       </c>
       <c r="B79" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C79" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="D79">
         <v>4</v>
@@ -3801,10 +3805,10 @@
         <v>24</v>
       </c>
       <c r="B80" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="C80" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -3849,7 +3853,7 @@
         <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D81">
         <v>4</v>
@@ -3880,10 +3884,10 @@
         <v>24</v>
       </c>
       <c r="B82" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C82" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="D82">
         <v>5</v>
@@ -3914,10 +3918,10 @@
         <v>24</v>
       </c>
       <c r="B83" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C83" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="D83">
         <v>6</v>
@@ -3948,10 +3952,10 @@
         <v>24</v>
       </c>
       <c r="B84" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C84" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="D84">
         <v>7</v>
@@ -3982,10 +3986,10 @@
         <v>24</v>
       </c>
       <c r="B85" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C85" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="D85">
         <v>8</v>
@@ -4016,10 +4020,10 @@
         <v>25</v>
       </c>
       <c r="B86" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="C86" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -4064,7 +4068,7 @@
         <v>4</v>
       </c>
       <c r="C87" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D87">
         <v>4</v>
@@ -4095,10 +4099,10 @@
         <v>25</v>
       </c>
       <c r="B88" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C88" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="D88">
         <v>10</v>
@@ -4129,10 +4133,10 @@
         <v>25</v>
       </c>
       <c r="B89" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C89" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="D89">
         <v>11</v>
@@ -4163,10 +4167,10 @@
         <v>25</v>
       </c>
       <c r="B90" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C90" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="D90">
         <v>12</v>
@@ -4197,10 +4201,10 @@
         <v>25</v>
       </c>
       <c r="B91" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C91" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="D91">
         <v>13</v>
@@ -4231,10 +4235,10 @@
         <v>25</v>
       </c>
       <c r="B92" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C92" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
       <c r="D92">
         <v>6</v>
@@ -4265,10 +4269,10 @@
         <v>25</v>
       </c>
       <c r="B93" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C93" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="D93">
         <v>7</v>
@@ -4299,10 +4303,10 @@
         <v>25</v>
       </c>
       <c r="B94" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C94" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="D94">
         <v>8</v>
@@ -4333,10 +4337,10 @@
         <v>25</v>
       </c>
       <c r="B95" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C95" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="D95">
         <v>2</v>
@@ -4367,10 +4371,10 @@
         <v>25</v>
       </c>
       <c r="B96" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C96" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="D96">
         <v>3</v>
@@ -4401,10 +4405,10 @@
         <v>25</v>
       </c>
       <c r="B97" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C97" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="D97">
         <v>4</v>
@@ -4435,10 +4439,10 @@
         <v>25</v>
       </c>
       <c r="B98" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C98" t="s">
-        <v>100</v>
+        <v>146</v>
       </c>
       <c r="D98">
         <v>5</v>
@@ -4469,10 +4473,10 @@
         <v>25</v>
       </c>
       <c r="B99" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C99" t="s">
-        <v>101</v>
+        <v>147</v>
       </c>
       <c r="D99">
         <v>14</v>
@@ -4503,10 +4507,10 @@
         <v>25</v>
       </c>
       <c r="B100" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C100" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D100">
         <v>9</v>
@@ -4537,10 +4541,10 @@
         <v>27</v>
       </c>
       <c r="B101" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="C101" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -4585,7 +4589,7 @@
         <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D102">
         <v>4</v>
@@ -4616,10 +4620,10 @@
         <v>27</v>
       </c>
       <c r="B103" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C103" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="D103">
         <v>10</v>
@@ -4650,10 +4654,10 @@
         <v>27</v>
       </c>
       <c r="B104" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C104" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="D104">
         <v>11</v>
@@ -4684,10 +4688,10 @@
         <v>27</v>
       </c>
       <c r="B105" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C105" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="D105">
         <v>12</v>
@@ -4718,10 +4722,10 @@
         <v>27</v>
       </c>
       <c r="B106" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C106" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="D106">
         <v>13</v>
@@ -4752,10 +4756,10 @@
         <v>27</v>
       </c>
       <c r="B107" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C107" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
       <c r="D107">
         <v>6</v>
@@ -4786,10 +4790,10 @@
         <v>27</v>
       </c>
       <c r="B108" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C108" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="D108">
         <v>7</v>
@@ -4820,10 +4824,10 @@
         <v>27</v>
       </c>
       <c r="B109" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C109" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="D109">
         <v>8</v>
@@ -4854,10 +4858,10 @@
         <v>27</v>
       </c>
       <c r="B110" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C110" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="D110">
         <v>2</v>
@@ -4888,10 +4892,10 @@
         <v>27</v>
       </c>
       <c r="B111" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C111" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="D111">
         <v>3</v>
@@ -4922,10 +4926,10 @@
         <v>27</v>
       </c>
       <c r="B112" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C112" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="D112">
         <v>4</v>
@@ -4956,10 +4960,10 @@
         <v>27</v>
       </c>
       <c r="B113" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C113" t="s">
-        <v>100</v>
+        <v>146</v>
       </c>
       <c r="D113">
         <v>5</v>
@@ -4990,10 +4994,10 @@
         <v>27</v>
       </c>
       <c r="B114" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C114" t="s">
-        <v>101</v>
+        <v>147</v>
       </c>
       <c r="D114">
         <v>14</v>
@@ -5024,10 +5028,10 @@
         <v>27</v>
       </c>
       <c r="B115" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C115" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D115">
         <v>9</v>
@@ -5058,10 +5062,10 @@
         <v>26</v>
       </c>
       <c r="B116" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="C116" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -5106,7 +5110,7 @@
         <v>4</v>
       </c>
       <c r="C117" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D117">
         <v>4</v>
@@ -5137,10 +5141,10 @@
         <v>26</v>
       </c>
       <c r="B118" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C118" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="D118">
         <v>10</v>
@@ -5171,10 +5175,10 @@
         <v>26</v>
       </c>
       <c r="B119" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C119" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="D119">
         <v>11</v>
@@ -5205,10 +5209,10 @@
         <v>26</v>
       </c>
       <c r="B120" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C120" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="D120">
         <v>12</v>
@@ -5239,10 +5243,10 @@
         <v>26</v>
       </c>
       <c r="B121" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C121" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="D121">
         <v>13</v>
@@ -5273,10 +5277,10 @@
         <v>26</v>
       </c>
       <c r="B122" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C122" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
       <c r="D122">
         <v>6</v>
@@ -5307,10 +5311,10 @@
         <v>26</v>
       </c>
       <c r="B123" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C123" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="D123">
         <v>7</v>
@@ -5341,10 +5345,10 @@
         <v>26</v>
       </c>
       <c r="B124" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C124" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="D124">
         <v>8</v>
@@ -5375,10 +5379,10 @@
         <v>26</v>
       </c>
       <c r="B125" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C125" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="D125">
         <v>2</v>
@@ -5409,10 +5413,10 @@
         <v>26</v>
       </c>
       <c r="B126" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C126" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="D126">
         <v>3</v>
@@ -5443,10 +5447,10 @@
         <v>26</v>
       </c>
       <c r="B127" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C127" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="D127">
         <v>4</v>
@@ -5477,10 +5481,10 @@
         <v>26</v>
       </c>
       <c r="B128" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C128" t="s">
-        <v>100</v>
+        <v>146</v>
       </c>
       <c r="D128">
         <v>5</v>
@@ -5511,10 +5515,10 @@
         <v>26</v>
       </c>
       <c r="B129" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C129" t="s">
-        <v>101</v>
+        <v>147</v>
       </c>
       <c r="D129">
         <v>14</v>
@@ -5545,10 +5549,10 @@
         <v>26</v>
       </c>
       <c r="B130" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C130" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D130">
         <v>9</v>
@@ -5579,10 +5583,10 @@
         <v>30</v>
       </c>
       <c r="B131" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="C131" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="D131">
         <v>0</v>
@@ -5627,7 +5631,7 @@
         <v>4</v>
       </c>
       <c r="C132" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D132">
         <v>4</v>
@@ -5661,7 +5665,7 @@
         <v>5</v>
       </c>
       <c r="C133" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="D133">
         <v>9</v>
@@ -5703,10 +5707,10 @@
         <v>30</v>
       </c>
       <c r="B134" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C134" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
       <c r="D134">
         <v>5</v>
@@ -5737,10 +5741,10 @@
         <v>30</v>
       </c>
       <c r="B135" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C135" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="D135">
         <v>2</v>
@@ -5771,10 +5775,10 @@
         <v>30</v>
       </c>
       <c r="B136" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C136" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="D136">
         <v>3</v>
@@ -5805,10 +5809,10 @@
         <v>30</v>
       </c>
       <c r="B137" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C137" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="D137">
         <v>6</v>
@@ -5839,10 +5843,10 @@
         <v>30</v>
       </c>
       <c r="B138" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C138" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="D138">
         <v>7</v>
@@ -5873,10 +5877,10 @@
         <v>30</v>
       </c>
       <c r="B139" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C139" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="D139">
         <v>11</v>
@@ -5907,10 +5911,10 @@
         <v>30</v>
       </c>
       <c r="B140" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C140" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="D140">
         <v>12</v>
@@ -5941,10 +5945,10 @@
         <v>8</v>
       </c>
       <c r="B141" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="C141" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="D141">
         <v>0</v>
@@ -5989,7 +5993,7 @@
         <v>4</v>
       </c>
       <c r="C142" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D142">
         <v>4</v>
@@ -6020,10 +6024,10 @@
         <v>8</v>
       </c>
       <c r="B143" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C143" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="D143">
         <v>9</v>
@@ -6054,10 +6058,10 @@
         <v>8</v>
       </c>
       <c r="B144" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C144" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="D144">
         <v>6</v>
@@ -6088,10 +6092,10 @@
         <v>8</v>
       </c>
       <c r="B145" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C145" t="s">
-        <v>40</v>
+        <v>155</v>
       </c>
       <c r="D145">
         <v>7</v>
@@ -6122,10 +6126,10 @@
         <v>8</v>
       </c>
       <c r="B146" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C146" t="s">
-        <v>114</v>
+        <v>156</v>
       </c>
       <c r="D146">
         <v>11</v>
@@ -6156,10 +6160,10 @@
         <v>8</v>
       </c>
       <c r="B147" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C147" t="s">
-        <v>113</v>
+        <v>157</v>
       </c>
       <c r="D147">
         <v>12</v>
@@ -6190,10 +6194,10 @@
         <v>8</v>
       </c>
       <c r="B148" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C148" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="D148">
         <v>14</v>

</xml_diff>

<commit_message>
eliminated errors in excel key image mapping and changed names of images
</commit_message>
<xml_diff>
--- a/prep/StreamdeckIconInputKeyMapping.xlsx
+++ b/prep/StreamdeckIconInputKeyMapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\biz.dfch.PhoneTap\prep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irene\src\biz.dfch.PhoneTap\prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897AE680-AD8E-46F7-B439-A6B1EAB407D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E113DA4D-6BED-406B-AA37-CB3D3B3C5C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{4419FAFA-D280-4090-97B7-CB07F6B7BE60}"/>
   </bookViews>
@@ -519,7 +519,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -562,10 +562,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -902,21 +901,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47861C0B-96C3-4FC0-B828-7FD785B358D7}">
   <dimension ref="A1:I148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="C143" sqref="C143"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.1875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.125" customWidth="1"/>
-    <col min="6" max="6" width="17.9375" customWidth="1"/>
-    <col min="7" max="7" width="22.5625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.3125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="45.8125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.1328125" customWidth="1"/>
+    <col min="6" max="6" width="17.9296875" customWidth="1"/>
+    <col min="7" max="7" width="22.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="13.9">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -945,7 +946,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -977,7 +978,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G2" s="2" t="str">
+      <c r="G2" t="str">
         <f t="shared" ref="G2" si="1">_xlfn.CONCAT(A2, "-", F2, "-", E2, ".png")</f>
         <v>FinalState-KEY_00-screen.png</v>
       </c>
@@ -990,7 +991,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1022,7 +1023,7 @@
 )</f>
         <v>KEY_04</v>
       </c>
-      <c r="G3" s="2" t="str">
+      <c r="G3" t="str">
         <f t="shared" ref="G3:G33" si="4">_xlfn.CONCAT(A3, "-", F3, "-", E3, ".png")</f>
         <v>FinalState-KEY_04-help.png</v>
       </c>
@@ -1035,7 +1036,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1059,7 +1060,7 @@
 )</f>
         <v>KEY_09</v>
       </c>
-      <c r="G4" s="2" t="str">
+      <c r="G4" t="str">
         <f t="shared" si="4"/>
         <v>FinalState-KEY_09-menu.png</v>
       </c>
@@ -1072,7 +1073,7 @@
         <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1104,7 +1105,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G5" s="2" t="str">
+      <c r="G5" t="str">
         <f t="shared" ref="G5" si="10">_xlfn.CONCAT(A5, "-", F5, "-", E5, ".png")</f>
         <v>InitialiseAudio-KEY_00-screen.png</v>
       </c>
@@ -1117,7 +1118,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1138,7 +1139,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G6" s="2" t="str">
+      <c r="G6" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseAudio-KEY_04-help.png</v>
       </c>
@@ -1151,7 +1152,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1172,7 +1173,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G7" s="2" t="str">
+      <c r="G7" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseAudio-KEY_05-init_audio.png</v>
       </c>
@@ -1185,7 +1186,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1206,7 +1207,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G8" s="2" t="str">
+      <c r="G8" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseAudio-KEY_06-skip_audio.png</v>
       </c>
@@ -1219,7 +1220,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1251,7 +1252,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G9" s="2" t="str">
+      <c r="G9" t="str">
         <f t="shared" ref="G9" si="15">_xlfn.CONCAT(A9, "-", F9, "-", E9, ".png")</f>
         <v>InitialiseEx1-KEY_00-screen.png</v>
       </c>
@@ -1264,7 +1265,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1285,7 +1286,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G10" s="2" t="str">
+      <c r="G10" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseEx1-KEY_04-help.png</v>
       </c>
@@ -1298,7 +1299,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1319,7 +1320,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G11" s="2" t="str">
+      <c r="G11" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseEx1-KEY_05-detect_device.png</v>
       </c>
@@ -1332,7 +1333,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1353,7 +1354,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G12" s="2" t="str">
+      <c r="G12" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseEx1-KEY_06-skip_device.png</v>
       </c>
@@ -1366,7 +1367,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1398,7 +1399,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G13" s="2" t="str">
+      <c r="G13" t="str">
         <f t="shared" ref="G13" si="20">_xlfn.CONCAT(A13, "-", F13, "-", E13, ".png")</f>
         <v>InitialiseEx2-KEY_00-screen.png</v>
       </c>
@@ -1411,7 +1412,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1432,7 +1433,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G14" s="2" t="str">
+      <c r="G14" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseEx2-KEY_04-help.png</v>
       </c>
@@ -1445,7 +1446,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1466,7 +1467,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G15" s="2" t="str">
+      <c r="G15" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseEx2-KEY_05-detect_device.png</v>
       </c>
@@ -1479,7 +1480,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1500,7 +1501,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G16" s="2" t="str">
+      <c r="G16" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseEx2-KEY_06-skip_device.png</v>
       </c>
@@ -1513,7 +1514,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1545,7 +1546,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G17" s="2" t="str">
+      <c r="G17" t="str">
         <f t="shared" ref="G17" si="25">_xlfn.CONCAT(A17, "-", F17, "-", E17, ".png")</f>
         <v>InitialiseHi1-KEY_00-screen.png</v>
       </c>
@@ -1558,7 +1559,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1579,7 +1580,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G18" s="2" t="str">
+      <c r="G18" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi1-KEY_04-help.png</v>
       </c>
@@ -1592,7 +1593,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1613,7 +1614,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G19" s="2" t="str">
+      <c r="G19" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi1-KEY_05-detect_device.png</v>
       </c>
@@ -1626,7 +1627,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1647,7 +1648,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G20" s="2" t="str">
+      <c r="G20" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi1-KEY_06-skip_device.png</v>
       </c>
@@ -1660,7 +1661,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1692,7 +1693,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G21" s="2" t="str">
+      <c r="G21" t="str">
         <f t="shared" ref="G21" si="30">_xlfn.CONCAT(A21, "-", F21, "-", E21, ".png")</f>
         <v>InitialiseHi2-KEY_00-screen.png</v>
       </c>
@@ -1705,7 +1706,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1726,7 +1727,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G22" s="2" t="str">
+      <c r="G22" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi2-KEY_04-help.png</v>
       </c>
@@ -1739,7 +1740,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1760,7 +1761,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G23" s="2" t="str">
+      <c r="G23" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi2-KEY_05-detect_device.png</v>
       </c>
@@ -1773,7 +1774,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1794,7 +1795,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G24" s="2" t="str">
+      <c r="G24" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi2-KEY_06-skip_device.png</v>
       </c>
@@ -1807,7 +1808,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1839,7 +1840,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G25" s="2" t="str">
+      <c r="G25" t="str">
         <f t="shared" ref="G25" si="35">_xlfn.CONCAT(A25, "-", F25, "-", E25, ".png")</f>
         <v>InitialiseHi3-KEY_00-screen.png</v>
       </c>
@@ -1852,7 +1853,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -1873,7 +1874,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G26" s="2" t="str">
+      <c r="G26" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi3-KEY_04-help.png</v>
       </c>
@@ -1886,7 +1887,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1907,7 +1908,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G27" s="2" t="str">
+      <c r="G27" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi3-KEY_05-detect_device.png</v>
       </c>
@@ -1920,7 +1921,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -1941,7 +1942,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G28" s="2" t="str">
+      <c r="G28" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseHi3-KEY_06-skip_device.png</v>
       </c>
@@ -1954,7 +1955,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1986,7 +1987,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G29" s="2" t="str">
+      <c r="G29" t="str">
         <f t="shared" ref="G29" si="40">_xlfn.CONCAT(A29, "-", F29, "-", E29, ".png")</f>
         <v>InitialiseLcl-KEY_00-screen.png</v>
       </c>
@@ -1999,7 +2000,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -2020,7 +2021,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G30" s="2" t="str">
+      <c r="G30" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseLcl-KEY_04-help.png</v>
       </c>
@@ -2033,7 +2034,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -2054,7 +2055,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G31" s="2" t="str">
+      <c r="G31" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseLcl-KEY_05-detect_device.png</v>
       </c>
@@ -2067,7 +2068,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -2088,7 +2089,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G32" s="2" t="str">
+      <c r="G32" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseLcl-KEY_06-skip_device.png</v>
       </c>
@@ -2101,7 +2102,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -2125,7 +2126,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G33" s="2" t="str">
+      <c r="G33" t="str">
         <f t="shared" si="4"/>
         <v>InitialiseRc1-KEY_00-screen.png</v>
       </c>
@@ -2138,7 +2139,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -2167,7 +2168,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G34" s="2" t="str">
+      <c r="G34" t="str">
         <f t="shared" ref="G34:G42" si="45">_xlfn.CONCAT(A34, "-", F34, "-", E34, ".png")</f>
         <v>InitialiseRc1-KEY_04-help.png</v>
       </c>
@@ -2180,7 +2181,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -2201,7 +2202,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G35" s="2" t="str">
+      <c r="G35" t="str">
         <f t="shared" si="45"/>
         <v>InitialiseRc1-KEY_05-detect_device.png</v>
       </c>
@@ -2214,7 +2215,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -2235,7 +2236,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G36" s="2" t="str">
+      <c r="G36" t="str">
         <f t="shared" si="45"/>
         <v>InitialiseRc1-KEY_06-skip_device.png</v>
       </c>
@@ -2248,7 +2249,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -2269,7 +2270,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0A</v>
       </c>
-      <c r="G37" s="2" t="str">
+      <c r="G37" t="str">
         <f t="shared" si="45"/>
         <v>InitialiseRc1-KEY_0A-format_device.png</v>
       </c>
@@ -2282,7 +2283,7 @@
         <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_6,</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -2303,7 +2304,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0B</v>
       </c>
-      <c r="G38" s="2" t="str">
+      <c r="G38" t="str">
         <f t="shared" si="45"/>
         <v>InitialiseRc1-KEY_0B-mount_device.png</v>
       </c>
@@ -2316,7 +2317,7 @@
         <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_7,</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -2337,7 +2338,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0C</v>
       </c>
-      <c r="G39" s="2" t="str">
+      <c r="G39" t="str">
         <f t="shared" si="45"/>
         <v>InitialiseRc1-KEY_0C-unmount_device.png</v>
       </c>
@@ -2350,7 +2351,7 @@
         <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_8,</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -2371,7 +2372,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0D</v>
       </c>
-      <c r="G40" s="2" t="str">
+      <c r="G40" t="str">
         <f t="shared" si="45"/>
         <v>InitialiseRc1-KEY_0D-clean_device.png</v>
       </c>
@@ -2384,7 +2385,7 @@
         <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_9,</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -2416,7 +2417,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G41" s="2" t="str">
+      <c r="G41" t="str">
         <f t="shared" ref="G41" si="50">_xlfn.CONCAT(A41, "-", F41, "-", E41, ".png")</f>
         <v>InitialiseRc2-KEY_00-screen.png</v>
       </c>
@@ -2429,7 +2430,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -2450,7 +2451,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G42" s="2" t="str">
+      <c r="G42" t="str">
         <f t="shared" si="45"/>
         <v>InitialiseRc2-KEY_04-help.png</v>
       </c>
@@ -2463,7 +2464,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -2492,7 +2493,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G43" s="2" t="str">
+      <c r="G43" t="str">
         <f t="shared" ref="G43:G50" si="54">_xlfn.CONCAT(A43, "-", F43, "-", E43, ".png")</f>
         <v>InitialiseRc2-KEY_05-detect_device.png</v>
       </c>
@@ -2505,7 +2506,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -2526,7 +2527,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G44" s="2" t="str">
+      <c r="G44" t="str">
         <f t="shared" si="54"/>
         <v>InitialiseRc2-KEY_06-skip_device.png</v>
       </c>
@@ -2539,7 +2540,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -2560,7 +2561,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0A</v>
       </c>
-      <c r="G45" s="2" t="str">
+      <c r="G45" t="str">
         <f t="shared" si="54"/>
         <v>InitialiseRc2-KEY_0A-format_device.png</v>
       </c>
@@ -2573,7 +2574,7 @@
         <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_6,</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -2594,7 +2595,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0B</v>
       </c>
-      <c r="G46" s="2" t="str">
+      <c r="G46" t="str">
         <f t="shared" si="54"/>
         <v>InitialiseRc2-KEY_0B-mount_device.png</v>
       </c>
@@ -2607,7 +2608,7 @@
         <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_7,</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -2628,7 +2629,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0C</v>
       </c>
-      <c r="G47" s="2" t="str">
+      <c r="G47" t="str">
         <f t="shared" si="54"/>
         <v>InitialiseRc2-KEY_0C-unmount_device.png</v>
       </c>
@@ -2641,7 +2642,7 @@
         <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_8,</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -2662,7 +2663,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0D</v>
       </c>
-      <c r="G48" s="2" t="str">
+      <c r="G48" t="str">
         <f t="shared" si="54"/>
         <v>InitialiseRc2-KEY_0D-clean_device.png</v>
       </c>
@@ -2675,7 +2676,7 @@
         <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_9,</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -2707,7 +2708,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G49" s="2" t="str">
+      <c r="G49" t="str">
         <f t="shared" ref="G49" si="59">_xlfn.CONCAT(A49, "-", F49, "-", E49, ".png")</f>
         <v>Main-KEY_00-screen.png</v>
       </c>
@@ -2720,7 +2721,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -2741,7 +2742,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G50" s="2" t="str">
+      <c r="G50" t="str">
         <f t="shared" si="54"/>
         <v>Main-KEY_04-help.png</v>
       </c>
@@ -2754,7 +2755,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -2783,7 +2784,7 @@
         <f t="shared" si="6"/>
         <v>KEY_05</v>
       </c>
-      <c r="G51" s="2" t="str">
+      <c r="G51" t="str">
         <f t="shared" ref="G51:G56" si="63">_xlfn.CONCAT(A51, "-", F51, "-", E51, ".png")</f>
         <v>Main-KEY_05-start_recording_mx0.png</v>
       </c>
@@ -2796,7 +2797,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -2817,7 +2818,7 @@
         <f t="shared" si="6"/>
         <v>KEY_06</v>
       </c>
-      <c r="G52" s="2" t="str">
+      <c r="G52" t="str">
         <f t="shared" si="63"/>
         <v>Main-KEY_06-start_recording_mx1.png</v>
       </c>
@@ -2830,7 +2831,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -2851,7 +2852,7 @@
         <f t="shared" si="6"/>
         <v>KEY_07</v>
       </c>
-      <c r="G53" s="2" t="str">
+      <c r="G53" t="str">
         <f t="shared" si="63"/>
         <v>Main-KEY_07-start_recording_mx2.png</v>
       </c>
@@ -2864,7 +2865,7 @@
         <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -2885,7 +2886,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0A</v>
       </c>
-      <c r="G54" s="2" t="str">
+      <c r="G54" t="str">
         <f t="shared" si="63"/>
         <v>Main-KEY_0A-start_playback.png</v>
       </c>
@@ -2898,7 +2899,7 @@
         <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_4,</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -2919,7 +2920,7 @@
         <f t="shared" si="6"/>
         <v>KEY_09</v>
       </c>
-      <c r="G55" s="2" t="str">
+      <c r="G55" t="str">
         <f t="shared" si="63"/>
         <v>Main-KEY_09-menu.png</v>
       </c>
@@ -2932,7 +2933,7 @@
         <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -2953,7 +2954,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0B</v>
       </c>
-      <c r="G56" s="2" t="str">
+      <c r="G56" t="str">
         <f t="shared" si="63"/>
         <v>Main-KEY_0B-set_name.png</v>
       </c>
@@ -2966,7 +2967,7 @@
         <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_6,</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -2987,7 +2988,7 @@
         <f t="shared" si="6"/>
         <v>KEY_0E</v>
       </c>
-      <c r="G57" s="2" t="str">
+      <c r="G57" t="str">
         <f t="shared" ref="G57:G59" si="66">_xlfn.CONCAT(A57, "-", F57, "-", E57, ".png")</f>
         <v>Main-KEY_0E-stop_system.png</v>
       </c>
@@ -3000,7 +3001,7 @@
         <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_9,</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -3032,7 +3033,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G58" s="2" t="str">
+      <c r="G58" t="str">
         <f t="shared" ref="G58" si="71">_xlfn.CONCAT(A58, "-", F58, "-", E58, ".png")</f>
         <v>OnRecord-KEY_00-screen.png</v>
       </c>
@@ -3045,7 +3046,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -3066,7 +3067,7 @@
         <f t="shared" si="6"/>
         <v>KEY_04</v>
       </c>
-      <c r="G59" s="2" t="str">
+      <c r="G59" t="str">
         <f t="shared" si="66"/>
         <v>OnRecord-KEY_04-help.png</v>
       </c>
@@ -3079,7 +3080,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>18</v>
       </c>
@@ -3111,7 +3112,7 @@
 )</f>
         <v>KEY_06</v>
       </c>
-      <c r="G60" s="2" t="str">
+      <c r="G60" t="str">
         <f t="shared" ref="G60:G64" si="76">_xlfn.CONCAT(A60, "-", F60, "-", E60, ".png")</f>
         <v>OnRecord-KEY_06-stop_recording.png</v>
       </c>
@@ -3124,7 +3125,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -3145,7 +3146,7 @@
         <f t="shared" si="75"/>
         <v>KEY_05</v>
       </c>
-      <c r="G61" s="2" t="str">
+      <c r="G61" t="str">
         <f t="shared" si="76"/>
         <v>OnRecord-KEY_05-set_cue.png</v>
       </c>
@@ -3158,7 +3159,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>18</v>
       </c>
@@ -3179,7 +3180,7 @@
         <f t="shared" si="75"/>
         <v>KEY_07</v>
       </c>
-      <c r="G62" s="2" t="str">
+      <c r="G62" t="str">
         <f t="shared" si="76"/>
         <v>OnRecord-KEY_07-toggle_mute.png</v>
       </c>
@@ -3192,7 +3193,7 @@
         <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>18</v>
       </c>
@@ -3213,7 +3214,7 @@
         <f t="shared" si="75"/>
         <v>KEY_0A</v>
       </c>
-      <c r="G63" s="2" t="str">
+      <c r="G63" t="str">
         <f t="shared" si="76"/>
         <v>OnRecord-KEY_0A-show_status.png</v>
       </c>
@@ -3226,7 +3227,7 @@
         <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_4,</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>29</v>
       </c>
@@ -3247,7 +3248,7 @@
         <f t="shared" si="75"/>
         <v>KEY_00</v>
       </c>
-      <c r="G64" s="2" t="str">
+      <c r="G64" t="str">
         <f t="shared" si="76"/>
         <v>PlaybackPaused-KEY_00-screen.png</v>
       </c>
@@ -3260,7 +3261,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>29</v>
       </c>
@@ -3292,7 +3293,7 @@
 )</f>
         <v>KEY_04</v>
       </c>
-      <c r="G65" s="2" t="str">
+      <c r="G65" t="str">
         <f t="shared" ref="G65:G132" si="81">_xlfn.CONCAT(A65, "-", F65, "-", E65, ".png")</f>
         <v>PlaybackPaused-KEY_04-help.png</v>
       </c>
@@ -3305,7 +3306,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>29</v>
       </c>
@@ -3326,7 +3327,7 @@
         <f t="shared" si="80"/>
         <v>KEY_05</v>
       </c>
-      <c r="G66" s="2" t="str">
+      <c r="G66" t="str">
         <f t="shared" si="81"/>
         <v>PlaybackPaused-KEY_05-pause_resume.png</v>
       </c>
@@ -3339,7 +3340,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_0,</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>29</v>
       </c>
@@ -3360,7 +3361,7 @@
         <f t="shared" si="80"/>
         <v>KEY_09</v>
       </c>
-      <c r="G67" s="2" t="str">
+      <c r="G67" t="str">
         <f t="shared" si="81"/>
         <v>PlaybackPaused-KEY_09-menu.png</v>
       </c>
@@ -3373,7 +3374,7 @@
         <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>28</v>
       </c>
@@ -3405,7 +3406,7 @@
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G68" s="2" t="str">
+      <c r="G68" t="str">
         <f t="shared" ref="G68" si="86">_xlfn.CONCAT(A68, "-", F68, "-", E68, ".png")</f>
         <v>Playback-KEY_00-screen.png</v>
       </c>
@@ -3418,7 +3419,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>28</v>
       </c>
@@ -3439,7 +3440,7 @@
         <f t="shared" si="80"/>
         <v>KEY_04</v>
       </c>
-      <c r="G69" s="2" t="str">
+      <c r="G69" t="str">
         <f t="shared" si="81"/>
         <v>Playback-KEY_04-help.png</v>
       </c>
@@ -3452,7 +3453,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>28</v>
       </c>
@@ -3473,7 +3474,7 @@
         <f t="shared" si="80"/>
         <v>KEY_07</v>
       </c>
-      <c r="G70" s="2" t="str">
+      <c r="G70" t="str">
         <f t="shared" si="81"/>
         <v>Playback-KEY_07-pause_resume.png</v>
       </c>
@@ -3486,7 +3487,7 @@
         <v>StreamdeckInput.KEY_07: InputEventMap.KEY_0,</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -3507,7 +3508,7 @@
         <f t="shared" si="80"/>
         <v>KEY_0B</v>
       </c>
-      <c r="G71" s="2" t="str">
+      <c r="G71" t="str">
         <f t="shared" si="81"/>
         <v>Playback-KEY_0B-jump_clip_end.png</v>
       </c>
@@ -3520,7 +3521,7 @@
         <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>28</v>
       </c>
@@ -3541,7 +3542,7 @@
         <f t="shared" si="80"/>
         <v>KEY_0C</v>
       </c>
-      <c r="G72" s="2" t="str">
+      <c r="G72" t="str">
         <f t="shared" si="81"/>
         <v>Playback-KEY_0C-seek_next.png</v>
       </c>
@@ -3554,7 +3555,7 @@
         <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>28</v>
       </c>
@@ -3575,7 +3576,7 @@
         <f t="shared" si="80"/>
         <v>KEY_0D</v>
       </c>
-      <c r="G73" s="2" t="str">
+      <c r="G73" t="str">
         <f t="shared" si="81"/>
         <v>Playback-KEY_0D-jump_cue_next.png</v>
       </c>
@@ -3588,7 +3589,7 @@
         <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>28</v>
       </c>
@@ -3622,7 +3623,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>28</v>
       </c>
@@ -3656,7 +3657,7 @@
         <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>28</v>
       </c>
@@ -3690,7 +3691,7 @@
         <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>28</v>
       </c>
@@ -3724,7 +3725,7 @@
         <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>28</v>
       </c>
@@ -3758,7 +3759,7 @@
         <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>28</v>
       </c>
@@ -3792,7 +3793,7 @@
         <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>24</v>
       </c>
@@ -3837,7 +3838,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>24</v>
       </c>
@@ -3871,7 +3872,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>24</v>
       </c>
@@ -3905,7 +3906,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>24</v>
       </c>
@@ -3939,7 +3940,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>24</v>
       </c>
@@ -3973,7 +3974,7 @@
         <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>24</v>
       </c>
@@ -4007,7 +4008,7 @@
         <v>StreamdeckInput.KEY_08: InputEventMap.KEY_4,</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>25</v>
       </c>
@@ -4052,7 +4053,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>25</v>
       </c>
@@ -4086,7 +4087,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>25</v>
       </c>
@@ -4120,7 +4121,7 @@
         <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>25</v>
       </c>
@@ -4154,7 +4155,7 @@
         <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>25</v>
       </c>
@@ -4188,7 +4189,7 @@
         <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>25</v>
       </c>
@@ -4222,7 +4223,7 @@
         <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>25</v>
       </c>
@@ -4256,7 +4257,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>25</v>
       </c>
@@ -4290,7 +4291,7 @@
         <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>25</v>
       </c>
@@ -4324,7 +4325,7 @@
         <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>25</v>
       </c>
@@ -4335,7 +4336,7 @@
         <v>143</v>
       </c>
       <c r="D95">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E95" t="str">
         <f t="shared" si="79"/>
@@ -4343,11 +4344,11 @@
       </c>
       <c r="F95" t="str">
         <f t="shared" si="80"/>
-        <v>KEY_02</v>
+        <v>KEY_01</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="81"/>
-        <v>SetDate-KEY_02-digit_7.png</v>
+        <v>SetDate-KEY_01-digit_7.png</v>
       </c>
       <c r="H95" t="str">
         <f t="shared" si="82"/>
@@ -4355,10 +4356,10 @@
       </c>
       <c r="I95" t="str">
         <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_7,</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9">
+        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>25</v>
       </c>
@@ -4369,7 +4370,7 @@
         <v>144</v>
       </c>
       <c r="D96">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E96" t="str">
         <f t="shared" si="79"/>
@@ -4377,11 +4378,11 @@
       </c>
       <c r="F96" t="str">
         <f t="shared" si="80"/>
-        <v>KEY_03</v>
+        <v>KEY_02</v>
       </c>
       <c r="G96" t="str">
         <f t="shared" si="81"/>
-        <v>SetDate-KEY_03-digit_8.png</v>
+        <v>SetDate-KEY_02-digit_8.png</v>
       </c>
       <c r="H96" t="str">
         <f t="shared" si="82"/>
@@ -4389,10 +4390,10 @@
       </c>
       <c r="I96" t="str">
         <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_8,</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9">
+        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>25</v>
       </c>
@@ -4403,7 +4404,7 @@
         <v>145</v>
       </c>
       <c r="D97">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E97" t="str">
         <f t="shared" si="79"/>
@@ -4411,11 +4412,11 @@
       </c>
       <c r="F97" t="str">
         <f t="shared" si="80"/>
-        <v>KEY_04</v>
+        <v>KEY_03</v>
       </c>
       <c r="G97" t="str">
         <f t="shared" si="81"/>
-        <v>SetDate-KEY_04-digit_9.png</v>
+        <v>SetDate-KEY_03-digit_9.png</v>
       </c>
       <c r="H97" t="str">
         <f t="shared" si="82"/>
@@ -4423,10 +4424,10 @@
       </c>
       <c r="I97" t="str">
         <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_9,</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9">
+        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>25</v>
       </c>
@@ -4460,7 +4461,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>25</v>
       </c>
@@ -4494,7 +4495,7 @@
         <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>25</v>
       </c>
@@ -4528,7 +4529,7 @@
         <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>27</v>
       </c>
@@ -4573,7 +4574,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>27</v>
       </c>
@@ -4607,7 +4608,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>27</v>
       </c>
@@ -4641,7 +4642,7 @@
         <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>27</v>
       </c>
@@ -4675,7 +4676,7 @@
         <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>27</v>
       </c>
@@ -4709,7 +4710,7 @@
         <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>27</v>
       </c>
@@ -4743,7 +4744,7 @@
         <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>27</v>
       </c>
@@ -4777,7 +4778,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>27</v>
       </c>
@@ -4811,7 +4812,7 @@
         <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>27</v>
       </c>
@@ -4845,7 +4846,7 @@
         <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>27</v>
       </c>
@@ -4856,7 +4857,7 @@
         <v>143</v>
       </c>
       <c r="D110">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E110" t="str">
         <f t="shared" si="79"/>
@@ -4864,11 +4865,11 @@
       </c>
       <c r="F110" t="str">
         <f t="shared" si="80"/>
-        <v>KEY_02</v>
+        <v>KEY_01</v>
       </c>
       <c r="G110" t="str">
         <f t="shared" si="81"/>
-        <v>SetName-KEY_02-digit_7.png</v>
+        <v>SetName-KEY_01-digit_7.png</v>
       </c>
       <c r="H110" t="str">
         <f t="shared" si="82"/>
@@ -4876,10 +4877,10 @@
       </c>
       <c r="I110" t="str">
         <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_7,</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9">
+        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>27</v>
       </c>
@@ -4890,7 +4891,7 @@
         <v>144</v>
       </c>
       <c r="D111">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E111" t="str">
         <f t="shared" si="79"/>
@@ -4898,11 +4899,11 @@
       </c>
       <c r="F111" t="str">
         <f t="shared" si="80"/>
-        <v>KEY_03</v>
+        <v>KEY_02</v>
       </c>
       <c r="G111" t="str">
         <f t="shared" si="81"/>
-        <v>SetName-KEY_03-digit_8.png</v>
+        <v>SetName-KEY_02-digit_8.png</v>
       </c>
       <c r="H111" t="str">
         <f t="shared" si="82"/>
@@ -4910,10 +4911,10 @@
       </c>
       <c r="I111" t="str">
         <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_8,</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9">
+        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>27</v>
       </c>
@@ -4924,7 +4925,7 @@
         <v>145</v>
       </c>
       <c r="D112">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E112" t="str">
         <f t="shared" si="79"/>
@@ -4932,11 +4933,11 @@
       </c>
       <c r="F112" t="str">
         <f t="shared" si="80"/>
-        <v>KEY_04</v>
+        <v>KEY_03</v>
       </c>
       <c r="G112" t="str">
         <f t="shared" si="81"/>
-        <v>SetName-KEY_04-digit_9.png</v>
+        <v>SetName-KEY_03-digit_9.png</v>
       </c>
       <c r="H112" t="str">
         <f t="shared" si="82"/>
@@ -4944,10 +4945,10 @@
       </c>
       <c r="I112" t="str">
         <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_9,</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9">
+        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>27</v>
       </c>
@@ -4981,7 +4982,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>27</v>
       </c>
@@ -5015,7 +5016,7 @@
         <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>27</v>
       </c>
@@ -5049,7 +5050,7 @@
         <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>26</v>
       </c>
@@ -5094,7 +5095,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>26</v>
       </c>
@@ -5128,7 +5129,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>26</v>
       </c>
@@ -5162,7 +5163,7 @@
         <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>26</v>
       </c>
@@ -5196,7 +5197,7 @@
         <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>26</v>
       </c>
@@ -5230,7 +5231,7 @@
         <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>26</v>
       </c>
@@ -5264,7 +5265,7 @@
         <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>26</v>
       </c>
@@ -5298,7 +5299,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>26</v>
       </c>
@@ -5332,7 +5333,7 @@
         <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>26</v>
       </c>
@@ -5366,7 +5367,7 @@
         <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
       </c>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>26</v>
       </c>
@@ -5377,7 +5378,7 @@
         <v>143</v>
       </c>
       <c r="D125">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E125" t="str">
         <f t="shared" si="79"/>
@@ -5385,11 +5386,11 @@
       </c>
       <c r="F125" t="str">
         <f t="shared" si="80"/>
-        <v>KEY_02</v>
+        <v>KEY_01</v>
       </c>
       <c r="G125" t="str">
         <f t="shared" si="81"/>
-        <v>SetTime-KEY_02-digit_7.png</v>
+        <v>SetTime-KEY_01-digit_7.png</v>
       </c>
       <c r="H125" t="str">
         <f t="shared" si="82"/>
@@ -5397,10 +5398,10 @@
       </c>
       <c r="I125" t="str">
         <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_7,</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9">
+        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>26</v>
       </c>
@@ -5411,7 +5412,7 @@
         <v>144</v>
       </c>
       <c r="D126">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E126" t="str">
         <f t="shared" si="79"/>
@@ -5419,11 +5420,11 @@
       </c>
       <c r="F126" t="str">
         <f t="shared" si="80"/>
-        <v>KEY_03</v>
+        <v>KEY_02</v>
       </c>
       <c r="G126" t="str">
         <f t="shared" si="81"/>
-        <v>SetTime-KEY_03-digit_8.png</v>
+        <v>SetTime-KEY_02-digit_8.png</v>
       </c>
       <c r="H126" t="str">
         <f t="shared" si="82"/>
@@ -5431,10 +5432,10 @@
       </c>
       <c r="I126" t="str">
         <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_8,</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9">
+        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>26</v>
       </c>
@@ -5445,7 +5446,7 @@
         <v>145</v>
       </c>
       <c r="D127">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E127" t="str">
         <f t="shared" si="79"/>
@@ -5453,11 +5454,11 @@
       </c>
       <c r="F127" t="str">
         <f t="shared" si="80"/>
-        <v>KEY_04</v>
+        <v>KEY_03</v>
       </c>
       <c r="G127" t="str">
         <f t="shared" si="81"/>
-        <v>SetTime-KEY_04-digit_9.png</v>
+        <v>SetTime-KEY_03-digit_9.png</v>
       </c>
       <c r="H127" t="str">
         <f t="shared" si="82"/>
@@ -5465,10 +5466,10 @@
       </c>
       <c r="I127" t="str">
         <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_9,</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9">
+        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>26</v>
       </c>
@@ -5502,7 +5503,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>26</v>
       </c>
@@ -5536,7 +5537,7 @@
         <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>26</v>
       </c>
@@ -5570,7 +5571,7 @@
         <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>30</v>
       </c>
@@ -5615,7 +5616,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>30</v>
       </c>
@@ -5649,7 +5650,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>30</v>
       </c>
@@ -5694,7 +5695,7 @@
         <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>30</v>
       </c>
@@ -5728,7 +5729,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_0,</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>30</v>
       </c>
@@ -5739,7 +5740,7 @@
         <v>93</v>
       </c>
       <c r="D135">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E135" t="str">
         <f t="shared" si="114"/>
@@ -5747,11 +5748,11 @@
       </c>
       <c r="F135" t="str">
         <f t="shared" si="115"/>
-        <v>KEY_02</v>
+        <v>KEY_01</v>
       </c>
       <c r="G135" t="str">
         <f t="shared" si="116"/>
-        <v>StorageManagement-KEY_02-detect_rc1.png</v>
+        <v>StorageManagement-KEY_01-detect_rc1.png</v>
       </c>
       <c r="H135" t="str">
         <f t="shared" si="117"/>
@@ -5759,10 +5760,10 @@
       </c>
       <c r="I135" t="str">
         <f t="shared" si="118"/>
-        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_1,</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9">
+        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_1,</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>30</v>
       </c>
@@ -5773,7 +5774,7 @@
         <v>93</v>
       </c>
       <c r="D136">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E136" t="str">
         <f t="shared" si="114"/>
@@ -5781,11 +5782,11 @@
       </c>
       <c r="F136" t="str">
         <f t="shared" si="115"/>
-        <v>KEY_03</v>
+        <v>KEY_02</v>
       </c>
       <c r="G136" t="str">
         <f t="shared" si="116"/>
-        <v>StorageManagement-KEY_03-detect_rc2.png</v>
+        <v>StorageManagement-KEY_02-detect_rc2.png</v>
       </c>
       <c r="H136" t="str">
         <f t="shared" si="117"/>
@@ -5793,10 +5794,10 @@
       </c>
       <c r="I136" t="str">
         <f t="shared" si="118"/>
-        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_3,</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9">
+        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_3,</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>30</v>
       </c>
@@ -5830,7 +5831,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>30</v>
       </c>
@@ -5864,7 +5865,7 @@
         <v>StreamdeckInput.KEY_07: InputEventMap.KEY_6,</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>30</v>
       </c>
@@ -5898,7 +5899,7 @@
         <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_7,</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>30</v>
       </c>
@@ -5932,7 +5933,7 @@
         <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_9,</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>8</v>
       </c>
@@ -5977,7 +5978,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>8</v>
       </c>
@@ -6011,7 +6012,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>8</v>
       </c>
@@ -6045,7 +6046,7 @@
         <v>StreamdeckInput.KEY_09: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>8</v>
       </c>
@@ -6079,7 +6080,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>8</v>
       </c>
@@ -6113,7 +6114,7 @@
         <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
       </c>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>8</v>
       </c>
@@ -6147,7 +6148,7 @@
         <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_4,</v>
       </c>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>8</v>
       </c>
@@ -6181,7 +6182,7 @@
         <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_6,</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
added missing key to main
</commit_message>
<xml_diff>
--- a/prep/StreamdeckIconInputKeyMapping.xlsx
+++ b/prep/StreamdeckIconInputKeyMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irene\src\biz.dfch.PhoneTap\prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE48585-AEB5-4DB4-A832-B70B6930994C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325AE261-9970-4833-9C9B-69C5B4FDEBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{4419FAFA-D280-4090-97B7-CB07F6B7BE60}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$148</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$149</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="159">
   <si>
     <t>States</t>
   </si>
@@ -513,6 +513,9 @@
   </si>
   <si>
     <t>ic_fluent_time_picker_24_regular.png</t>
+  </si>
+  <si>
+    <t>        DELETE_LAST_TAKE = InputEventMap.KEY_7</t>
   </si>
 </sst>
 </file>
@@ -899,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47861C0B-96C3-4FC0-B828-7FD785B358D7}">
-  <dimension ref="A1:I148"/>
+  <dimension ref="A1:I149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="C38" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1054,7 +1057,7 @@
         <v>menu</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F59" si="6">"KEY_" &amp; CHOOSE(
+        <f t="shared" ref="F4:F60" si="6">"KEY_" &amp; CHOOSE(
     D4+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
@@ -2769,7 +2772,7 @@
         <v>5</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" ref="E51:E59" si="62">LOWER(
+        <f t="shared" ref="E51:E60" si="62">LOWER(
   TRIM(
     SUBSTITUTE(
       LEFT(B51, FIND(" = InputEventMap", B51) - 1),
@@ -2785,15 +2788,15 @@
         <v>KEY_05</v>
       </c>
       <c r="G51" t="str">
-        <f t="shared" ref="G51:G56" si="63">_xlfn.CONCAT(A51, "-", F51, "-", E51, ".png")</f>
+        <f t="shared" ref="G51:G57" si="63">_xlfn.CONCAT(A51, "-", F51, "-", E51, ".png")</f>
         <v>Main-KEY_05-start_recording_mx0.png</v>
       </c>
       <c r="H51" t="str">
-        <f t="shared" ref="H51:H56" si="64">MID(B51, FIND("InputEventMap", B51), LEN(B51))</f>
+        <f t="shared" ref="H51:H57" si="64">MID(B51, FIND("InputEventMap", B51), LEN(B51))</f>
         <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I51" t="str">
-        <f t="shared" ref="I51:I56" si="65">_xlfn.CONCAT("StreamdeckInput.", F51, ": ", H51, ",")</f>
+        <f t="shared" ref="I51:I57" si="65">_xlfn.CONCAT("StreamdeckInput.", F51, ": ", H51, ",")</f>
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
@@ -2972,53 +2975,98 @@
         <v>7</v>
       </c>
       <c r="B57" t="s">
+        <v>158</v>
+      </c>
+      <c r="C57" t="s">
+        <v>97</v>
+      </c>
+      <c r="D57">
+        <v>12</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" ref="E57" si="66">LOWER(
+  TRIM(
+    SUBSTITUTE(
+      LEFT(B57, FIND(" = InputEventMap", B57) - 1),
+      CHAR(160),
+      " "
+    )
+  )
+)</f>
+        <v>delete_last_take</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" ref="F57" si="67">"KEY_" &amp; CHOOSE(
+    D57+1,
+    "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
+)</f>
+        <v>KEY_0C</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="63"/>
+        <v>Main-KEY_0C-delete_last_take.png</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="64"/>
+        <v>InputEventMap.KEY_7</v>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="65"/>
+        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_7,</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" t="s">
         <v>45</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>104</v>
       </c>
-      <c r="D57">
+      <c r="D58">
         <v>14</v>
       </c>
-      <c r="E57" t="str">
+      <c r="E58" t="str">
         <f t="shared" si="62"/>
         <v>stop_system</v>
       </c>
-      <c r="F57" t="str">
+      <c r="F58" t="str">
         <f t="shared" si="6"/>
         <v>KEY_0E</v>
       </c>
-      <c r="G57" t="str">
-        <f t="shared" ref="G57:G59" si="66">_xlfn.CONCAT(A57, "-", F57, "-", E57, ".png")</f>
+      <c r="G58" t="str">
+        <f t="shared" ref="G58:G60" si="68">_xlfn.CONCAT(A58, "-", F58, "-", E58, ".png")</f>
         <v>Main-KEY_0E-stop_system.png</v>
       </c>
-      <c r="H57" t="str">
-        <f t="shared" ref="H57:H59" si="67">MID(B57, FIND("InputEventMap", B57), LEN(B57))</f>
+      <c r="H58" t="str">
+        <f t="shared" ref="H58:H60" si="69">MID(B58, FIND("InputEventMap", B58), LEN(B58))</f>
         <v>InputEventMap.KEY_9</v>
       </c>
-      <c r="I57" t="str">
-        <f t="shared" ref="I57:I59" si="68">_xlfn.CONCAT("StreamdeckInput.", F57, ": ", H57, ",")</f>
+      <c r="I58" t="str">
+        <f t="shared" ref="I58:I60" si="70">_xlfn.CONCAT("StreamdeckInput.", F58, ": ", H58, ",")</f>
         <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_9,</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
         <v>18</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>100</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>115</v>
       </c>
-      <c r="D58">
+      <c r="D59">
         <v>0</v>
       </c>
-      <c r="E58" t="str">
-        <f t="shared" ref="E58" si="69">LOWER(
+      <c r="E59" t="str">
+        <f t="shared" ref="E59" si="71">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B58, FIND(" = InputEventMap", B58) - 1),
+      LEFT(B59, FIND(" = InputEventMap", B59) - 1),
       CHAR(160),
       " "
     )
@@ -3026,58 +3074,24 @@
 )</f>
         <v>screen</v>
       </c>
-      <c r="F58" t="str">
-        <f t="shared" ref="F58" si="70">"KEY_" &amp; CHOOSE(
-    D58+1,
+      <c r="F59" t="str">
+        <f t="shared" ref="F59" si="72">"KEY_" &amp; CHOOSE(
+    D59+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G58" t="str">
-        <f t="shared" ref="G58" si="71">_xlfn.CONCAT(A58, "-", F58, "-", E58, ".png")</f>
+      <c r="G59" t="str">
+        <f t="shared" ref="G59" si="73">_xlfn.CONCAT(A59, "-", F59, "-", E59, ".png")</f>
         <v>OnRecord-KEY_00-screen.png</v>
       </c>
-      <c r="H58" t="str">
-        <f t="shared" ref="H58" si="72">MID(B58, FIND("InputEventMap", B58), LEN(B58))</f>
+      <c r="H59" t="str">
+        <f t="shared" ref="H59" si="74">MID(B59, FIND("InputEventMap", B59), LEN(B59))</f>
         <v>InputEventMap.KEY_ASTERISK</v>
       </c>
-      <c r="I58" t="str">
-        <f t="shared" ref="I58" si="73">_xlfn.CONCAT("StreamdeckInput.", F58, ": ", H58, ",")</f>
+      <c r="I59" t="str">
+        <f t="shared" ref="I59" si="75">_xlfn.CONCAT("StreamdeckInput.", F59, ": ", H59, ",")</f>
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>18</v>
-      </c>
-      <c r="B59" t="s">
-        <v>4</v>
-      </c>
-      <c r="C59" t="s">
-        <v>89</v>
-      </c>
-      <c r="D59">
-        <v>4</v>
-      </c>
-      <c r="E59" t="str">
-        <f t="shared" si="62"/>
-        <v>help</v>
-      </c>
-      <c r="F59" t="str">
-        <f t="shared" si="6"/>
-        <v>KEY_04</v>
-      </c>
-      <c r="G59" t="str">
-        <f t="shared" si="66"/>
-        <v>OnRecord-KEY_04-help.png</v>
-      </c>
-      <c r="H59" t="str">
-        <f t="shared" si="67"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
-      </c>
-      <c r="I59" t="str">
-        <f t="shared" si="68"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
@@ -3085,19 +3099,53 @@
         <v>18</v>
       </c>
       <c r="B60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" t="s">
+        <v>89</v>
+      </c>
+      <c r="D60">
+        <v>4</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="62"/>
+        <v>help</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="6"/>
+        <v>KEY_04</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="68"/>
+        <v>OnRecord-KEY_04-help.png</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="69"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
+      </c>
+      <c r="I60" t="str">
+        <f t="shared" si="70"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" t="s">
         <v>46</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>116</v>
       </c>
-      <c r="D60">
+      <c r="D61">
         <v>6</v>
       </c>
-      <c r="E60" t="str">
-        <f t="shared" ref="E60:E64" si="74">LOWER(
+      <c r="E61" t="str">
+        <f t="shared" ref="E61:E65" si="76">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B60, FIND(" = InputEventMap", B60) - 1),
+      LEFT(B61, FIND(" = InputEventMap", B61) - 1),
       CHAR(160),
       " "
     )
@@ -3105,58 +3153,24 @@
 )</f>
         <v>stop_recording</v>
       </c>
-      <c r="F60" t="str">
-        <f t="shared" ref="F60:F64" si="75">"KEY_" &amp; CHOOSE(
-    D60+1,
+      <c r="F61" t="str">
+        <f t="shared" ref="F61:F65" si="77">"KEY_" &amp; CHOOSE(
+    D61+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_06</v>
       </c>
-      <c r="G60" t="str">
-        <f t="shared" ref="G60:G64" si="76">_xlfn.CONCAT(A60, "-", F60, "-", E60, ".png")</f>
+      <c r="G61" t="str">
+        <f t="shared" ref="G61:G65" si="78">_xlfn.CONCAT(A61, "-", F61, "-", E61, ".png")</f>
         <v>OnRecord-KEY_06-stop_recording.png</v>
       </c>
-      <c r="H60" t="str">
-        <f t="shared" ref="H60:H64" si="77">MID(B60, FIND("InputEventMap", B60), LEN(B60))</f>
+      <c r="H61" t="str">
+        <f t="shared" ref="H61:H65" si="79">MID(B61, FIND("InputEventMap", B61), LEN(B61))</f>
         <v>InputEventMap.KEY_1</v>
       </c>
-      <c r="I60" t="str">
-        <f t="shared" ref="I60:I64" si="78">_xlfn.CONCAT("StreamdeckInput.", F60, ": ", H60, ",")</f>
+      <c r="I61" t="str">
+        <f t="shared" ref="I61:I65" si="80">_xlfn.CONCAT("StreamdeckInput.", F61, ": ", H61, ",")</f>
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_1,</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>18</v>
-      </c>
-      <c r="B61" t="s">
-        <v>47</v>
-      </c>
-      <c r="C61" t="s">
-        <v>117</v>
-      </c>
-      <c r="D61">
-        <v>5</v>
-      </c>
-      <c r="E61" t="str">
-        <f t="shared" si="74"/>
-        <v>set_cue</v>
-      </c>
-      <c r="F61" t="str">
-        <f t="shared" si="75"/>
-        <v>KEY_05</v>
-      </c>
-      <c r="G61" t="str">
-        <f t="shared" si="76"/>
-        <v>OnRecord-KEY_05-set_cue.png</v>
-      </c>
-      <c r="H61" t="str">
-        <f t="shared" si="77"/>
-        <v>InputEventMap.KEY_2</v>
-      </c>
-      <c r="I61" t="str">
-        <f t="shared" si="78"/>
-        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.45">
@@ -3164,33 +3178,33 @@
         <v>18</v>
       </c>
       <c r="B62" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C62" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D62">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E62" t="str">
-        <f t="shared" si="74"/>
-        <v>toggle_mute</v>
+        <f t="shared" si="76"/>
+        <v>set_cue</v>
       </c>
       <c r="F62" t="str">
-        <f t="shared" si="75"/>
-        <v>KEY_07</v>
+        <f t="shared" si="77"/>
+        <v>KEY_05</v>
       </c>
       <c r="G62" t="str">
-        <f t="shared" si="76"/>
-        <v>OnRecord-KEY_07-toggle_mute.png</v>
+        <f t="shared" si="78"/>
+        <v>OnRecord-KEY_05-set_cue.png</v>
       </c>
       <c r="H62" t="str">
-        <f t="shared" si="77"/>
-        <v>InputEventMap.KEY_3</v>
+        <f t="shared" si="79"/>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I62" t="str">
-        <f t="shared" si="78"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
+        <f t="shared" si="80"/>
+        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.45">
@@ -3198,67 +3212,67 @@
         <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C63" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D63">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E63" t="str">
-        <f t="shared" si="74"/>
-        <v>show_status</v>
+        <f t="shared" si="76"/>
+        <v>toggle_mute</v>
       </c>
       <c r="F63" t="str">
-        <f t="shared" si="75"/>
-        <v>KEY_0A</v>
+        <f t="shared" si="77"/>
+        <v>KEY_07</v>
       </c>
       <c r="G63" t="str">
-        <f t="shared" si="76"/>
-        <v>OnRecord-KEY_0A-show_status.png</v>
+        <f t="shared" si="78"/>
+        <v>OnRecord-KEY_07-toggle_mute.png</v>
       </c>
       <c r="H63" t="str">
-        <f t="shared" si="77"/>
-        <v>InputEventMap.KEY_4</v>
+        <f t="shared" si="79"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I63" t="str">
-        <f t="shared" si="78"/>
-        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_4,</v>
+        <f t="shared" si="80"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B64" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="C64" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E64" t="str">
-        <f t="shared" si="74"/>
-        <v>screen</v>
+        <f t="shared" si="76"/>
+        <v>show_status</v>
       </c>
       <c r="F64" t="str">
-        <f t="shared" si="75"/>
-        <v>KEY_00</v>
+        <f t="shared" si="77"/>
+        <v>KEY_0A</v>
       </c>
       <c r="G64" t="str">
-        <f t="shared" si="76"/>
-        <v>PlaybackPaused-KEY_00-screen.png</v>
+        <f t="shared" si="78"/>
+        <v>OnRecord-KEY_0A-show_status.png</v>
       </c>
       <c r="H64" t="str">
-        <f t="shared" si="77"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
+        <f t="shared" si="79"/>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I64" t="str">
-        <f t="shared" si="78"/>
-        <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
+        <f t="shared" si="80"/>
+        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_4,</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.45">
@@ -3266,19 +3280,53 @@
         <v>29</v>
       </c>
       <c r="B65" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="76"/>
+        <v>screen</v>
+      </c>
+      <c r="F65" t="str">
+        <f t="shared" si="77"/>
+        <v>KEY_00</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="78"/>
+        <v>PlaybackPaused-KEY_00-screen.png</v>
+      </c>
+      <c r="H65" t="str">
+        <f t="shared" si="79"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
+      </c>
+      <c r="I65" t="str">
+        <f t="shared" si="80"/>
+        <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>29</v>
+      </c>
+      <c r="B66" t="s">
         <v>4</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>89</v>
       </c>
-      <c r="D65">
+      <c r="D66">
         <v>4</v>
       </c>
-      <c r="E65" t="str">
-        <f t="shared" ref="E65:E132" si="79">LOWER(
+      <c r="E66" t="str">
+        <f t="shared" ref="E66:E133" si="81">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B65, FIND(" = InputEventMap", B65) - 1),
+      LEFT(B66, FIND(" = InputEventMap", B66) - 1),
       CHAR(160),
       " "
     )
@@ -3286,58 +3334,24 @@
 )</f>
         <v>help</v>
       </c>
-      <c r="F65" t="str">
-        <f t="shared" ref="F65:F132" si="80">"KEY_" &amp; CHOOSE(
-    D65+1,
+      <c r="F66" t="str">
+        <f t="shared" ref="F66:F133" si="82">"KEY_" &amp; CHOOSE(
+    D66+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_04</v>
       </c>
-      <c r="G65" t="str">
-        <f t="shared" ref="G65:G132" si="81">_xlfn.CONCAT(A65, "-", F65, "-", E65, ".png")</f>
+      <c r="G66" t="str">
+        <f t="shared" ref="G66:G133" si="83">_xlfn.CONCAT(A66, "-", F66, "-", E66, ".png")</f>
         <v>PlaybackPaused-KEY_04-help.png</v>
       </c>
-      <c r="H65" t="str">
-        <f t="shared" ref="H65:H132" si="82">MID(B65, FIND("InputEventMap", B65), LEN(B65))</f>
+      <c r="H66" t="str">
+        <f t="shared" ref="H66:H133" si="84">MID(B66, FIND("InputEventMap", B66), LEN(B66))</f>
         <v>InputEventMap.KEY_ASTERISK</v>
       </c>
-      <c r="I65" t="str">
-        <f t="shared" ref="I65:I132" si="83">_xlfn.CONCAT("StreamdeckInput.", F65, ": ", H65, ",")</f>
+      <c r="I66" t="str">
+        <f t="shared" ref="I66:I133" si="85">_xlfn.CONCAT("StreamdeckInput.", F66, ": ", H66, ",")</f>
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
-        <v>29</v>
-      </c>
-      <c r="B66" t="s">
-        <v>50</v>
-      </c>
-      <c r="C66" t="s">
-        <v>113</v>
-      </c>
-      <c r="D66">
-        <v>7</v>
-      </c>
-      <c r="E66" t="str">
-        <f t="shared" si="79"/>
-        <v>pause_resume</v>
-      </c>
-      <c r="F66" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_07</v>
-      </c>
-      <c r="G66" t="str">
-        <f t="shared" si="81"/>
-        <v>PlaybackPaused-KEY_07-pause_resume.png</v>
-      </c>
-      <c r="H66" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_0</v>
-      </c>
-      <c r="I66" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_0,</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
@@ -3345,53 +3359,87 @@
         <v>29</v>
       </c>
       <c r="B67" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="C67" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="D67">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" si="79"/>
-        <v>menu</v>
+        <f t="shared" si="81"/>
+        <v>pause_resume</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_09</v>
+        <f t="shared" si="82"/>
+        <v>KEY_07</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" si="81"/>
-        <v>PlaybackPaused-KEY_09-menu.png</v>
+        <f t="shared" si="83"/>
+        <v>PlaybackPaused-KEY_07-pause_resume.png</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_5</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_0</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_0,</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
+        <v>29</v>
+      </c>
+      <c r="B68" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
+        <v>98</v>
+      </c>
+      <c r="D68">
+        <v>9</v>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" si="81"/>
+        <v>menu</v>
+      </c>
+      <c r="F68" t="str">
+        <f t="shared" si="82"/>
+        <v>KEY_09</v>
+      </c>
+      <c r="G68" t="str">
+        <f t="shared" si="83"/>
+        <v>PlaybackPaused-KEY_09-menu.png</v>
+      </c>
+      <c r="H68" t="str">
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_5</v>
+      </c>
+      <c r="I68" t="str">
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
         <v>28</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>100</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" t="s">
         <v>120</v>
       </c>
-      <c r="D68">
+      <c r="D69">
         <v>0</v>
       </c>
-      <c r="E68" t="str">
-        <f t="shared" ref="E68" si="84">LOWER(
+      <c r="E69" t="str">
+        <f t="shared" ref="E69" si="86">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B68, FIND(" = InputEventMap", B68) - 1),
+      LEFT(B69, FIND(" = InputEventMap", B69) - 1),
       CHAR(160),
       " "
     )
@@ -3399,58 +3447,24 @@
 )</f>
         <v>screen</v>
       </c>
-      <c r="F68" t="str">
-        <f t="shared" ref="F68" si="85">"KEY_" &amp; CHOOSE(
-    D68+1,
+      <c r="F69" t="str">
+        <f t="shared" ref="F69" si="87">"KEY_" &amp; CHOOSE(
+    D69+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G68" t="str">
-        <f t="shared" ref="G68" si="86">_xlfn.CONCAT(A68, "-", F68, "-", E68, ".png")</f>
+      <c r="G69" t="str">
+        <f t="shared" ref="G69" si="88">_xlfn.CONCAT(A69, "-", F69, "-", E69, ".png")</f>
         <v>Playback-KEY_00-screen.png</v>
       </c>
-      <c r="H68" t="str">
-        <f t="shared" ref="H68" si="87">MID(B68, FIND("InputEventMap", B68), LEN(B68))</f>
+      <c r="H69" t="str">
+        <f t="shared" ref="H69" si="89">MID(B69, FIND("InputEventMap", B69), LEN(B69))</f>
         <v>InputEventMap.KEY_ASTERISK</v>
       </c>
-      <c r="I68" t="str">
-        <f t="shared" ref="I68" si="88">_xlfn.CONCAT("StreamdeckInput.", F68, ": ", H68, ",")</f>
+      <c r="I69" t="str">
+        <f t="shared" ref="I69" si="90">_xlfn.CONCAT("StreamdeckInput.", F69, ": ", H69, ",")</f>
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
-        <v>28</v>
-      </c>
-      <c r="B69" t="s">
-        <v>4</v>
-      </c>
-      <c r="C69" t="s">
-        <v>89</v>
-      </c>
-      <c r="D69">
-        <v>4</v>
-      </c>
-      <c r="E69" t="str">
-        <f t="shared" si="79"/>
-        <v>help</v>
-      </c>
-      <c r="F69" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_04</v>
-      </c>
-      <c r="G69" t="str">
-        <f t="shared" si="81"/>
-        <v>Playback-KEY_04-help.png</v>
-      </c>
-      <c r="H69" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
-      </c>
-      <c r="I69" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.45">
@@ -3458,33 +3472,33 @@
         <v>28</v>
       </c>
       <c r="B70" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>121</v>
+        <v>89</v>
       </c>
       <c r="D70">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="79"/>
-        <v>pause_resume</v>
+        <f t="shared" si="81"/>
+        <v>help</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_07</v>
+        <f t="shared" si="82"/>
+        <v>KEY_04</v>
       </c>
       <c r="G70" t="str">
-        <f t="shared" si="81"/>
-        <v>Playback-KEY_07-pause_resume.png</v>
+        <f t="shared" si="83"/>
+        <v>Playback-KEY_04-help.png</v>
       </c>
       <c r="H70" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_0</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
       </c>
       <c r="I70" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_0,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.45">
@@ -3492,33 +3506,33 @@
         <v>28</v>
       </c>
       <c r="B71" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C71" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D71">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E71" t="str">
-        <f t="shared" si="79"/>
-        <v>jump_clip_end</v>
+        <f t="shared" si="81"/>
+        <v>pause_resume</v>
       </c>
       <c r="F71" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0B</v>
+        <f t="shared" si="82"/>
+        <v>KEY_07</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" si="81"/>
-        <v>Playback-KEY_0B-jump_clip_end.png</v>
+        <f t="shared" si="83"/>
+        <v>Playback-KEY_07-pause_resume.png</v>
       </c>
       <c r="H71" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_1</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_0</v>
       </c>
       <c r="I71" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_0,</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.45">
@@ -3526,33 +3540,33 @@
         <v>28</v>
       </c>
       <c r="B72" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C72" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D72">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E72" t="str">
-        <f t="shared" si="79"/>
-        <v>seek_next</v>
+        <f t="shared" si="81"/>
+        <v>jump_clip_end</v>
       </c>
       <c r="F72" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0C</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0B</v>
       </c>
       <c r="G72" t="str">
-        <f t="shared" si="81"/>
-        <v>Playback-KEY_0C-seek_next.png</v>
+        <f t="shared" si="83"/>
+        <v>Playback-KEY_0B-jump_clip_end.png</v>
       </c>
       <c r="H72" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_2</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I72" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.45">
@@ -3560,33 +3574,33 @@
         <v>28</v>
       </c>
       <c r="B73" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C73" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D73">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E73" t="str">
-        <f t="shared" si="79"/>
-        <v>jump_cue_next</v>
+        <f t="shared" si="81"/>
+        <v>seek_next</v>
       </c>
       <c r="F73" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0D</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0C</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="81"/>
-        <v>Playback-KEY_0D-jump_cue_next.png</v>
+        <f t="shared" si="83"/>
+        <v>Playback-KEY_0C-seek_next.png</v>
       </c>
       <c r="H73" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_3</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I73" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.45">
@@ -3594,33 +3608,33 @@
         <v>28</v>
       </c>
       <c r="B74" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C74" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D74">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E74" t="str">
-        <f t="shared" si="79"/>
-        <v>jump_clip_previous</v>
+        <f t="shared" si="81"/>
+        <v>jump_cue_next</v>
       </c>
       <c r="F74" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_06</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0D</v>
       </c>
       <c r="G74" t="str">
-        <f t="shared" si="81"/>
-        <v>Playback-KEY_06-jump_clip_previous.png</v>
+        <f t="shared" si="83"/>
+        <v>Playback-KEY_0D-jump_cue_next.png</v>
       </c>
       <c r="H74" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_4</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I74" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.45">
@@ -3628,33 +3642,33 @@
         <v>28</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="C75" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="D75">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E75" t="str">
-        <f t="shared" si="79"/>
-        <v>menu</v>
+        <f t="shared" si="81"/>
+        <v>jump_clip_previous</v>
       </c>
       <c r="F75" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_09</v>
+        <f t="shared" si="82"/>
+        <v>KEY_06</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" si="81"/>
-        <v>Playback-KEY_09-menu.png</v>
+        <f t="shared" si="83"/>
+        <v>Playback-KEY_06-jump_clip_previous.png</v>
       </c>
       <c r="H75" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_5</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I75" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
@@ -3662,33 +3676,33 @@
         <v>28</v>
       </c>
       <c r="B76" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="D76">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E76" t="str">
-        <f t="shared" si="79"/>
-        <v>jump_clip_next</v>
+        <f t="shared" si="81"/>
+        <v>menu</v>
       </c>
       <c r="F76" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_08</v>
+        <f t="shared" si="82"/>
+        <v>KEY_09</v>
       </c>
       <c r="G76" t="str">
-        <f t="shared" si="81"/>
-        <v>Playback-KEY_08-jump_clip_next.png</v>
+        <f t="shared" si="83"/>
+        <v>Playback-KEY_09-menu.png</v>
       </c>
       <c r="H76" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_6</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_5</v>
       </c>
       <c r="I76" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.45">
@@ -3696,33 +3710,33 @@
         <v>28</v>
       </c>
       <c r="B77" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C77" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D77">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E77" t="str">
-        <f t="shared" si="79"/>
-        <v>jump_clip_start</v>
+        <f t="shared" si="81"/>
+        <v>jump_clip_next</v>
       </c>
       <c r="F77" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_01</v>
+        <f t="shared" si="82"/>
+        <v>KEY_08</v>
       </c>
       <c r="G77" t="str">
-        <f t="shared" si="81"/>
-        <v>Playback-KEY_01-jump_clip_start.png</v>
+        <f t="shared" si="83"/>
+        <v>Playback-KEY_08-jump_clip_next.png</v>
       </c>
       <c r="H77" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_7</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_6</v>
       </c>
       <c r="I77" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.45">
@@ -3730,33 +3744,33 @@
         <v>28</v>
       </c>
       <c r="B78" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C78" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E78" t="str">
-        <f t="shared" si="79"/>
-        <v>seek_previous</v>
+        <f t="shared" si="81"/>
+        <v>jump_clip_start</v>
       </c>
       <c r="F78" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_02</v>
+        <f t="shared" si="82"/>
+        <v>KEY_01</v>
       </c>
       <c r="G78" t="str">
-        <f t="shared" si="81"/>
-        <v>Playback-KEY_02-seek_previous.png</v>
+        <f t="shared" si="83"/>
+        <v>Playback-KEY_01-jump_clip_start.png</v>
       </c>
       <c r="H78" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_8</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_7</v>
       </c>
       <c r="I78" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.45">
@@ -3764,53 +3778,87 @@
         <v>28</v>
       </c>
       <c r="B79" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C79" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D79">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E79" t="str">
-        <f t="shared" si="79"/>
-        <v>jump_cue_previous</v>
+        <f t="shared" si="81"/>
+        <v>seek_previous</v>
       </c>
       <c r="F79" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_03</v>
+        <f t="shared" si="82"/>
+        <v>KEY_02</v>
       </c>
       <c r="G79" t="str">
-        <f t="shared" si="81"/>
-        <v>Playback-KEY_03-jump_cue_previous.png</v>
+        <f t="shared" si="83"/>
+        <v>Playback-KEY_02-seek_previous.png</v>
       </c>
       <c r="H79" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_9</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_8</v>
       </c>
       <c r="I79" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
+        <v>28</v>
+      </c>
+      <c r="B80" t="s">
+        <v>58</v>
+      </c>
+      <c r="C80" t="s">
+        <v>125</v>
+      </c>
+      <c r="D80">
+        <v>3</v>
+      </c>
+      <c r="E80" t="str">
+        <f t="shared" si="81"/>
+        <v>jump_cue_previous</v>
+      </c>
+      <c r="F80" t="str">
+        <f t="shared" si="82"/>
+        <v>KEY_03</v>
+      </c>
+      <c r="G80" t="str">
+        <f t="shared" si="83"/>
+        <v>Playback-KEY_03-jump_cue_previous.png</v>
+      </c>
+      <c r="H80" t="str">
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_9</v>
+      </c>
+      <c r="I80" t="str">
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
         <v>24</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>100</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C81" t="s">
         <v>130</v>
       </c>
-      <c r="D80">
+      <c r="D81">
         <v>0</v>
       </c>
-      <c r="E80" t="str">
-        <f t="shared" ref="E80" si="89">LOWER(
+      <c r="E81" t="str">
+        <f t="shared" ref="E81" si="91">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B80, FIND(" = InputEventMap", B80) - 1),
+      LEFT(B81, FIND(" = InputEventMap", B81) - 1),
       CHAR(160),
       " "
     )
@@ -3818,58 +3866,24 @@
 )</f>
         <v>screen</v>
       </c>
-      <c r="F80" t="str">
-        <f t="shared" ref="F80" si="90">"KEY_" &amp; CHOOSE(
-    D80+1,
+      <c r="F81" t="str">
+        <f t="shared" ref="F81" si="92">"KEY_" &amp; CHOOSE(
+    D81+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G80" t="str">
-        <f t="shared" ref="G80" si="91">_xlfn.CONCAT(A80, "-", F80, "-", E80, ".png")</f>
+      <c r="G81" t="str">
+        <f t="shared" ref="G81" si="93">_xlfn.CONCAT(A81, "-", F81, "-", E81, ".png")</f>
         <v>SelectLanguage-KEY_00-screen.png</v>
       </c>
-      <c r="H80" t="str">
-        <f t="shared" ref="H80" si="92">MID(B80, FIND("InputEventMap", B80), LEN(B80))</f>
+      <c r="H81" t="str">
+        <f t="shared" ref="H81" si="94">MID(B81, FIND("InputEventMap", B81), LEN(B81))</f>
         <v>InputEventMap.KEY_ASTERISK</v>
       </c>
-      <c r="I80" t="str">
-        <f t="shared" ref="I80" si="93">_xlfn.CONCAT("StreamdeckInput.", F80, ": ", H80, ",")</f>
+      <c r="I81" t="str">
+        <f t="shared" ref="I81" si="95">_xlfn.CONCAT("StreamdeckInput.", F81, ": ", H81, ",")</f>
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
-        <v>24</v>
-      </c>
-      <c r="B81" t="s">
-        <v>4</v>
-      </c>
-      <c r="C81" t="s">
-        <v>89</v>
-      </c>
-      <c r="D81">
-        <v>4</v>
-      </c>
-      <c r="E81" t="str">
-        <f t="shared" si="79"/>
-        <v>help</v>
-      </c>
-      <c r="F81" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_04</v>
-      </c>
-      <c r="G81" t="str">
-        <f t="shared" si="81"/>
-        <v>SelectLanguage-KEY_04-help.png</v>
-      </c>
-      <c r="H81" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
-      </c>
-      <c r="I81" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.45">
@@ -3877,33 +3891,33 @@
         <v>24</v>
       </c>
       <c r="B82" t="s">
-        <v>59</v>
+        <v>4</v>
       </c>
       <c r="C82" t="s">
-        <v>131</v>
+        <v>89</v>
       </c>
       <c r="D82">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E82" t="str">
-        <f t="shared" si="79"/>
-        <v>select_english</v>
+        <f t="shared" si="81"/>
+        <v>help</v>
       </c>
       <c r="F82" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_05</v>
+        <f t="shared" si="82"/>
+        <v>KEY_04</v>
       </c>
       <c r="G82" t="str">
-        <f t="shared" si="81"/>
-        <v>SelectLanguage-KEY_05-select_english.png</v>
+        <f t="shared" si="83"/>
+        <v>SelectLanguage-KEY_04-help.png</v>
       </c>
       <c r="H82" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_1</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
       </c>
       <c r="I82" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.45">
@@ -3911,33 +3925,33 @@
         <v>24</v>
       </c>
       <c r="B83" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C83" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D83">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E83" t="str">
-        <f t="shared" si="79"/>
-        <v>select_german</v>
+        <f t="shared" si="81"/>
+        <v>select_english</v>
       </c>
       <c r="F83" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_06</v>
+        <f t="shared" si="82"/>
+        <v>KEY_05</v>
       </c>
       <c r="G83" t="str">
-        <f t="shared" si="81"/>
-        <v>SelectLanguage-KEY_06-select_german.png</v>
+        <f t="shared" si="83"/>
+        <v>SelectLanguage-KEY_05-select_english.png</v>
       </c>
       <c r="H83" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_2</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I83" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.45">
@@ -3945,33 +3959,33 @@
         <v>24</v>
       </c>
       <c r="B84" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C84" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D84">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E84" t="str">
-        <f t="shared" si="79"/>
-        <v>select_french</v>
+        <f t="shared" si="81"/>
+        <v>select_german</v>
       </c>
       <c r="F84" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_07</v>
+        <f t="shared" si="82"/>
+        <v>KEY_06</v>
       </c>
       <c r="G84" t="str">
-        <f t="shared" si="81"/>
-        <v>SelectLanguage-KEY_07-select_french.png</v>
+        <f t="shared" si="83"/>
+        <v>SelectLanguage-KEY_06-select_german.png</v>
       </c>
       <c r="H84" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_3</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I84" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.45">
@@ -3979,53 +3993,87 @@
         <v>24</v>
       </c>
       <c r="B85" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C85" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D85">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E85" t="str">
-        <f t="shared" si="79"/>
-        <v>select_italian</v>
+        <f t="shared" si="81"/>
+        <v>select_french</v>
       </c>
       <c r="F85" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_08</v>
+        <f t="shared" si="82"/>
+        <v>KEY_07</v>
       </c>
       <c r="G85" t="str">
-        <f t="shared" si="81"/>
-        <v>SelectLanguage-KEY_08-select_italian.png</v>
+        <f t="shared" si="83"/>
+        <v>SelectLanguage-KEY_07-select_french.png</v>
       </c>
       <c r="H85" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_4</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I85" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_4,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
+        <v>24</v>
+      </c>
+      <c r="B86" t="s">
+        <v>62</v>
+      </c>
+      <c r="C86" t="s">
+        <v>134</v>
+      </c>
+      <c r="D86">
+        <v>8</v>
+      </c>
+      <c r="E86" t="str">
+        <f t="shared" si="81"/>
+        <v>select_italian</v>
+      </c>
+      <c r="F86" t="str">
+        <f t="shared" si="82"/>
+        <v>KEY_08</v>
+      </c>
+      <c r="G86" t="str">
+        <f t="shared" si="83"/>
+        <v>SelectLanguage-KEY_08-select_italian.png</v>
+      </c>
+      <c r="H86" t="str">
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_4</v>
+      </c>
+      <c r="I86" t="str">
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_4,</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A87" t="s">
         <v>25</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>100</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C87" t="s">
         <v>135</v>
       </c>
-      <c r="D86">
+      <c r="D87">
         <v>0</v>
       </c>
-      <c r="E86" t="str">
-        <f t="shared" ref="E86" si="94">LOWER(
+      <c r="E87" t="str">
+        <f t="shared" ref="E87" si="96">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B86, FIND(" = InputEventMap", B86) - 1),
+      LEFT(B87, FIND(" = InputEventMap", B87) - 1),
       CHAR(160),
       " "
     )
@@ -4033,58 +4081,24 @@
 )</f>
         <v>screen</v>
       </c>
-      <c r="F86" t="str">
-        <f t="shared" ref="F86" si="95">"KEY_" &amp; CHOOSE(
-    D86+1,
+      <c r="F87" t="str">
+        <f t="shared" ref="F87" si="97">"KEY_" &amp; CHOOSE(
+    D87+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G86" t="str">
-        <f t="shared" ref="G86" si="96">_xlfn.CONCAT(A86, "-", F86, "-", E86, ".png")</f>
+      <c r="G87" t="str">
+        <f t="shared" ref="G87" si="98">_xlfn.CONCAT(A87, "-", F87, "-", E87, ".png")</f>
         <v>SetDate-KEY_00-screen.png</v>
       </c>
-      <c r="H86" t="str">
-        <f t="shared" ref="H86" si="97">MID(B86, FIND("InputEventMap", B86), LEN(B86))</f>
+      <c r="H87" t="str">
+        <f t="shared" ref="H87" si="99">MID(B87, FIND("InputEventMap", B87), LEN(B87))</f>
         <v>InputEventMap.KEY_ASTERISK</v>
       </c>
-      <c r="I86" t="str">
-        <f t="shared" ref="I86" si="98">_xlfn.CONCAT("StreamdeckInput.", F86, ": ", H86, ",")</f>
+      <c r="I87" t="str">
+        <f t="shared" ref="I87" si="100">_xlfn.CONCAT("StreamdeckInput.", F87, ": ", H87, ",")</f>
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A87" t="s">
-        <v>25</v>
-      </c>
-      <c r="B87" t="s">
-        <v>4</v>
-      </c>
-      <c r="C87" t="s">
-        <v>89</v>
-      </c>
-      <c r="D87">
-        <v>4</v>
-      </c>
-      <c r="E87" t="str">
-        <f t="shared" si="79"/>
-        <v>help</v>
-      </c>
-      <c r="F87" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_04</v>
-      </c>
-      <c r="G87" t="str">
-        <f t="shared" si="81"/>
-        <v>SetDate-KEY_04-help.png</v>
-      </c>
-      <c r="H87" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
-      </c>
-      <c r="I87" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.45">
@@ -4092,33 +4106,33 @@
         <v>25</v>
       </c>
       <c r="B88" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="C88" t="s">
-        <v>136</v>
+        <v>89</v>
       </c>
       <c r="D88">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E88" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_0</v>
+        <f t="shared" si="81"/>
+        <v>help</v>
       </c>
       <c r="F88" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0A</v>
+        <f t="shared" si="82"/>
+        <v>KEY_04</v>
       </c>
       <c r="G88" t="str">
-        <f t="shared" si="81"/>
-        <v>SetDate-KEY_0A-digit_0.png</v>
+        <f t="shared" si="83"/>
+        <v>SetDate-KEY_04-help.png</v>
       </c>
       <c r="H88" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_0</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
       </c>
       <c r="I88" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.45">
@@ -4126,33 +4140,33 @@
         <v>25</v>
       </c>
       <c r="B89" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C89" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D89">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E89" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_1</v>
+        <f t="shared" si="81"/>
+        <v>digit_0</v>
       </c>
       <c r="F89" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0B</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0A</v>
       </c>
       <c r="G89" t="str">
-        <f t="shared" si="81"/>
-        <v>SetDate-KEY_0B-digit_1.png</v>
+        <f t="shared" si="83"/>
+        <v>SetDate-KEY_0A-digit_0.png</v>
       </c>
       <c r="H89" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_1</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_0</v>
       </c>
       <c r="I89" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.45">
@@ -4160,33 +4174,33 @@
         <v>25</v>
       </c>
       <c r="B90" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C90" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D90">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E90" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_2</v>
+        <f t="shared" si="81"/>
+        <v>digit_1</v>
       </c>
       <c r="F90" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0C</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0B</v>
       </c>
       <c r="G90" t="str">
-        <f t="shared" si="81"/>
-        <v>SetDate-KEY_0C-digit_2.png</v>
+        <f t="shared" si="83"/>
+        <v>SetDate-KEY_0B-digit_1.png</v>
       </c>
       <c r="H90" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_2</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I90" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.45">
@@ -4194,33 +4208,33 @@
         <v>25</v>
       </c>
       <c r="B91" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C91" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D91">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E91" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_3</v>
+        <f t="shared" si="81"/>
+        <v>digit_2</v>
       </c>
       <c r="F91" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0D</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0C</v>
       </c>
       <c r="G91" t="str">
-        <f t="shared" si="81"/>
-        <v>SetDate-KEY_0D-digit_3.png</v>
+        <f t="shared" si="83"/>
+        <v>SetDate-KEY_0C-digit_2.png</v>
       </c>
       <c r="H91" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_3</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I91" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.45">
@@ -4228,33 +4242,33 @@
         <v>25</v>
       </c>
       <c r="B92" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C92" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D92">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E92" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_4</v>
+        <f t="shared" si="81"/>
+        <v>digit_3</v>
       </c>
       <c r="F92" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_06</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0D</v>
       </c>
       <c r="G92" t="str">
-        <f t="shared" si="81"/>
-        <v>SetDate-KEY_06-digit_4.png</v>
+        <f t="shared" si="83"/>
+        <v>SetDate-KEY_0D-digit_3.png</v>
       </c>
       <c r="H92" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_4</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I92" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.45">
@@ -4262,33 +4276,33 @@
         <v>25</v>
       </c>
       <c r="B93" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C93" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D93">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E93" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_5</v>
+        <f t="shared" si="81"/>
+        <v>digit_4</v>
       </c>
       <c r="F93" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_07</v>
+        <f t="shared" si="82"/>
+        <v>KEY_06</v>
       </c>
       <c r="G93" t="str">
-        <f t="shared" si="81"/>
-        <v>SetDate-KEY_07-digit_5.png</v>
+        <f t="shared" si="83"/>
+        <v>SetDate-KEY_06-digit_4.png</v>
       </c>
       <c r="H93" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_5</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I93" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.45">
@@ -4296,33 +4310,33 @@
         <v>25</v>
       </c>
       <c r="B94" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C94" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D94">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E94" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_6</v>
+        <f t="shared" si="81"/>
+        <v>digit_5</v>
       </c>
       <c r="F94" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_08</v>
+        <f t="shared" si="82"/>
+        <v>KEY_07</v>
       </c>
       <c r="G94" t="str">
-        <f t="shared" si="81"/>
-        <v>SetDate-KEY_08-digit_6.png</v>
+        <f t="shared" si="83"/>
+        <v>SetDate-KEY_07-digit_5.png</v>
       </c>
       <c r="H94" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_6</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_5</v>
       </c>
       <c r="I94" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.45">
@@ -4330,33 +4344,33 @@
         <v>25</v>
       </c>
       <c r="B95" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C95" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D95">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E95" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_7</v>
+        <f t="shared" si="81"/>
+        <v>digit_6</v>
       </c>
       <c r="F95" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_01</v>
+        <f t="shared" si="82"/>
+        <v>KEY_08</v>
       </c>
       <c r="G95" t="str">
-        <f t="shared" si="81"/>
-        <v>SetDate-KEY_01-digit_7.png</v>
+        <f t="shared" si="83"/>
+        <v>SetDate-KEY_08-digit_6.png</v>
       </c>
       <c r="H95" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_7</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_6</v>
       </c>
       <c r="I95" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.45">
@@ -4364,33 +4378,33 @@
         <v>25</v>
       </c>
       <c r="B96" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C96" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D96">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E96" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_8</v>
+        <f t="shared" si="81"/>
+        <v>digit_7</v>
       </c>
       <c r="F96" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_02</v>
+        <f t="shared" si="82"/>
+        <v>KEY_01</v>
       </c>
       <c r="G96" t="str">
-        <f t="shared" si="81"/>
-        <v>SetDate-KEY_02-digit_8.png</v>
+        <f t="shared" si="83"/>
+        <v>SetDate-KEY_01-digit_7.png</v>
       </c>
       <c r="H96" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_8</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_7</v>
       </c>
       <c r="I96" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.45">
@@ -4398,33 +4412,33 @@
         <v>25</v>
       </c>
       <c r="B97" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C97" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D97">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E97" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_9</v>
+        <f t="shared" si="81"/>
+        <v>digit_8</v>
       </c>
       <c r="F97" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_03</v>
+        <f t="shared" si="82"/>
+        <v>KEY_02</v>
       </c>
       <c r="G97" t="str">
-        <f t="shared" si="81"/>
-        <v>SetDate-KEY_03-digit_9.png</v>
+        <f t="shared" si="83"/>
+        <v>SetDate-KEY_02-digit_8.png</v>
       </c>
       <c r="H97" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_9</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_8</v>
       </c>
       <c r="I97" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.45">
@@ -4432,33 +4446,33 @@
         <v>25</v>
       </c>
       <c r="B98" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C98" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D98">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E98" t="str">
-        <f t="shared" si="79"/>
-        <v>back_space</v>
+        <f t="shared" si="81"/>
+        <v>digit_9</v>
       </c>
       <c r="F98" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_05</v>
+        <f t="shared" si="82"/>
+        <v>KEY_03</v>
       </c>
       <c r="G98" t="str">
-        <f t="shared" si="81"/>
-        <v>SetDate-KEY_05-back_space.png</v>
+        <f t="shared" si="83"/>
+        <v>SetDate-KEY_03-digit_9.png</v>
       </c>
       <c r="H98" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_BACKSPACE</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_9</v>
       </c>
       <c r="I98" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.45">
@@ -4466,33 +4480,33 @@
         <v>25</v>
       </c>
       <c r="B99" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C99" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D99">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E99" t="str">
-        <f t="shared" si="79"/>
-        <v>enter</v>
+        <f t="shared" si="81"/>
+        <v>back_space</v>
       </c>
       <c r="F99" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0E</v>
+        <f t="shared" si="82"/>
+        <v>KEY_05</v>
       </c>
       <c r="G99" t="str">
-        <f t="shared" si="81"/>
-        <v>SetDate-KEY_0E-enter.png</v>
+        <f t="shared" si="83"/>
+        <v>SetDate-KEY_05-back_space.png</v>
       </c>
       <c r="H99" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_ENTER</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_BACKSPACE</v>
       </c>
       <c r="I99" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.45">
@@ -4500,53 +4514,87 @@
         <v>25</v>
       </c>
       <c r="B100" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C100" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D100">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E100" t="str">
-        <f t="shared" si="79"/>
-        <v>jump_next</v>
+        <f t="shared" si="81"/>
+        <v>enter</v>
       </c>
       <c r="F100" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_09</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0E</v>
       </c>
       <c r="G100" t="str">
-        <f t="shared" si="81"/>
-        <v>SetDate-KEY_09-jump_next.png</v>
+        <f t="shared" si="83"/>
+        <v>SetDate-KEY_0E-enter.png</v>
       </c>
       <c r="H100" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_TAB</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_ENTER</v>
       </c>
       <c r="I100" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
+        <v>25</v>
+      </c>
+      <c r="B101" t="s">
+        <v>75</v>
+      </c>
+      <c r="C101" t="s">
+        <v>148</v>
+      </c>
+      <c r="D101">
+        <v>9</v>
+      </c>
+      <c r="E101" t="str">
+        <f t="shared" si="81"/>
+        <v>jump_next</v>
+      </c>
+      <c r="F101" t="str">
+        <f t="shared" si="82"/>
+        <v>KEY_09</v>
+      </c>
+      <c r="G101" t="str">
+        <f t="shared" si="83"/>
+        <v>SetDate-KEY_09-jump_next.png</v>
+      </c>
+      <c r="H101" t="str">
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_TAB</v>
+      </c>
+      <c r="I101" t="str">
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A102" t="s">
         <v>27</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B102" t="s">
         <v>100</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C102" t="s">
         <v>149</v>
       </c>
-      <c r="D101">
+      <c r="D102">
         <v>0</v>
       </c>
-      <c r="E101" t="str">
-        <f t="shared" ref="E101" si="99">LOWER(
+      <c r="E102" t="str">
+        <f t="shared" ref="E102" si="101">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B101, FIND(" = InputEventMap", B101) - 1),
+      LEFT(B102, FIND(" = InputEventMap", B102) - 1),
       CHAR(160),
       " "
     )
@@ -4554,58 +4602,24 @@
 )</f>
         <v>screen</v>
       </c>
-      <c r="F101" t="str">
-        <f t="shared" ref="F101" si="100">"KEY_" &amp; CHOOSE(
-    D101+1,
+      <c r="F102" t="str">
+        <f t="shared" ref="F102" si="102">"KEY_" &amp; CHOOSE(
+    D102+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G101" t="str">
-        <f t="shared" ref="G101" si="101">_xlfn.CONCAT(A101, "-", F101, "-", E101, ".png")</f>
+      <c r="G102" t="str">
+        <f t="shared" ref="G102" si="103">_xlfn.CONCAT(A102, "-", F102, "-", E102, ".png")</f>
         <v>SetName-KEY_00-screen.png</v>
       </c>
-      <c r="H101" t="str">
-        <f t="shared" ref="H101" si="102">MID(B101, FIND("InputEventMap", B101), LEN(B101))</f>
+      <c r="H102" t="str">
+        <f t="shared" ref="H102" si="104">MID(B102, FIND("InputEventMap", B102), LEN(B102))</f>
         <v>InputEventMap.KEY_ASTERISK</v>
       </c>
-      <c r="I101" t="str">
-        <f t="shared" ref="I101" si="103">_xlfn.CONCAT("StreamdeckInput.", F101, ": ", H101, ",")</f>
+      <c r="I102" t="str">
+        <f t="shared" ref="I102" si="105">_xlfn.CONCAT("StreamdeckInput.", F102, ": ", H102, ",")</f>
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A102" t="s">
-        <v>27</v>
-      </c>
-      <c r="B102" t="s">
-        <v>4</v>
-      </c>
-      <c r="C102" t="s">
-        <v>89</v>
-      </c>
-      <c r="D102">
-        <v>4</v>
-      </c>
-      <c r="E102" t="str">
-        <f t="shared" si="79"/>
-        <v>help</v>
-      </c>
-      <c r="F102" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_04</v>
-      </c>
-      <c r="G102" t="str">
-        <f t="shared" si="81"/>
-        <v>SetName-KEY_04-help.png</v>
-      </c>
-      <c r="H102" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
-      </c>
-      <c r="I102" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.45">
@@ -4613,33 +4627,33 @@
         <v>27</v>
       </c>
       <c r="B103" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="C103" t="s">
-        <v>136</v>
+        <v>89</v>
       </c>
       <c r="D103">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E103" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_0</v>
+        <f t="shared" si="81"/>
+        <v>help</v>
       </c>
       <c r="F103" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0A</v>
+        <f t="shared" si="82"/>
+        <v>KEY_04</v>
       </c>
       <c r="G103" t="str">
-        <f t="shared" si="81"/>
-        <v>SetName-KEY_0A-digit_0.png</v>
+        <f t="shared" si="83"/>
+        <v>SetName-KEY_04-help.png</v>
       </c>
       <c r="H103" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_0</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
       </c>
       <c r="I103" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.45">
@@ -4647,33 +4661,33 @@
         <v>27</v>
       </c>
       <c r="B104" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C104" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D104">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E104" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_1</v>
+        <f t="shared" si="81"/>
+        <v>digit_0</v>
       </c>
       <c r="F104" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0B</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0A</v>
       </c>
       <c r="G104" t="str">
-        <f t="shared" si="81"/>
-        <v>SetName-KEY_0B-digit_1.png</v>
+        <f t="shared" si="83"/>
+        <v>SetName-KEY_0A-digit_0.png</v>
       </c>
       <c r="H104" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_1</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_0</v>
       </c>
       <c r="I104" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.45">
@@ -4681,33 +4695,33 @@
         <v>27</v>
       </c>
       <c r="B105" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C105" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D105">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E105" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_2</v>
+        <f t="shared" si="81"/>
+        <v>digit_1</v>
       </c>
       <c r="F105" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0C</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0B</v>
       </c>
       <c r="G105" t="str">
-        <f t="shared" si="81"/>
-        <v>SetName-KEY_0C-digit_2.png</v>
+        <f t="shared" si="83"/>
+        <v>SetName-KEY_0B-digit_1.png</v>
       </c>
       <c r="H105" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_2</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I105" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.45">
@@ -4715,33 +4729,33 @@
         <v>27</v>
       </c>
       <c r="B106" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C106" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D106">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E106" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_3</v>
+        <f t="shared" si="81"/>
+        <v>digit_2</v>
       </c>
       <c r="F106" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0D</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0C</v>
       </c>
       <c r="G106" t="str">
-        <f t="shared" si="81"/>
-        <v>SetName-KEY_0D-digit_3.png</v>
+        <f t="shared" si="83"/>
+        <v>SetName-KEY_0C-digit_2.png</v>
       </c>
       <c r="H106" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_3</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I106" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.45">
@@ -4749,33 +4763,33 @@
         <v>27</v>
       </c>
       <c r="B107" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C107" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D107">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E107" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_4</v>
+        <f t="shared" si="81"/>
+        <v>digit_3</v>
       </c>
       <c r="F107" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_06</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0D</v>
       </c>
       <c r="G107" t="str">
-        <f t="shared" si="81"/>
-        <v>SetName-KEY_06-digit_4.png</v>
+        <f t="shared" si="83"/>
+        <v>SetName-KEY_0D-digit_3.png</v>
       </c>
       <c r="H107" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_4</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I107" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.45">
@@ -4783,33 +4797,33 @@
         <v>27</v>
       </c>
       <c r="B108" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C108" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D108">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E108" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_5</v>
+        <f t="shared" si="81"/>
+        <v>digit_4</v>
       </c>
       <c r="F108" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_07</v>
+        <f t="shared" si="82"/>
+        <v>KEY_06</v>
       </c>
       <c r="G108" t="str">
-        <f t="shared" si="81"/>
-        <v>SetName-KEY_07-digit_5.png</v>
+        <f t="shared" si="83"/>
+        <v>SetName-KEY_06-digit_4.png</v>
       </c>
       <c r="H108" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_5</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I108" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.45">
@@ -4817,33 +4831,33 @@
         <v>27</v>
       </c>
       <c r="B109" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C109" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D109">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E109" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_6</v>
+        <f t="shared" si="81"/>
+        <v>digit_5</v>
       </c>
       <c r="F109" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_08</v>
+        <f t="shared" si="82"/>
+        <v>KEY_07</v>
       </c>
       <c r="G109" t="str">
-        <f t="shared" si="81"/>
-        <v>SetName-KEY_08-digit_6.png</v>
+        <f t="shared" si="83"/>
+        <v>SetName-KEY_07-digit_5.png</v>
       </c>
       <c r="H109" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_6</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_5</v>
       </c>
       <c r="I109" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.45">
@@ -4851,33 +4865,33 @@
         <v>27</v>
       </c>
       <c r="B110" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C110" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D110">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E110" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_7</v>
+        <f t="shared" si="81"/>
+        <v>digit_6</v>
       </c>
       <c r="F110" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_01</v>
+        <f t="shared" si="82"/>
+        <v>KEY_08</v>
       </c>
       <c r="G110" t="str">
-        <f t="shared" si="81"/>
-        <v>SetName-KEY_01-digit_7.png</v>
+        <f t="shared" si="83"/>
+        <v>SetName-KEY_08-digit_6.png</v>
       </c>
       <c r="H110" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_7</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_6</v>
       </c>
       <c r="I110" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.45">
@@ -4885,33 +4899,33 @@
         <v>27</v>
       </c>
       <c r="B111" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C111" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D111">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E111" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_8</v>
+        <f t="shared" si="81"/>
+        <v>digit_7</v>
       </c>
       <c r="F111" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_02</v>
+        <f t="shared" si="82"/>
+        <v>KEY_01</v>
       </c>
       <c r="G111" t="str">
-        <f t="shared" si="81"/>
-        <v>SetName-KEY_02-digit_8.png</v>
+        <f t="shared" si="83"/>
+        <v>SetName-KEY_01-digit_7.png</v>
       </c>
       <c r="H111" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_8</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_7</v>
       </c>
       <c r="I111" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.45">
@@ -4919,33 +4933,33 @@
         <v>27</v>
       </c>
       <c r="B112" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C112" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D112">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E112" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_9</v>
+        <f t="shared" si="81"/>
+        <v>digit_8</v>
       </c>
       <c r="F112" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_03</v>
+        <f t="shared" si="82"/>
+        <v>KEY_02</v>
       </c>
       <c r="G112" t="str">
-        <f t="shared" si="81"/>
-        <v>SetName-KEY_03-digit_9.png</v>
+        <f t="shared" si="83"/>
+        <v>SetName-KEY_02-digit_8.png</v>
       </c>
       <c r="H112" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_9</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_8</v>
       </c>
       <c r="I112" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.45">
@@ -4953,33 +4967,33 @@
         <v>27</v>
       </c>
       <c r="B113" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C113" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D113">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E113" t="str">
-        <f t="shared" si="79"/>
-        <v>back_space</v>
+        <f t="shared" si="81"/>
+        <v>digit_9</v>
       </c>
       <c r="F113" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_05</v>
+        <f t="shared" si="82"/>
+        <v>KEY_03</v>
       </c>
       <c r="G113" t="str">
-        <f t="shared" si="81"/>
-        <v>SetName-KEY_05-back_space.png</v>
+        <f t="shared" si="83"/>
+        <v>SetName-KEY_03-digit_9.png</v>
       </c>
       <c r="H113" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_BACKSPACE</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_9</v>
       </c>
       <c r="I113" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.45">
@@ -4987,33 +5001,33 @@
         <v>27</v>
       </c>
       <c r="B114" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C114" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D114">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E114" t="str">
-        <f t="shared" si="79"/>
-        <v>enter</v>
+        <f t="shared" si="81"/>
+        <v>back_space</v>
       </c>
       <c r="F114" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0E</v>
+        <f t="shared" si="82"/>
+        <v>KEY_05</v>
       </c>
       <c r="G114" t="str">
-        <f t="shared" si="81"/>
-        <v>SetName-KEY_0E-enter.png</v>
+        <f t="shared" si="83"/>
+        <v>SetName-KEY_05-back_space.png</v>
       </c>
       <c r="H114" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_ENTER</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_BACKSPACE</v>
       </c>
       <c r="I114" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.45">
@@ -5021,53 +5035,87 @@
         <v>27</v>
       </c>
       <c r="B115" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C115" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D115">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E115" t="str">
-        <f t="shared" si="79"/>
-        <v>jump_next</v>
+        <f t="shared" si="81"/>
+        <v>enter</v>
       </c>
       <c r="F115" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_09</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0E</v>
       </c>
       <c r="G115" t="str">
-        <f t="shared" si="81"/>
-        <v>SetName-KEY_09-jump_next.png</v>
+        <f t="shared" si="83"/>
+        <v>SetName-KEY_0E-enter.png</v>
       </c>
       <c r="H115" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_TAB</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_ENTER</v>
       </c>
       <c r="I115" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
+        <v>27</v>
+      </c>
+      <c r="B116" t="s">
+        <v>75</v>
+      </c>
+      <c r="C116" t="s">
+        <v>148</v>
+      </c>
+      <c r="D116">
+        <v>9</v>
+      </c>
+      <c r="E116" t="str">
+        <f t="shared" si="81"/>
+        <v>jump_next</v>
+      </c>
+      <c r="F116" t="str">
+        <f t="shared" si="82"/>
+        <v>KEY_09</v>
+      </c>
+      <c r="G116" t="str">
+        <f t="shared" si="83"/>
+        <v>SetName-KEY_09-jump_next.png</v>
+      </c>
+      <c r="H116" t="str">
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_TAB</v>
+      </c>
+      <c r="I116" t="str">
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A117" t="s">
         <v>26</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B117" t="s">
         <v>100</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C117" t="s">
         <v>150</v>
       </c>
-      <c r="D116">
+      <c r="D117">
         <v>0</v>
       </c>
-      <c r="E116" t="str">
-        <f t="shared" ref="E116" si="104">LOWER(
+      <c r="E117" t="str">
+        <f t="shared" ref="E117" si="106">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B116, FIND(" = InputEventMap", B116) - 1),
+      LEFT(B117, FIND(" = InputEventMap", B117) - 1),
       CHAR(160),
       " "
     )
@@ -5075,58 +5123,24 @@
 )</f>
         <v>screen</v>
       </c>
-      <c r="F116" t="str">
-        <f t="shared" ref="F116" si="105">"KEY_" &amp; CHOOSE(
-    D116+1,
+      <c r="F117" t="str">
+        <f t="shared" ref="F117" si="107">"KEY_" &amp; CHOOSE(
+    D117+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G116" t="str">
-        <f t="shared" ref="G116" si="106">_xlfn.CONCAT(A116, "-", F116, "-", E116, ".png")</f>
+      <c r="G117" t="str">
+        <f t="shared" ref="G117" si="108">_xlfn.CONCAT(A117, "-", F117, "-", E117, ".png")</f>
         <v>SetTime-KEY_00-screen.png</v>
       </c>
-      <c r="H116" t="str">
-        <f t="shared" ref="H116" si="107">MID(B116, FIND("InputEventMap", B116), LEN(B116))</f>
+      <c r="H117" t="str">
+        <f t="shared" ref="H117" si="109">MID(B117, FIND("InputEventMap", B117), LEN(B117))</f>
         <v>InputEventMap.KEY_ASTERISK</v>
       </c>
-      <c r="I116" t="str">
-        <f t="shared" ref="I116" si="108">_xlfn.CONCAT("StreamdeckInput.", F116, ": ", H116, ",")</f>
+      <c r="I117" t="str">
+        <f t="shared" ref="I117" si="110">_xlfn.CONCAT("StreamdeckInput.", F117, ": ", H117, ",")</f>
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A117" t="s">
-        <v>26</v>
-      </c>
-      <c r="B117" t="s">
-        <v>4</v>
-      </c>
-      <c r="C117" t="s">
-        <v>89</v>
-      </c>
-      <c r="D117">
-        <v>4</v>
-      </c>
-      <c r="E117" t="str">
-        <f t="shared" si="79"/>
-        <v>help</v>
-      </c>
-      <c r="F117" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_04</v>
-      </c>
-      <c r="G117" t="str">
-        <f t="shared" si="81"/>
-        <v>SetTime-KEY_04-help.png</v>
-      </c>
-      <c r="H117" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
-      </c>
-      <c r="I117" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.45">
@@ -5134,33 +5148,33 @@
         <v>26</v>
       </c>
       <c r="B118" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="C118" t="s">
-        <v>136</v>
+        <v>89</v>
       </c>
       <c r="D118">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E118" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_0</v>
+        <f t="shared" si="81"/>
+        <v>help</v>
       </c>
       <c r="F118" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0A</v>
+        <f t="shared" si="82"/>
+        <v>KEY_04</v>
       </c>
       <c r="G118" t="str">
-        <f t="shared" si="81"/>
-        <v>SetTime-KEY_0A-digit_0.png</v>
+        <f t="shared" si="83"/>
+        <v>SetTime-KEY_04-help.png</v>
       </c>
       <c r="H118" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_0</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
       </c>
       <c r="I118" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.45">
@@ -5168,33 +5182,33 @@
         <v>26</v>
       </c>
       <c r="B119" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C119" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D119">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E119" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_1</v>
+        <f t="shared" si="81"/>
+        <v>digit_0</v>
       </c>
       <c r="F119" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0B</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0A</v>
       </c>
       <c r="G119" t="str">
-        <f t="shared" si="81"/>
-        <v>SetTime-KEY_0B-digit_1.png</v>
+        <f t="shared" si="83"/>
+        <v>SetTime-KEY_0A-digit_0.png</v>
       </c>
       <c r="H119" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_1</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_0</v>
       </c>
       <c r="I119" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.45">
@@ -5202,33 +5216,33 @@
         <v>26</v>
       </c>
       <c r="B120" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C120" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D120">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E120" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_2</v>
+        <f t="shared" si="81"/>
+        <v>digit_1</v>
       </c>
       <c r="F120" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0C</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0B</v>
       </c>
       <c r="G120" t="str">
-        <f t="shared" si="81"/>
-        <v>SetTime-KEY_0C-digit_2.png</v>
+        <f t="shared" si="83"/>
+        <v>SetTime-KEY_0B-digit_1.png</v>
       </c>
       <c r="H120" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_2</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I120" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.45">
@@ -5236,33 +5250,33 @@
         <v>26</v>
       </c>
       <c r="B121" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C121" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D121">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E121" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_3</v>
+        <f t="shared" si="81"/>
+        <v>digit_2</v>
       </c>
       <c r="F121" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0D</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0C</v>
       </c>
       <c r="G121" t="str">
-        <f t="shared" si="81"/>
-        <v>SetTime-KEY_0D-digit_3.png</v>
+        <f t="shared" si="83"/>
+        <v>SetTime-KEY_0C-digit_2.png</v>
       </c>
       <c r="H121" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_3</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I121" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.45">
@@ -5270,33 +5284,33 @@
         <v>26</v>
       </c>
       <c r="B122" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C122" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D122">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E122" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_4</v>
+        <f t="shared" si="81"/>
+        <v>digit_3</v>
       </c>
       <c r="F122" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_06</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0D</v>
       </c>
       <c r="G122" t="str">
-        <f t="shared" si="81"/>
-        <v>SetTime-KEY_06-digit_4.png</v>
+        <f t="shared" si="83"/>
+        <v>SetTime-KEY_0D-digit_3.png</v>
       </c>
       <c r="H122" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_4</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I122" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.45">
@@ -5304,33 +5318,33 @@
         <v>26</v>
       </c>
       <c r="B123" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C123" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D123">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E123" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_5</v>
+        <f t="shared" si="81"/>
+        <v>digit_4</v>
       </c>
       <c r="F123" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_07</v>
+        <f t="shared" si="82"/>
+        <v>KEY_06</v>
       </c>
       <c r="G123" t="str">
-        <f t="shared" si="81"/>
-        <v>SetTime-KEY_07-digit_5.png</v>
+        <f t="shared" si="83"/>
+        <v>SetTime-KEY_06-digit_4.png</v>
       </c>
       <c r="H123" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_5</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I123" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.45">
@@ -5338,33 +5352,33 @@
         <v>26</v>
       </c>
       <c r="B124" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C124" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D124">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E124" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_6</v>
+        <f t="shared" si="81"/>
+        <v>digit_5</v>
       </c>
       <c r="F124" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_08</v>
+        <f t="shared" si="82"/>
+        <v>KEY_07</v>
       </c>
       <c r="G124" t="str">
-        <f t="shared" si="81"/>
-        <v>SetTime-KEY_08-digit_6.png</v>
+        <f t="shared" si="83"/>
+        <v>SetTime-KEY_07-digit_5.png</v>
       </c>
       <c r="H124" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_6</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_5</v>
       </c>
       <c r="I124" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.45">
@@ -5372,33 +5386,33 @@
         <v>26</v>
       </c>
       <c r="B125" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C125" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D125">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E125" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_7</v>
+        <f t="shared" si="81"/>
+        <v>digit_6</v>
       </c>
       <c r="F125" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_01</v>
+        <f t="shared" si="82"/>
+        <v>KEY_08</v>
       </c>
       <c r="G125" t="str">
-        <f t="shared" si="81"/>
-        <v>SetTime-KEY_01-digit_7.png</v>
+        <f t="shared" si="83"/>
+        <v>SetTime-KEY_08-digit_6.png</v>
       </c>
       <c r="H125" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_7</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_6</v>
       </c>
       <c r="I125" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.45">
@@ -5406,33 +5420,33 @@
         <v>26</v>
       </c>
       <c r="B126" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C126" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D126">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E126" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_8</v>
+        <f t="shared" si="81"/>
+        <v>digit_7</v>
       </c>
       <c r="F126" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_02</v>
+        <f t="shared" si="82"/>
+        <v>KEY_01</v>
       </c>
       <c r="G126" t="str">
-        <f t="shared" si="81"/>
-        <v>SetTime-KEY_02-digit_8.png</v>
+        <f t="shared" si="83"/>
+        <v>SetTime-KEY_01-digit_7.png</v>
       </c>
       <c r="H126" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_8</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_7</v>
       </c>
       <c r="I126" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.45">
@@ -5440,33 +5454,33 @@
         <v>26</v>
       </c>
       <c r="B127" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C127" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D127">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E127" t="str">
-        <f t="shared" si="79"/>
-        <v>digit_9</v>
+        <f t="shared" si="81"/>
+        <v>digit_8</v>
       </c>
       <c r="F127" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_03</v>
+        <f t="shared" si="82"/>
+        <v>KEY_02</v>
       </c>
       <c r="G127" t="str">
-        <f t="shared" si="81"/>
-        <v>SetTime-KEY_03-digit_9.png</v>
+        <f t="shared" si="83"/>
+        <v>SetTime-KEY_02-digit_8.png</v>
       </c>
       <c r="H127" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_9</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_8</v>
       </c>
       <c r="I127" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.45">
@@ -5474,33 +5488,33 @@
         <v>26</v>
       </c>
       <c r="B128" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C128" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D128">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E128" t="str">
-        <f t="shared" si="79"/>
-        <v>back_space</v>
+        <f t="shared" si="81"/>
+        <v>digit_9</v>
       </c>
       <c r="F128" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_05</v>
+        <f t="shared" si="82"/>
+        <v>KEY_03</v>
       </c>
       <c r="G128" t="str">
-        <f t="shared" si="81"/>
-        <v>SetTime-KEY_05-back_space.png</v>
+        <f t="shared" si="83"/>
+        <v>SetTime-KEY_03-digit_9.png</v>
       </c>
       <c r="H128" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_BACKSPACE</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_9</v>
       </c>
       <c r="I128" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.45">
@@ -5508,33 +5522,33 @@
         <v>26</v>
       </c>
       <c r="B129" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C129" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D129">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E129" t="str">
-        <f t="shared" si="79"/>
-        <v>enter</v>
+        <f t="shared" si="81"/>
+        <v>back_space</v>
       </c>
       <c r="F129" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_0E</v>
+        <f t="shared" si="82"/>
+        <v>KEY_05</v>
       </c>
       <c r="G129" t="str">
-        <f t="shared" si="81"/>
-        <v>SetTime-KEY_0E-enter.png</v>
+        <f t="shared" si="83"/>
+        <v>SetTime-KEY_05-back_space.png</v>
       </c>
       <c r="H129" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_ENTER</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_BACKSPACE</v>
       </c>
       <c r="I129" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.45">
@@ -5542,53 +5556,87 @@
         <v>26</v>
       </c>
       <c r="B130" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C130" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D130">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E130" t="str">
-        <f t="shared" si="79"/>
-        <v>jump_next</v>
+        <f t="shared" si="81"/>
+        <v>enter</v>
       </c>
       <c r="F130" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_09</v>
+        <f t="shared" si="82"/>
+        <v>KEY_0E</v>
       </c>
       <c r="G130" t="str">
-        <f t="shared" si="81"/>
-        <v>SetTime-KEY_09-jump_next.png</v>
+        <f t="shared" si="83"/>
+        <v>SetTime-KEY_0E-enter.png</v>
       </c>
       <c r="H130" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_TAB</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_ENTER</v>
       </c>
       <c r="I130" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
+        <v>26</v>
+      </c>
+      <c r="B131" t="s">
+        <v>75</v>
+      </c>
+      <c r="C131" t="s">
+        <v>148</v>
+      </c>
+      <c r="D131">
+        <v>9</v>
+      </c>
+      <c r="E131" t="str">
+        <f t="shared" si="81"/>
+        <v>jump_next</v>
+      </c>
+      <c r="F131" t="str">
+        <f t="shared" si="82"/>
+        <v>KEY_09</v>
+      </c>
+      <c r="G131" t="str">
+        <f t="shared" si="83"/>
+        <v>SetTime-KEY_09-jump_next.png</v>
+      </c>
+      <c r="H131" t="str">
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_TAB</v>
+      </c>
+      <c r="I131" t="str">
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A132" t="s">
         <v>30</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B132" t="s">
         <v>100</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C132" t="s">
         <v>151</v>
       </c>
-      <c r="D131">
+      <c r="D132">
         <v>0</v>
       </c>
-      <c r="E131" t="str">
-        <f t="shared" ref="E131" si="109">LOWER(
+      <c r="E132" t="str">
+        <f t="shared" ref="E132" si="111">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B131, FIND(" = InputEventMap", B131) - 1),
+      LEFT(B132, FIND(" = InputEventMap", B132) - 1),
       CHAR(160),
       " "
     )
@@ -5596,58 +5644,24 @@
 )</f>
         <v>screen</v>
       </c>
-      <c r="F131" t="str">
-        <f t="shared" ref="F131" si="110">"KEY_" &amp; CHOOSE(
-    D131+1,
+      <c r="F132" t="str">
+        <f t="shared" ref="F132" si="112">"KEY_" &amp; CHOOSE(
+    D132+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G131" t="str">
-        <f t="shared" ref="G131" si="111">_xlfn.CONCAT(A131, "-", F131, "-", E131, ".png")</f>
+      <c r="G132" t="str">
+        <f t="shared" ref="G132" si="113">_xlfn.CONCAT(A132, "-", F132, "-", E132, ".png")</f>
         <v>StorageManagement-KEY_00-screen.png</v>
       </c>
-      <c r="H131" t="str">
-        <f t="shared" ref="H131" si="112">MID(B131, FIND("InputEventMap", B131), LEN(B131))</f>
+      <c r="H132" t="str">
+        <f t="shared" ref="H132" si="114">MID(B132, FIND("InputEventMap", B132), LEN(B132))</f>
         <v>InputEventMap.KEY_ASTERISK</v>
       </c>
-      <c r="I131" t="str">
-        <f t="shared" ref="I131" si="113">_xlfn.CONCAT("StreamdeckInput.", F131, ": ", H131, ",")</f>
+      <c r="I132" t="str">
+        <f t="shared" ref="I132" si="115">_xlfn.CONCAT("StreamdeckInput.", F132, ": ", H132, ",")</f>
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A132" t="s">
-        <v>30</v>
-      </c>
-      <c r="B132" t="s">
-        <v>4</v>
-      </c>
-      <c r="C132" t="s">
-        <v>89</v>
-      </c>
-      <c r="D132">
-        <v>4</v>
-      </c>
-      <c r="E132" t="str">
-        <f t="shared" si="79"/>
-        <v>help</v>
-      </c>
-      <c r="F132" t="str">
-        <f t="shared" si="80"/>
-        <v>KEY_04</v>
-      </c>
-      <c r="G132" t="str">
-        <f t="shared" si="81"/>
-        <v>StorageManagement-KEY_04-help.png</v>
-      </c>
-      <c r="H132" t="str">
-        <f t="shared" si="82"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
-      </c>
-      <c r="I132" t="str">
-        <f t="shared" si="83"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.45">
@@ -5655,19 +5669,53 @@
         <v>30</v>
       </c>
       <c r="B133" t="s">
+        <v>4</v>
+      </c>
+      <c r="C133" t="s">
+        <v>89</v>
+      </c>
+      <c r="D133">
+        <v>4</v>
+      </c>
+      <c r="E133" t="str">
+        <f t="shared" si="81"/>
+        <v>help</v>
+      </c>
+      <c r="F133" t="str">
+        <f t="shared" si="82"/>
+        <v>KEY_04</v>
+      </c>
+      <c r="G133" t="str">
+        <f t="shared" si="83"/>
+        <v>StorageManagement-KEY_04-help.png</v>
+      </c>
+      <c r="H133" t="str">
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
+      </c>
+      <c r="I133" t="str">
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A134" t="s">
+        <v>30</v>
+      </c>
+      <c r="B134" t="s">
         <v>5</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C134" t="s">
         <v>90</v>
       </c>
-      <c r="D133">
+      <c r="D134">
         <v>9</v>
       </c>
-      <c r="E133" t="str">
-        <f t="shared" ref="E133:E148" si="114">LOWER(
+      <c r="E134" t="str">
+        <f t="shared" ref="E134:E149" si="116">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B133, FIND(" = InputEventMap", B133) - 1),
+      LEFT(B134, FIND(" = InputEventMap", B134) - 1),
       CHAR(160),
       " "
     )
@@ -5675,58 +5723,24 @@
 )</f>
         <v>menu</v>
       </c>
-      <c r="F133" t="str">
-        <f t="shared" ref="F133:F148" si="115">"KEY_" &amp; CHOOSE(
-    D133+1,
+      <c r="F134" t="str">
+        <f t="shared" ref="F134:F149" si="117">"KEY_" &amp; CHOOSE(
+    D134+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_09</v>
       </c>
-      <c r="G133" t="str">
-        <f t="shared" ref="G133:G148" si="116">_xlfn.CONCAT(A133, "-", F133, "-", E133, ".png")</f>
+      <c r="G134" t="str">
+        <f t="shared" ref="G134:G149" si="118">_xlfn.CONCAT(A134, "-", F134, "-", E134, ".png")</f>
         <v>StorageManagement-KEY_09-menu.png</v>
       </c>
-      <c r="H133" t="str">
-        <f t="shared" ref="H133:H148" si="117">MID(B133, FIND("InputEventMap", B133), LEN(B133))</f>
+      <c r="H134" t="str">
+        <f t="shared" ref="H134:H149" si="119">MID(B134, FIND("InputEventMap", B134), LEN(B134))</f>
         <v>InputEventMap.KEY_5</v>
       </c>
-      <c r="I133" t="str">
-        <f t="shared" ref="I133:I148" si="118">_xlfn.CONCAT("StreamdeckInput.", F133, ": ", H133, ",")</f>
+      <c r="I134" t="str">
+        <f t="shared" ref="I134:I149" si="120">_xlfn.CONCAT("StreamdeckInput.", F134, ": ", H134, ",")</f>
         <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A134" t="s">
-        <v>30</v>
-      </c>
-      <c r="B134" t="s">
-        <v>76</v>
-      </c>
-      <c r="C134" t="s">
-        <v>152</v>
-      </c>
-      <c r="D134">
-        <v>5</v>
-      </c>
-      <c r="E134" t="str">
-        <f t="shared" si="114"/>
-        <v>disconnect_storage</v>
-      </c>
-      <c r="F134" t="str">
-        <f t="shared" si="115"/>
-        <v>KEY_05</v>
-      </c>
-      <c r="G134" t="str">
-        <f t="shared" si="116"/>
-        <v>StorageManagement-KEY_05-disconnect_storage.png</v>
-      </c>
-      <c r="H134" t="str">
-        <f t="shared" si="117"/>
-        <v>InputEventMap.KEY_0</v>
-      </c>
-      <c r="I134" t="str">
-        <f t="shared" si="118"/>
-        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_0,</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.45">
@@ -5734,33 +5748,33 @@
         <v>30</v>
       </c>
       <c r="B135" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C135" t="s">
-        <v>93</v>
+        <v>152</v>
       </c>
       <c r="D135">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E135" t="str">
-        <f t="shared" si="114"/>
-        <v>detect_rc1</v>
+        <f t="shared" si="116"/>
+        <v>disconnect_storage</v>
       </c>
       <c r="F135" t="str">
-        <f t="shared" si="115"/>
-        <v>KEY_01</v>
+        <f t="shared" si="117"/>
+        <v>KEY_05</v>
       </c>
       <c r="G135" t="str">
-        <f t="shared" si="116"/>
-        <v>StorageManagement-KEY_01-detect_rc1.png</v>
+        <f t="shared" si="118"/>
+        <v>StorageManagement-KEY_05-disconnect_storage.png</v>
       </c>
       <c r="H135" t="str">
-        <f t="shared" si="117"/>
-        <v>InputEventMap.KEY_1</v>
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_0</v>
       </c>
       <c r="I135" t="str">
-        <f t="shared" si="118"/>
-        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_1,</v>
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_0,</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.45">
@@ -5768,33 +5782,33 @@
         <v>30</v>
       </c>
       <c r="B136" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C136" t="s">
         <v>93</v>
       </c>
       <c r="D136">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E136" t="str">
-        <f t="shared" si="114"/>
-        <v>detect_rc2</v>
+        <f t="shared" si="116"/>
+        <v>detect_rc1</v>
       </c>
       <c r="F136" t="str">
-        <f t="shared" si="115"/>
-        <v>KEY_02</v>
+        <f t="shared" si="117"/>
+        <v>KEY_01</v>
       </c>
       <c r="G136" t="str">
-        <f t="shared" si="116"/>
-        <v>StorageManagement-KEY_02-detect_rc2.png</v>
+        <f t="shared" si="118"/>
+        <v>StorageManagement-KEY_01-detect_rc1.png</v>
       </c>
       <c r="H136" t="str">
-        <f t="shared" si="117"/>
-        <v>InputEventMap.KEY_3</v>
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I136" t="str">
-        <f t="shared" si="118"/>
-        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_3,</v>
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_1,</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.45">
@@ -5802,33 +5816,33 @@
         <v>30</v>
       </c>
       <c r="B137" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C137" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D137">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E137" t="str">
-        <f t="shared" si="114"/>
-        <v>format_rc1</v>
+        <f t="shared" si="116"/>
+        <v>detect_rc2</v>
       </c>
       <c r="F137" t="str">
-        <f t="shared" si="115"/>
-        <v>KEY_06</v>
+        <f t="shared" si="117"/>
+        <v>KEY_02</v>
       </c>
       <c r="G137" t="str">
-        <f t="shared" si="116"/>
-        <v>StorageManagement-KEY_06-format_rc1.png</v>
+        <f t="shared" si="118"/>
+        <v>StorageManagement-KEY_02-detect_rc2.png</v>
       </c>
       <c r="H137" t="str">
-        <f t="shared" si="117"/>
-        <v>InputEventMap.KEY_4</v>
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I137" t="str">
-        <f t="shared" si="118"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_3,</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.45">
@@ -5836,33 +5850,33 @@
         <v>30</v>
       </c>
       <c r="B138" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C138" t="s">
         <v>94</v>
       </c>
       <c r="D138">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E138" t="str">
-        <f t="shared" si="114"/>
-        <v>format_rc2</v>
+        <f t="shared" si="116"/>
+        <v>format_rc1</v>
       </c>
       <c r="F138" t="str">
-        <f t="shared" si="115"/>
-        <v>KEY_07</v>
+        <f t="shared" si="117"/>
+        <v>KEY_06</v>
       </c>
       <c r="G138" t="str">
-        <f t="shared" si="116"/>
-        <v>StorageManagement-KEY_07-format_rc2.png</v>
+        <f t="shared" si="118"/>
+        <v>StorageManagement-KEY_06-format_rc1.png</v>
       </c>
       <c r="H138" t="str">
-        <f t="shared" si="117"/>
-        <v>InputEventMap.KEY_6</v>
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I138" t="str">
-        <f t="shared" si="118"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_6,</v>
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.45">
@@ -5870,33 +5884,33 @@
         <v>30</v>
       </c>
       <c r="B139" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C139" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D139">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E139" t="str">
-        <f t="shared" si="114"/>
-        <v>clean_rc1</v>
+        <f t="shared" si="116"/>
+        <v>format_rc2</v>
       </c>
       <c r="F139" t="str">
-        <f t="shared" si="115"/>
-        <v>KEY_0B</v>
+        <f t="shared" si="117"/>
+        <v>KEY_07</v>
       </c>
       <c r="G139" t="str">
-        <f t="shared" si="116"/>
-        <v>StorageManagement-KEY_0B-clean_rc1.png</v>
+        <f t="shared" si="118"/>
+        <v>StorageManagement-KEY_07-format_rc2.png</v>
       </c>
       <c r="H139" t="str">
-        <f t="shared" si="117"/>
-        <v>InputEventMap.KEY_7</v>
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_6</v>
       </c>
       <c r="I139" t="str">
-        <f t="shared" si="118"/>
-        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_7,</v>
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_6,</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.45">
@@ -5904,53 +5918,87 @@
         <v>30</v>
       </c>
       <c r="B140" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C140" t="s">
         <v>97</v>
       </c>
       <c r="D140">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E140" t="str">
-        <f t="shared" si="114"/>
-        <v>clean_rc2</v>
+        <f t="shared" si="116"/>
+        <v>clean_rc1</v>
       </c>
       <c r="F140" t="str">
-        <f t="shared" si="115"/>
-        <v>KEY_0C</v>
+        <f t="shared" si="117"/>
+        <v>KEY_0B</v>
       </c>
       <c r="G140" t="str">
-        <f t="shared" si="116"/>
-        <v>StorageManagement-KEY_0C-clean_rc2.png</v>
+        <f t="shared" si="118"/>
+        <v>StorageManagement-KEY_0B-clean_rc1.png</v>
       </c>
       <c r="H140" t="str">
-        <f t="shared" si="117"/>
-        <v>InputEventMap.KEY_9</v>
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_7</v>
       </c>
       <c r="I140" t="str">
-        <f t="shared" si="118"/>
-        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_9,</v>
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_7,</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
+        <v>30</v>
+      </c>
+      <c r="B141" t="s">
+        <v>82</v>
+      </c>
+      <c r="C141" t="s">
+        <v>97</v>
+      </c>
+      <c r="D141">
+        <v>12</v>
+      </c>
+      <c r="E141" t="str">
+        <f t="shared" si="116"/>
+        <v>clean_rc2</v>
+      </c>
+      <c r="F141" t="str">
+        <f t="shared" si="117"/>
+        <v>KEY_0C</v>
+      </c>
+      <c r="G141" t="str">
+        <f t="shared" si="118"/>
+        <v>StorageManagement-KEY_0C-clean_rc2.png</v>
+      </c>
+      <c r="H141" t="str">
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_9</v>
+      </c>
+      <c r="I141" t="str">
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_9,</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A142" t="s">
         <v>8</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B142" t="s">
         <v>100</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C142" t="s">
         <v>153</v>
       </c>
-      <c r="D141">
+      <c r="D142">
         <v>0</v>
       </c>
-      <c r="E141" t="str">
-        <f t="shared" ref="E141" si="119">LOWER(
+      <c r="E142" t="str">
+        <f t="shared" ref="E142" si="121">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B141, FIND(" = InputEventMap", B141) - 1),
+      LEFT(B142, FIND(" = InputEventMap", B142) - 1),
       CHAR(160),
       " "
     )
@@ -5958,58 +6006,24 @@
 )</f>
         <v>screen</v>
       </c>
-      <c r="F141" t="str">
-        <f t="shared" ref="F141" si="120">"KEY_" &amp; CHOOSE(
-    D141+1,
+      <c r="F142" t="str">
+        <f t="shared" ref="F142" si="122">"KEY_" &amp; CHOOSE(
+    D142+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G141" t="str">
-        <f t="shared" ref="G141" si="121">_xlfn.CONCAT(A141, "-", F141, "-", E141, ".png")</f>
+      <c r="G142" t="str">
+        <f t="shared" ref="G142" si="123">_xlfn.CONCAT(A142, "-", F142, "-", E142, ".png")</f>
         <v>System-KEY_00-screen.png</v>
       </c>
-      <c r="H141" t="str">
-        <f t="shared" ref="H141" si="122">MID(B141, FIND("InputEventMap", B141), LEN(B141))</f>
+      <c r="H142" t="str">
+        <f t="shared" ref="H142" si="124">MID(B142, FIND("InputEventMap", B142), LEN(B142))</f>
         <v>InputEventMap.KEY_ASTERISK</v>
       </c>
-      <c r="I141" t="str">
-        <f t="shared" ref="I141" si="123">_xlfn.CONCAT("StreamdeckInput.", F141, ": ", H141, ",")</f>
+      <c r="I142" t="str">
+        <f t="shared" ref="I142" si="125">_xlfn.CONCAT("StreamdeckInput.", F142, ": ", H142, ",")</f>
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A142" t="s">
-        <v>8</v>
-      </c>
-      <c r="B142" t="s">
-        <v>4</v>
-      </c>
-      <c r="C142" t="s">
-        <v>89</v>
-      </c>
-      <c r="D142">
-        <v>4</v>
-      </c>
-      <c r="E142" t="str">
-        <f t="shared" si="114"/>
-        <v>help</v>
-      </c>
-      <c r="F142" t="str">
-        <f t="shared" si="115"/>
-        <v>KEY_04</v>
-      </c>
-      <c r="G142" t="str">
-        <f t="shared" si="116"/>
-        <v>System-KEY_04-help.png</v>
-      </c>
-      <c r="H142" t="str">
-        <f t="shared" si="117"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
-      </c>
-      <c r="I142" t="str">
-        <f t="shared" si="118"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.45">
@@ -6017,33 +6031,33 @@
         <v>8</v>
       </c>
       <c r="B143" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
       <c r="C143" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D143">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E143" t="str">
-        <f t="shared" si="114"/>
-        <v>select_main</v>
+        <f t="shared" si="116"/>
+        <v>help</v>
       </c>
       <c r="F143" t="str">
-        <f t="shared" si="115"/>
-        <v>KEY_09</v>
+        <f t="shared" si="117"/>
+        <v>KEY_04</v>
       </c>
       <c r="G143" t="str">
-        <f t="shared" si="116"/>
-        <v>System-KEY_09-select_main.png</v>
+        <f t="shared" si="118"/>
+        <v>System-KEY_04-help.png</v>
       </c>
       <c r="H143" t="str">
-        <f t="shared" si="117"/>
-        <v>InputEventMap.KEY_1</v>
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
       </c>
       <c r="I143" t="str">
-        <f t="shared" si="118"/>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_1,</v>
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.45">
@@ -6051,33 +6065,33 @@
         <v>8</v>
       </c>
       <c r="B144" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C144" t="s">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="D144">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E144" t="str">
-        <f t="shared" si="114"/>
-        <v>select_language</v>
+        <f t="shared" si="116"/>
+        <v>select_main</v>
       </c>
       <c r="F144" t="str">
-        <f t="shared" si="115"/>
-        <v>KEY_06</v>
+        <f t="shared" si="117"/>
+        <v>KEY_09</v>
       </c>
       <c r="G144" t="str">
-        <f t="shared" si="116"/>
-        <v>System-KEY_06-select_language.png</v>
+        <f t="shared" si="118"/>
+        <v>System-KEY_09-select_main.png</v>
       </c>
       <c r="H144" t="str">
-        <f t="shared" si="117"/>
-        <v>InputEventMap.KEY_2</v>
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I144" t="str">
-        <f t="shared" si="118"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_1,</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.45">
@@ -6085,33 +6099,33 @@
         <v>8</v>
       </c>
       <c r="B145" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C145" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D145">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E145" t="str">
-        <f t="shared" si="114"/>
-        <v>select_storage</v>
+        <f t="shared" si="116"/>
+        <v>select_language</v>
       </c>
       <c r="F145" t="str">
-        <f t="shared" si="115"/>
-        <v>KEY_07</v>
+        <f t="shared" si="117"/>
+        <v>KEY_06</v>
       </c>
       <c r="G145" t="str">
-        <f t="shared" si="116"/>
-        <v>System-KEY_07-select_storage.png</v>
+        <f t="shared" si="118"/>
+        <v>System-KEY_06-select_language.png</v>
       </c>
       <c r="H145" t="str">
-        <f t="shared" si="117"/>
-        <v>InputEventMap.KEY_3</v>
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I145" t="str">
-        <f t="shared" si="118"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.45">
@@ -6119,33 +6133,33 @@
         <v>8</v>
       </c>
       <c r="B146" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C146" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D146">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E146" t="str">
-        <f t="shared" si="114"/>
-        <v>set_date</v>
+        <f t="shared" si="116"/>
+        <v>select_storage</v>
       </c>
       <c r="F146" t="str">
-        <f t="shared" si="115"/>
-        <v>KEY_0B</v>
+        <f t="shared" si="117"/>
+        <v>KEY_07</v>
       </c>
       <c r="G146" t="str">
-        <f t="shared" si="116"/>
-        <v>System-KEY_0B-set_date.png</v>
+        <f t="shared" si="118"/>
+        <v>System-KEY_07-select_storage.png</v>
       </c>
       <c r="H146" t="str">
-        <f t="shared" si="117"/>
-        <v>InputEventMap.KEY_4</v>
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I146" t="str">
-        <f t="shared" si="118"/>
-        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_4,</v>
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.45">
@@ -6153,33 +6167,33 @@
         <v>8</v>
       </c>
       <c r="B147" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C147" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D147">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E147" t="str">
-        <f t="shared" si="114"/>
-        <v>set_time</v>
+        <f t="shared" si="116"/>
+        <v>set_date</v>
       </c>
       <c r="F147" t="str">
-        <f t="shared" si="115"/>
-        <v>KEY_0C</v>
+        <f t="shared" si="117"/>
+        <v>KEY_0B</v>
       </c>
       <c r="G147" t="str">
-        <f t="shared" si="116"/>
-        <v>System-KEY_0C-set_time.png</v>
+        <f t="shared" si="118"/>
+        <v>System-KEY_0B-set_date.png</v>
       </c>
       <c r="H147" t="str">
-        <f t="shared" si="117"/>
-        <v>InputEventMap.KEY_6</v>
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I147" t="str">
-        <f t="shared" si="118"/>
-        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_6,</v>
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_4,</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.45">
@@ -6187,37 +6201,71 @@
         <v>8</v>
       </c>
       <c r="B148" t="s">
+        <v>87</v>
+      </c>
+      <c r="C148" t="s">
+        <v>157</v>
+      </c>
+      <c r="D148">
+        <v>12</v>
+      </c>
+      <c r="E148" t="str">
+        <f t="shared" si="116"/>
+        <v>set_time</v>
+      </c>
+      <c r="F148" t="str">
+        <f t="shared" si="117"/>
+        <v>KEY_0C</v>
+      </c>
+      <c r="G148" t="str">
+        <f t="shared" si="118"/>
+        <v>System-KEY_0C-set_time.png</v>
+      </c>
+      <c r="H148" t="str">
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_6</v>
+      </c>
+      <c r="I148" t="str">
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_6,</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A149" t="s">
+        <v>8</v>
+      </c>
+      <c r="B149" t="s">
         <v>45</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C149" t="s">
         <v>104</v>
       </c>
-      <c r="D148">
+      <c r="D149">
         <v>14</v>
       </c>
-      <c r="E148" t="str">
-        <f t="shared" si="114"/>
+      <c r="E149" t="str">
+        <f t="shared" si="116"/>
         <v>stop_system</v>
       </c>
-      <c r="F148" t="str">
-        <f t="shared" si="115"/>
+      <c r="F149" t="str">
+        <f t="shared" si="117"/>
         <v>KEY_0E</v>
       </c>
-      <c r="G148" t="str">
-        <f t="shared" si="116"/>
+      <c r="G149" t="str">
+        <f t="shared" si="118"/>
         <v>System-KEY_0E-stop_system.png</v>
       </c>
-      <c r="H148" t="str">
-        <f t="shared" si="117"/>
+      <c r="H149" t="str">
+        <f t="shared" si="119"/>
         <v>InputEventMap.KEY_9</v>
       </c>
-      <c r="I148" t="str">
-        <f t="shared" si="118"/>
+      <c r="I149" t="str">
+        <f t="shared" si="120"/>
         <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_9,</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I148" xr:uid="{47861C0B-96C3-4FC0-B828-7FD785B358D7}"/>
+  <autoFilter ref="A1:I149" xr:uid="{47861C0B-96C3-4FC0-B828-7FD785B358D7}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Menu SetDate, SetTime, SetName
* KEY_09: remove TAB
* KEY_05 - > KEY_09: change BACKSPACE key
* update xlsx
* update event map
</commit_message>
<xml_diff>
--- a/prep/StreamdeckIconInputKeyMapping.xlsx
+++ b/prep/StreamdeckIconInputKeyMapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irene\src\biz.dfch.PhoneTap\prep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\biz.dfch.PhoneTap\prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325AE261-9970-4833-9C9B-69C5B4FDEBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2311B48B-77F7-4AD1-8A76-8C00CEFE9440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{4419FAFA-D280-4090-97B7-CB07F6B7BE60}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$149</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$146</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="157">
   <si>
     <t>States</t>
   </si>
@@ -266,9 +266,6 @@
     <t>        ENTER = InputEventMap.KEY_ENTER</t>
   </si>
   <si>
-    <t>        JUMP_NEXT = InputEventMap.KEY_TAB</t>
-  </si>
-  <si>
     <t>        DISCONNECT_STORAGE = InputEventMap.KEY_0</t>
   </si>
   <si>
@@ -483,9 +480,6 @@
   </si>
   <si>
     <t>ic_fluent_arrow_enter_left_24_regular.png</t>
-  </si>
-  <si>
-    <t>ic_fluent_keyboard_tab_24_regular.png</t>
   </si>
   <si>
     <t>ic_fluent_text_edit_style_character_a_32_regular_pink.png</t>
@@ -522,7 +516,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -902,25 +896,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47861C0B-96C3-4FC0-B828-7FD785B358D7}">
-  <dimension ref="A1:I149"/>
+  <dimension ref="A1:I146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C38" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.1328125" customWidth="1"/>
-    <col min="6" max="6" width="17.9296875" customWidth="1"/>
-    <col min="7" max="7" width="22.53125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="45.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.125" customWidth="1"/>
+    <col min="6" max="6" width="17.9375" customWidth="1"/>
+    <col min="7" max="7" width="22.5625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.3125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.8125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="13.9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -949,15 +943,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -994,7 +988,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1002,7 +996,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -1039,7 +1033,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1047,7 +1041,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D4">
         <v>9</v>
@@ -1076,15 +1070,15 @@
         <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" t="s">
         <v>100</v>
-      </c>
-      <c r="C5" t="s">
-        <v>101</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1121,7 +1115,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1129,7 +1123,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1155,7 +1149,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1163,7 +1157,7 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1189,7 +1183,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1197,7 +1191,7 @@
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1223,15 +1217,15 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1268,7 +1262,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1276,7 +1270,7 @@
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -1302,7 +1296,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1310,7 +1304,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -1336,7 +1330,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1344,7 +1338,7 @@
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -1370,15 +1364,15 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1415,7 +1409,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1423,7 +1417,7 @@
         <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -1449,7 +1443,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1457,7 +1451,7 @@
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -1483,7 +1477,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1491,7 +1485,7 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D16">
         <v>6</v>
@@ -1517,15 +1511,15 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1562,7 +1556,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1570,7 +1564,7 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -1596,7 +1590,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1604,7 +1598,7 @@
         <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D19">
         <v>5</v>
@@ -1630,7 +1624,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1638,7 +1632,7 @@
         <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D20">
         <v>6</v>
@@ -1664,15 +1658,15 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1709,7 +1703,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1717,7 +1711,7 @@
         <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D22">
         <v>4</v>
@@ -1743,7 +1737,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1751,7 +1745,7 @@
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23">
         <v>5</v>
@@ -1777,7 +1771,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1785,7 +1779,7 @@
         <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D24">
         <v>6</v>
@@ -1811,15 +1805,15 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1856,7 +1850,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -1864,7 +1858,7 @@
         <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D26">
         <v>4</v>
@@ -1890,7 +1884,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1898,7 +1892,7 @@
         <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D27">
         <v>5</v>
@@ -1924,7 +1918,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -1932,7 +1926,7 @@
         <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D28">
         <v>6</v>
@@ -1958,15 +1952,15 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2003,7 +1997,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -2011,7 +2005,7 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30">
         <v>4</v>
@@ -2037,7 +2031,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -2045,7 +2039,7 @@
         <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D31">
         <v>5</v>
@@ -2071,7 +2065,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -2079,7 +2073,7 @@
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D32">
         <v>6</v>
@@ -2105,15 +2099,15 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2142,7 +2136,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -2150,7 +2144,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D34">
         <v>4</v>
@@ -2184,7 +2178,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -2192,7 +2186,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D35">
         <v>5</v>
@@ -2218,7 +2212,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -2226,7 +2220,7 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D36">
         <v>6</v>
@@ -2252,7 +2246,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -2260,7 +2254,7 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D37">
         <v>10</v>
@@ -2286,7 +2280,7 @@
         <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_6,</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -2294,7 +2288,7 @@
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D38">
         <v>11</v>
@@ -2320,7 +2314,7 @@
         <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_7,</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -2328,7 +2322,7 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D39">
         <v>12</v>
@@ -2354,7 +2348,7 @@
         <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_8,</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -2362,7 +2356,7 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D40">
         <v>13</v>
@@ -2388,15 +2382,15 @@
         <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_9,</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -2433,7 +2427,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -2441,7 +2435,7 @@
         <v>33</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D42">
         <v>4</v>
@@ -2467,7 +2461,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -2475,7 +2469,7 @@
         <v>34</v>
       </c>
       <c r="C43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D43">
         <v>5</v>
@@ -2509,7 +2503,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -2517,7 +2511,7 @@
         <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D44">
         <v>6</v>
@@ -2543,7 +2537,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -2551,7 +2545,7 @@
         <v>36</v>
       </c>
       <c r="C45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D45">
         <v>10</v>
@@ -2577,7 +2571,7 @@
         <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_6,</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -2585,7 +2579,7 @@
         <v>37</v>
       </c>
       <c r="C46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D46">
         <v>11</v>
@@ -2611,7 +2605,7 @@
         <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_7,</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -2619,7 +2613,7 @@
         <v>38</v>
       </c>
       <c r="C47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D47">
         <v>12</v>
@@ -2645,7 +2639,7 @@
         <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_8,</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -2653,7 +2647,7 @@
         <v>39</v>
       </c>
       <c r="C48" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D48">
         <v>13</v>
@@ -2679,15 +2673,15 @@
         <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_9,</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -2724,7 +2718,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -2732,7 +2726,7 @@
         <v>33</v>
       </c>
       <c r="C50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D50">
         <v>4</v>
@@ -2758,7 +2752,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -2766,7 +2760,7 @@
         <v>40</v>
       </c>
       <c r="C51" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D51">
         <v>5</v>
@@ -2800,7 +2794,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -2808,7 +2802,7 @@
         <v>41</v>
       </c>
       <c r="C52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D52">
         <v>6</v>
@@ -2834,7 +2828,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -2842,7 +2836,7 @@
         <v>42</v>
       </c>
       <c r="C53" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D53">
         <v>7</v>
@@ -2868,7 +2862,7 @@
         <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -2876,7 +2870,7 @@
         <v>43</v>
       </c>
       <c r="C54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D54">
         <v>10</v>
@@ -2902,7 +2896,7 @@
         <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_4,</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -2910,7 +2904,7 @@
         <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D55">
         <v>9</v>
@@ -2936,7 +2930,7 @@
         <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -2944,7 +2938,7 @@
         <v>44</v>
       </c>
       <c r="C56" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D56">
         <v>11</v>
@@ -2970,15 +2964,15 @@
         <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_6,</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C57" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D57">
         <v>12</v>
@@ -3015,7 +3009,7 @@
         <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_7,</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -3023,7 +3017,7 @@
         <v>45</v>
       </c>
       <c r="C58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D58">
         <v>14</v>
@@ -3049,15 +3043,15 @@
         <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_9,</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>18</v>
       </c>
       <c r="B59" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -3094,7 +3088,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>18</v>
       </c>
@@ -3102,7 +3096,7 @@
         <v>4</v>
       </c>
       <c r="C60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D60">
         <v>4</v>
@@ -3128,7 +3122,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -3136,7 +3130,7 @@
         <v>46</v>
       </c>
       <c r="C61" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D61">
         <v>6</v>
@@ -3173,7 +3167,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>18</v>
       </c>
@@ -3181,7 +3175,7 @@
         <v>47</v>
       </c>
       <c r="C62" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D62">
         <v>5</v>
@@ -3207,7 +3201,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
         <v>18</v>
       </c>
@@ -3215,7 +3209,7 @@
         <v>48</v>
       </c>
       <c r="C63" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D63">
         <v>7</v>
@@ -3241,7 +3235,7 @@
         <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9">
       <c r="A64" t="s">
         <v>18</v>
       </c>
@@ -3249,7 +3243,7 @@
         <v>49</v>
       </c>
       <c r="C64" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D64">
         <v>10</v>
@@ -3275,15 +3269,15 @@
         <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_4,</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9">
       <c r="A65" t="s">
         <v>29</v>
       </c>
       <c r="B65" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C65" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -3309,7 +3303,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9">
       <c r="A66" t="s">
         <v>29</v>
       </c>
@@ -3317,13 +3311,13 @@
         <v>4</v>
       </c>
       <c r="C66" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D66">
         <v>4</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" ref="E66:E133" si="81">LOWER(
+        <f t="shared" ref="E66:E130" si="81">LOWER(
   TRIM(
     SUBSTITUTE(
       LEFT(B66, FIND(" = InputEventMap", B66) - 1),
@@ -3335,26 +3329,26 @@
         <v>help</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" ref="F66:F133" si="82">"KEY_" &amp; CHOOSE(
+        <f t="shared" ref="F66:F130" si="82">"KEY_" &amp; CHOOSE(
     D66+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_04</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" ref="G66:G133" si="83">_xlfn.CONCAT(A66, "-", F66, "-", E66, ".png")</f>
+        <f t="shared" ref="G66:G130" si="83">_xlfn.CONCAT(A66, "-", F66, "-", E66, ".png")</f>
         <v>PlaybackPaused-KEY_04-help.png</v>
       </c>
       <c r="H66" t="str">
-        <f t="shared" ref="H66:H133" si="84">MID(B66, FIND("InputEventMap", B66), LEN(B66))</f>
+        <f t="shared" ref="H66:H130" si="84">MID(B66, FIND("InputEventMap", B66), LEN(B66))</f>
         <v>InputEventMap.KEY_ASTERISK</v>
       </c>
       <c r="I66" t="str">
-        <f t="shared" ref="I66:I133" si="85">_xlfn.CONCAT("StreamdeckInput.", F66, ": ", H66, ",")</f>
+        <f t="shared" ref="I66:I130" si="85">_xlfn.CONCAT("StreamdeckInput.", F66, ": ", H66, ",")</f>
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9">
       <c r="A67" t="s">
         <v>29</v>
       </c>
@@ -3362,7 +3356,7 @@
         <v>50</v>
       </c>
       <c r="C67" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D67">
         <v>7</v>
@@ -3388,7 +3382,7 @@
         <v>StreamdeckInput.KEY_07: InputEventMap.KEY_0,</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9">
       <c r="A68" t="s">
         <v>29</v>
       </c>
@@ -3396,7 +3390,7 @@
         <v>5</v>
       </c>
       <c r="C68" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D68">
         <v>9</v>
@@ -3422,15 +3416,15 @@
         <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9">
       <c r="A69" t="s">
         <v>28</v>
       </c>
       <c r="B69" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C69" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -3467,7 +3461,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9">
       <c r="A70" t="s">
         <v>28</v>
       </c>
@@ -3475,7 +3469,7 @@
         <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D70">
         <v>4</v>
@@ -3501,7 +3495,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -3509,7 +3503,7 @@
         <v>50</v>
       </c>
       <c r="C71" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D71">
         <v>7</v>
@@ -3535,7 +3529,7 @@
         <v>StreamdeckInput.KEY_07: InputEventMap.KEY_0,</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9">
       <c r="A72" t="s">
         <v>28</v>
       </c>
@@ -3543,7 +3537,7 @@
         <v>51</v>
       </c>
       <c r="C72" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D72">
         <v>11</v>
@@ -3569,7 +3563,7 @@
         <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9">
       <c r="A73" t="s">
         <v>28</v>
       </c>
@@ -3577,7 +3571,7 @@
         <v>52</v>
       </c>
       <c r="C73" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D73">
         <v>12</v>
@@ -3603,7 +3597,7 @@
         <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9">
       <c r="A74" t="s">
         <v>28</v>
       </c>
@@ -3611,7 +3605,7 @@
         <v>53</v>
       </c>
       <c r="C74" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D74">
         <v>13</v>
@@ -3637,7 +3631,7 @@
         <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9">
       <c r="A75" t="s">
         <v>28</v>
       </c>
@@ -3645,7 +3639,7 @@
         <v>54</v>
       </c>
       <c r="C75" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D75">
         <v>6</v>
@@ -3671,7 +3665,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9">
       <c r="A76" t="s">
         <v>28</v>
       </c>
@@ -3679,7 +3673,7 @@
         <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D76">
         <v>9</v>
@@ -3705,7 +3699,7 @@
         <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9">
       <c r="A77" t="s">
         <v>28</v>
       </c>
@@ -3713,7 +3707,7 @@
         <v>55</v>
       </c>
       <c r="C77" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D77">
         <v>8</v>
@@ -3739,7 +3733,7 @@
         <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9">
       <c r="A78" t="s">
         <v>28</v>
       </c>
@@ -3747,7 +3741,7 @@
         <v>56</v>
       </c>
       <c r="C78" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -3773,7 +3767,7 @@
         <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9">
       <c r="A79" t="s">
         <v>28</v>
       </c>
@@ -3781,7 +3775,7 @@
         <v>57</v>
       </c>
       <c r="C79" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D79">
         <v>2</v>
@@ -3807,7 +3801,7 @@
         <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9">
       <c r="A80" t="s">
         <v>28</v>
       </c>
@@ -3815,7 +3809,7 @@
         <v>58</v>
       </c>
       <c r="C80" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D80">
         <v>3</v>
@@ -3841,15 +3835,15 @@
         <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:9">
       <c r="A81" t="s">
         <v>24</v>
       </c>
       <c r="B81" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C81" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -3886,7 +3880,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:9">
       <c r="A82" t="s">
         <v>24</v>
       </c>
@@ -3894,7 +3888,7 @@
         <v>4</v>
       </c>
       <c r="C82" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D82">
         <v>4</v>
@@ -3920,7 +3914,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:9">
       <c r="A83" t="s">
         <v>24</v>
       </c>
@@ -3928,7 +3922,7 @@
         <v>59</v>
       </c>
       <c r="C83" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D83">
         <v>5</v>
@@ -3954,7 +3948,7 @@
         <v>StreamdeckInput.KEY_05: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:9">
       <c r="A84" t="s">
         <v>24</v>
       </c>
@@ -3962,7 +3956,7 @@
         <v>60</v>
       </c>
       <c r="C84" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D84">
         <v>6</v>
@@ -3988,7 +3982,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:9">
       <c r="A85" t="s">
         <v>24</v>
       </c>
@@ -3996,7 +3990,7 @@
         <v>61</v>
       </c>
       <c r="C85" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D85">
         <v>7</v>
@@ -4022,7 +4016,7 @@
         <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:9">
       <c r="A86" t="s">
         <v>24</v>
       </c>
@@ -4030,7 +4024,7 @@
         <v>62</v>
       </c>
       <c r="C86" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D86">
         <v>8</v>
@@ -4056,15 +4050,15 @@
         <v>StreamdeckInput.KEY_08: InputEventMap.KEY_4,</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:9">
       <c r="A87" t="s">
         <v>25</v>
       </c>
       <c r="B87" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C87" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -4101,7 +4095,7 @@
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:9">
       <c r="A88" t="s">
         <v>25</v>
       </c>
@@ -4109,7 +4103,7 @@
         <v>4</v>
       </c>
       <c r="C88" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D88">
         <v>4</v>
@@ -4135,7 +4129,7 @@
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:9">
       <c r="A89" t="s">
         <v>25</v>
       </c>
@@ -4143,7 +4137,7 @@
         <v>63</v>
       </c>
       <c r="C89" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D89">
         <v>10</v>
@@ -4169,7 +4163,7 @@
         <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:9">
       <c r="A90" t="s">
         <v>25</v>
       </c>
@@ -4177,7 +4171,7 @@
         <v>64</v>
       </c>
       <c r="C90" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D90">
         <v>11</v>
@@ -4203,7 +4197,7 @@
         <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:9">
       <c r="A91" t="s">
         <v>25</v>
       </c>
@@ -4211,7 +4205,7 @@
         <v>65</v>
       </c>
       <c r="C91" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D91">
         <v>12</v>
@@ -4237,7 +4231,7 @@
         <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:9">
       <c r="A92" t="s">
         <v>25</v>
       </c>
@@ -4245,7 +4239,7 @@
         <v>66</v>
       </c>
       <c r="C92" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D92">
         <v>13</v>
@@ -4271,7 +4265,7 @@
         <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:9">
       <c r="A93" t="s">
         <v>25</v>
       </c>
@@ -4279,7 +4273,7 @@
         <v>67</v>
       </c>
       <c r="C93" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D93">
         <v>6</v>
@@ -4305,7 +4299,7 @@
         <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:9">
       <c r="A94" t="s">
         <v>25</v>
       </c>
@@ -4313,7 +4307,7 @@
         <v>68</v>
       </c>
       <c r="C94" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D94">
         <v>7</v>
@@ -4339,7 +4333,7 @@
         <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:9">
       <c r="A95" t="s">
         <v>25</v>
       </c>
@@ -4347,7 +4341,7 @@
         <v>69</v>
       </c>
       <c r="C95" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D95">
         <v>8</v>
@@ -4373,7 +4367,7 @@
         <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:9">
       <c r="A96" t="s">
         <v>25</v>
       </c>
@@ -4381,7 +4375,7 @@
         <v>70</v>
       </c>
       <c r="C96" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -4407,7 +4401,7 @@
         <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:9">
       <c r="A97" t="s">
         <v>25</v>
       </c>
@@ -4415,7 +4409,7 @@
         <v>71</v>
       </c>
       <c r="C97" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D97">
         <v>2</v>
@@ -4441,7 +4435,7 @@
         <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:9">
       <c r="A98" t="s">
         <v>25</v>
       </c>
@@ -4449,7 +4443,7 @@
         <v>72</v>
       </c>
       <c r="C98" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D98">
         <v>3</v>
@@ -4475,7 +4469,7 @@
         <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:9">
       <c r="A99" t="s">
         <v>25</v>
       </c>
@@ -4483,10 +4477,10 @@
         <v>73</v>
       </c>
       <c r="C99" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D99">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E99" t="str">
         <f t="shared" si="81"/>
@@ -4494,11 +4488,11 @@
       </c>
       <c r="F99" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_05</v>
+        <v>KEY_09</v>
       </c>
       <c r="G99" t="str">
         <f t="shared" si="83"/>
-        <v>SetDate-KEY_05-back_space.png</v>
+        <v>SetDate-KEY_09-back_space.png</v>
       </c>
       <c r="H99" t="str">
         <f t="shared" si="84"/>
@@ -4506,10 +4500,10 @@
       </c>
       <c r="I99" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_BACKSPACE,</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
       <c r="A100" t="s">
         <v>25</v>
       </c>
@@ -4517,7 +4511,7 @@
         <v>74</v>
       </c>
       <c r="C100" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D100">
         <v>14</v>
@@ -4543,58 +4537,24 @@
         <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:9">
       <c r="A101" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B101" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="C101" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D101">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E101" t="str">
-        <f t="shared" si="81"/>
-        <v>jump_next</v>
-      </c>
-      <c r="F101" t="str">
-        <f t="shared" si="82"/>
-        <v>KEY_09</v>
-      </c>
-      <c r="G101" t="str">
-        <f t="shared" si="83"/>
-        <v>SetDate-KEY_09-jump_next.png</v>
-      </c>
-      <c r="H101" t="str">
-        <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_TAB</v>
-      </c>
-      <c r="I101" t="str">
-        <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A102" t="s">
-        <v>27</v>
-      </c>
-      <c r="B102" t="s">
-        <v>100</v>
-      </c>
-      <c r="C102" t="s">
-        <v>149</v>
-      </c>
-      <c r="D102">
-        <v>0</v>
-      </c>
-      <c r="E102" t="str">
-        <f t="shared" ref="E102" si="101">LOWER(
+        <f t="shared" ref="E101" si="101">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B102, FIND(" = InputEventMap", B102) - 1),
+      LEFT(B101, FIND(" = InputEventMap", B101) - 1),
       CHAR(160),
       " "
     )
@@ -4602,520 +4562,486 @@
 )</f>
         <v>screen</v>
       </c>
-      <c r="F102" t="str">
-        <f t="shared" ref="F102" si="102">"KEY_" &amp; CHOOSE(
-    D102+1,
+      <c r="F101" t="str">
+        <f t="shared" ref="F101" si="102">"KEY_" &amp; CHOOSE(
+    D101+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_00</v>
       </c>
+      <c r="G101" t="str">
+        <f t="shared" ref="G101" si="103">_xlfn.CONCAT(A101, "-", F101, "-", E101, ".png")</f>
+        <v>SetName-KEY_00-screen.png</v>
+      </c>
+      <c r="H101" t="str">
+        <f t="shared" ref="H101" si="104">MID(B101, FIND("InputEventMap", B101), LEN(B101))</f>
+        <v>InputEventMap.KEY_ASTERISK</v>
+      </c>
+      <c r="I101" t="str">
+        <f t="shared" ref="I101" si="105">_xlfn.CONCAT("StreamdeckInput.", F101, ": ", H101, ",")</f>
+        <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102" t="s">
+        <v>27</v>
+      </c>
+      <c r="B102" t="s">
+        <v>4</v>
+      </c>
+      <c r="C102" t="s">
+        <v>88</v>
+      </c>
+      <c r="D102">
+        <v>4</v>
+      </c>
+      <c r="E102" t="str">
+        <f t="shared" si="81"/>
+        <v>help</v>
+      </c>
+      <c r="F102" t="str">
+        <f t="shared" si="82"/>
+        <v>KEY_04</v>
+      </c>
       <c r="G102" t="str">
-        <f t="shared" ref="G102" si="103">_xlfn.CONCAT(A102, "-", F102, "-", E102, ".png")</f>
-        <v>SetName-KEY_00-screen.png</v>
+        <f t="shared" si="83"/>
+        <v>SetName-KEY_04-help.png</v>
       </c>
       <c r="H102" t="str">
-        <f t="shared" ref="H102" si="104">MID(B102, FIND("InputEventMap", B102), LEN(B102))</f>
+        <f t="shared" si="84"/>
         <v>InputEventMap.KEY_ASTERISK</v>
       </c>
       <c r="I102" t="str">
-        <f t="shared" ref="I102" si="105">_xlfn.CONCAT("StreamdeckInput.", F102, ": ", H102, ",")</f>
-        <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
       <c r="A103" t="s">
         <v>27</v>
       </c>
       <c r="B103" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="C103" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="D103">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E103" t="str">
         <f t="shared" si="81"/>
-        <v>help</v>
+        <v>digit_0</v>
       </c>
       <c r="F103" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_04</v>
+        <v>KEY_0A</v>
       </c>
       <c r="G103" t="str">
         <f t="shared" si="83"/>
-        <v>SetName-KEY_04-help.png</v>
+        <v>SetName-KEY_0A-digit_0.png</v>
       </c>
       <c r="H103" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
+        <v>InputEventMap.KEY_0</v>
       </c>
       <c r="I103" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
       <c r="A104" t="s">
         <v>27</v>
       </c>
       <c r="B104" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C104" t="s">
         <v>136</v>
       </c>
       <c r="D104">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E104" t="str">
         <f t="shared" si="81"/>
-        <v>digit_0</v>
+        <v>digit_1</v>
       </c>
       <c r="F104" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_0A</v>
+        <v>KEY_0B</v>
       </c>
       <c r="G104" t="str">
         <f t="shared" si="83"/>
-        <v>SetName-KEY_0A-digit_0.png</v>
+        <v>SetName-KEY_0B-digit_1.png</v>
       </c>
       <c r="H104" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_0</v>
+        <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I104" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
       <c r="A105" t="s">
         <v>27</v>
       </c>
       <c r="B105" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C105" t="s">
         <v>137</v>
       </c>
       <c r="D105">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E105" t="str">
         <f t="shared" si="81"/>
-        <v>digit_1</v>
+        <v>digit_2</v>
       </c>
       <c r="F105" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_0B</v>
+        <v>KEY_0C</v>
       </c>
       <c r="G105" t="str">
         <f t="shared" si="83"/>
-        <v>SetName-KEY_0B-digit_1.png</v>
+        <v>SetName-KEY_0C-digit_2.png</v>
       </c>
       <c r="H105" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_1</v>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I105" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
       <c r="A106" t="s">
         <v>27</v>
       </c>
       <c r="B106" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C106" t="s">
         <v>138</v>
       </c>
       <c r="D106">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E106" t="str">
         <f t="shared" si="81"/>
-        <v>digit_2</v>
+        <v>digit_3</v>
       </c>
       <c r="F106" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_0C</v>
+        <v>KEY_0D</v>
       </c>
       <c r="G106" t="str">
         <f t="shared" si="83"/>
-        <v>SetName-KEY_0C-digit_2.png</v>
+        <v>SetName-KEY_0D-digit_3.png</v>
       </c>
       <c r="H106" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_2</v>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I106" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
       <c r="A107" t="s">
         <v>27</v>
       </c>
       <c r="B107" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C107" t="s">
         <v>139</v>
       </c>
       <c r="D107">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E107" t="str">
         <f t="shared" si="81"/>
-        <v>digit_3</v>
+        <v>digit_4</v>
       </c>
       <c r="F107" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_0D</v>
+        <v>KEY_06</v>
       </c>
       <c r="G107" t="str">
         <f t="shared" si="83"/>
-        <v>SetName-KEY_0D-digit_3.png</v>
+        <v>SetName-KEY_06-digit_4.png</v>
       </c>
       <c r="H107" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_3</v>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I107" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
       <c r="A108" t="s">
         <v>27</v>
       </c>
       <c r="B108" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C108" t="s">
         <v>140</v>
       </c>
       <c r="D108">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E108" t="str">
         <f t="shared" si="81"/>
-        <v>digit_4</v>
+        <v>digit_5</v>
       </c>
       <c r="F108" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_06</v>
+        <v>KEY_07</v>
       </c>
       <c r="G108" t="str">
         <f t="shared" si="83"/>
-        <v>SetName-KEY_06-digit_4.png</v>
+        <v>SetName-KEY_07-digit_5.png</v>
       </c>
       <c r="H108" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_4</v>
+        <v>InputEventMap.KEY_5</v>
       </c>
       <c r="I108" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
       <c r="A109" t="s">
         <v>27</v>
       </c>
       <c r="B109" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C109" t="s">
         <v>141</v>
       </c>
       <c r="D109">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E109" t="str">
         <f t="shared" si="81"/>
-        <v>digit_5</v>
+        <v>digit_6</v>
       </c>
       <c r="F109" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_07</v>
+        <v>KEY_08</v>
       </c>
       <c r="G109" t="str">
         <f t="shared" si="83"/>
-        <v>SetName-KEY_07-digit_5.png</v>
+        <v>SetName-KEY_08-digit_6.png</v>
       </c>
       <c r="H109" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_5</v>
+        <v>InputEventMap.KEY_6</v>
       </c>
       <c r="I109" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
       <c r="A110" t="s">
         <v>27</v>
       </c>
       <c r="B110" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C110" t="s">
         <v>142</v>
       </c>
       <c r="D110">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E110" t="str">
         <f t="shared" si="81"/>
-        <v>digit_6</v>
+        <v>digit_7</v>
       </c>
       <c r="F110" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_08</v>
+        <v>KEY_01</v>
       </c>
       <c r="G110" t="str">
         <f t="shared" si="83"/>
-        <v>SetName-KEY_08-digit_6.png</v>
+        <v>SetName-KEY_01-digit_7.png</v>
       </c>
       <c r="H110" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_6</v>
+        <v>InputEventMap.KEY_7</v>
       </c>
       <c r="I110" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
       <c r="A111" t="s">
         <v>27</v>
       </c>
       <c r="B111" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C111" t="s">
         <v>143</v>
       </c>
       <c r="D111">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E111" t="str">
         <f t="shared" si="81"/>
-        <v>digit_7</v>
+        <v>digit_8</v>
       </c>
       <c r="F111" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_01</v>
+        <v>KEY_02</v>
       </c>
       <c r="G111" t="str">
         <f t="shared" si="83"/>
-        <v>SetName-KEY_01-digit_7.png</v>
+        <v>SetName-KEY_02-digit_8.png</v>
       </c>
       <c r="H111" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_7</v>
+        <v>InputEventMap.KEY_8</v>
       </c>
       <c r="I111" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
       <c r="A112" t="s">
         <v>27</v>
       </c>
       <c r="B112" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C112" t="s">
         <v>144</v>
       </c>
       <c r="D112">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E112" t="str">
         <f t="shared" si="81"/>
-        <v>digit_8</v>
+        <v>digit_9</v>
       </c>
       <c r="F112" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_02</v>
+        <v>KEY_03</v>
       </c>
       <c r="G112" t="str">
         <f t="shared" si="83"/>
-        <v>SetName-KEY_02-digit_8.png</v>
+        <v>SetName-KEY_03-digit_9.png</v>
       </c>
       <c r="H112" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_8</v>
+        <v>InputEventMap.KEY_9</v>
       </c>
       <c r="I112" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
       <c r="A113" t="s">
         <v>27</v>
       </c>
       <c r="B113" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C113" t="s">
         <v>145</v>
       </c>
       <c r="D113">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E113" t="str">
         <f t="shared" si="81"/>
-        <v>digit_9</v>
+        <v>back_space</v>
       </c>
       <c r="F113" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_03</v>
+        <v>KEY_09</v>
       </c>
       <c r="G113" t="str">
         <f t="shared" si="83"/>
-        <v>SetName-KEY_03-digit_9.png</v>
+        <v>SetName-KEY_09-back_space.png</v>
       </c>
       <c r="H113" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_9</v>
+        <v>InputEventMap.KEY_BACKSPACE</v>
       </c>
       <c r="I113" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_BACKSPACE,</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
       <c r="A114" t="s">
         <v>27</v>
       </c>
       <c r="B114" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C114" t="s">
         <v>146</v>
       </c>
       <c r="D114">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E114" t="str">
         <f t="shared" si="81"/>
-        <v>back_space</v>
+        <v>enter</v>
       </c>
       <c r="F114" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_05</v>
+        <v>KEY_0E</v>
       </c>
       <c r="G114" t="str">
         <f t="shared" si="83"/>
-        <v>SetName-KEY_05-back_space.png</v>
+        <v>SetName-KEY_0E-enter.png</v>
       </c>
       <c r="H114" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_BACKSPACE</v>
+        <v>InputEventMap.KEY_ENTER</v>
       </c>
       <c r="I114" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
       <c r="A115" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B115" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="C115" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D115">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E115" t="str">
-        <f t="shared" si="81"/>
-        <v>enter</v>
-      </c>
-      <c r="F115" t="str">
-        <f t="shared" si="82"/>
-        <v>KEY_0E</v>
-      </c>
-      <c r="G115" t="str">
-        <f t="shared" si="83"/>
-        <v>SetName-KEY_0E-enter.png</v>
-      </c>
-      <c r="H115" t="str">
-        <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_ENTER</v>
-      </c>
-      <c r="I115" t="str">
-        <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A116" t="s">
-        <v>27</v>
-      </c>
-      <c r="B116" t="s">
-        <v>75</v>
-      </c>
-      <c r="C116" t="s">
-        <v>148</v>
-      </c>
-      <c r="D116">
-        <v>9</v>
-      </c>
-      <c r="E116" t="str">
-        <f t="shared" si="81"/>
-        <v>jump_next</v>
-      </c>
-      <c r="F116" t="str">
-        <f t="shared" si="82"/>
-        <v>KEY_09</v>
-      </c>
-      <c r="G116" t="str">
-        <f t="shared" si="83"/>
-        <v>SetName-KEY_09-jump_next.png</v>
-      </c>
-      <c r="H116" t="str">
-        <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_TAB</v>
-      </c>
-      <c r="I116" t="str">
-        <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A117" t="s">
-        <v>26</v>
-      </c>
-      <c r="B117" t="s">
-        <v>100</v>
-      </c>
-      <c r="C117" t="s">
-        <v>150</v>
-      </c>
-      <c r="D117">
-        <v>0</v>
-      </c>
-      <c r="E117" t="str">
-        <f t="shared" ref="E117" si="106">LOWER(
+        <f t="shared" ref="E115" si="106">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B117, FIND(" = InputEventMap", B117) - 1),
+      LEFT(B115, FIND(" = InputEventMap", B115) - 1),
       CHAR(160),
       " "
     )
@@ -5123,520 +5049,486 @@
 )</f>
         <v>screen</v>
       </c>
-      <c r="F117" t="str">
-        <f t="shared" ref="F117" si="107">"KEY_" &amp; CHOOSE(
-    D117+1,
+      <c r="F115" t="str">
+        <f t="shared" ref="F115" si="107">"KEY_" &amp; CHOOSE(
+    D115+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_00</v>
       </c>
+      <c r="G115" t="str">
+        <f t="shared" ref="G115" si="108">_xlfn.CONCAT(A115, "-", F115, "-", E115, ".png")</f>
+        <v>SetTime-KEY_00-screen.png</v>
+      </c>
+      <c r="H115" t="str">
+        <f t="shared" ref="H115" si="109">MID(B115, FIND("InputEventMap", B115), LEN(B115))</f>
+        <v>InputEventMap.KEY_ASTERISK</v>
+      </c>
+      <c r="I115" t="str">
+        <f t="shared" ref="I115" si="110">_xlfn.CONCAT("StreamdeckInput.", F115, ": ", H115, ",")</f>
+        <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
+      <c r="A116" t="s">
+        <v>26</v>
+      </c>
+      <c r="B116" t="s">
+        <v>4</v>
+      </c>
+      <c r="C116" t="s">
+        <v>88</v>
+      </c>
+      <c r="D116">
+        <v>4</v>
+      </c>
+      <c r="E116" t="str">
+        <f t="shared" si="81"/>
+        <v>help</v>
+      </c>
+      <c r="F116" t="str">
+        <f t="shared" si="82"/>
+        <v>KEY_04</v>
+      </c>
+      <c r="G116" t="str">
+        <f t="shared" si="83"/>
+        <v>SetTime-KEY_04-help.png</v>
+      </c>
+      <c r="H116" t="str">
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
+      </c>
+      <c r="I116" t="str">
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
+      <c r="A117" t="s">
+        <v>26</v>
+      </c>
+      <c r="B117" t="s">
+        <v>63</v>
+      </c>
+      <c r="C117" t="s">
+        <v>135</v>
+      </c>
+      <c r="D117">
+        <v>10</v>
+      </c>
+      <c r="E117" t="str">
+        <f t="shared" si="81"/>
+        <v>digit_0</v>
+      </c>
+      <c r="F117" t="str">
+        <f t="shared" si="82"/>
+        <v>KEY_0A</v>
+      </c>
       <c r="G117" t="str">
-        <f t="shared" ref="G117" si="108">_xlfn.CONCAT(A117, "-", F117, "-", E117, ".png")</f>
-        <v>SetTime-KEY_00-screen.png</v>
+        <f t="shared" si="83"/>
+        <v>SetTime-KEY_0A-digit_0.png</v>
       </c>
       <c r="H117" t="str">
-        <f t="shared" ref="H117" si="109">MID(B117, FIND("InputEventMap", B117), LEN(B117))</f>
-        <v>InputEventMap.KEY_ASTERISK</v>
+        <f t="shared" si="84"/>
+        <v>InputEventMap.KEY_0</v>
       </c>
       <c r="I117" t="str">
-        <f t="shared" ref="I117" si="110">_xlfn.CONCAT("StreamdeckInput.", F117, ": ", H117, ",")</f>
-        <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
+        <f t="shared" si="85"/>
+        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
       <c r="A118" t="s">
         <v>26</v>
       </c>
       <c r="B118" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="C118" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="D118">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E118" t="str">
         <f t="shared" si="81"/>
-        <v>help</v>
+        <v>digit_1</v>
       </c>
       <c r="F118" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_04</v>
+        <v>KEY_0B</v>
       </c>
       <c r="G118" t="str">
         <f t="shared" si="83"/>
-        <v>SetTime-KEY_04-help.png</v>
+        <v>SetTime-KEY_0B-digit_1.png</v>
       </c>
       <c r="H118" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
+        <v>InputEventMap.KEY_1</v>
       </c>
       <c r="I118" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
       <c r="A119" t="s">
         <v>26</v>
       </c>
       <c r="B119" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C119" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D119">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E119" t="str">
         <f t="shared" si="81"/>
-        <v>digit_0</v>
+        <v>digit_2</v>
       </c>
       <c r="F119" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_0A</v>
+        <v>KEY_0C</v>
       </c>
       <c r="G119" t="str">
         <f t="shared" si="83"/>
-        <v>SetTime-KEY_0A-digit_0.png</v>
+        <v>SetTime-KEY_0C-digit_2.png</v>
       </c>
       <c r="H119" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_0</v>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I119" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_0A: InputEventMap.KEY_0,</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
       <c r="A120" t="s">
         <v>26</v>
       </c>
       <c r="B120" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C120" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D120">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E120" t="str">
         <f t="shared" si="81"/>
-        <v>digit_1</v>
+        <v>digit_3</v>
       </c>
       <c r="F120" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_0B</v>
+        <v>KEY_0D</v>
       </c>
       <c r="G120" t="str">
         <f t="shared" si="83"/>
-        <v>SetTime-KEY_0B-digit_1.png</v>
+        <v>SetTime-KEY_0D-digit_3.png</v>
       </c>
       <c r="H120" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_1</v>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I120" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_1,</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
       <c r="A121" t="s">
         <v>26</v>
       </c>
       <c r="B121" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C121" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D121">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E121" t="str">
         <f t="shared" si="81"/>
-        <v>digit_2</v>
+        <v>digit_4</v>
       </c>
       <c r="F121" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_0C</v>
+        <v>KEY_06</v>
       </c>
       <c r="G121" t="str">
         <f t="shared" si="83"/>
-        <v>SetTime-KEY_0C-digit_2.png</v>
+        <v>SetTime-KEY_06-digit_4.png</v>
       </c>
       <c r="H121" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_2</v>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I121" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_2,</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
       <c r="A122" t="s">
         <v>26</v>
       </c>
       <c r="B122" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C122" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D122">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E122" t="str">
         <f t="shared" si="81"/>
-        <v>digit_3</v>
+        <v>digit_5</v>
       </c>
       <c r="F122" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_0D</v>
+        <v>KEY_07</v>
       </c>
       <c r="G122" t="str">
         <f t="shared" si="83"/>
-        <v>SetTime-KEY_0D-digit_3.png</v>
+        <v>SetTime-KEY_07-digit_5.png</v>
       </c>
       <c r="H122" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_3</v>
+        <v>InputEventMap.KEY_5</v>
       </c>
       <c r="I122" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_0D: InputEventMap.KEY_3,</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
       <c r="A123" t="s">
         <v>26</v>
       </c>
       <c r="B123" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C123" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D123">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E123" t="str">
         <f t="shared" si="81"/>
-        <v>digit_4</v>
+        <v>digit_6</v>
       </c>
       <c r="F123" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_06</v>
+        <v>KEY_08</v>
       </c>
       <c r="G123" t="str">
         <f t="shared" si="83"/>
-        <v>SetTime-KEY_06-digit_4.png</v>
+        <v>SetTime-KEY_08-digit_6.png</v>
       </c>
       <c r="H123" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_4</v>
+        <v>InputEventMap.KEY_6</v>
       </c>
       <c r="I123" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
       <c r="A124" t="s">
         <v>26</v>
       </c>
       <c r="B124" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C124" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D124">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E124" t="str">
         <f t="shared" si="81"/>
-        <v>digit_5</v>
+        <v>digit_7</v>
       </c>
       <c r="F124" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_07</v>
+        <v>KEY_01</v>
       </c>
       <c r="G124" t="str">
         <f t="shared" si="83"/>
-        <v>SetTime-KEY_07-digit_5.png</v>
+        <v>SetTime-KEY_01-digit_7.png</v>
       </c>
       <c r="H124" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_5</v>
+        <v>InputEventMap.KEY_7</v>
       </c>
       <c r="I124" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_5,</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
       <c r="A125" t="s">
         <v>26</v>
       </c>
       <c r="B125" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C125" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D125">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E125" t="str">
         <f t="shared" si="81"/>
-        <v>digit_6</v>
+        <v>digit_8</v>
       </c>
       <c r="F125" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_08</v>
+        <v>KEY_02</v>
       </c>
       <c r="G125" t="str">
         <f t="shared" si="83"/>
-        <v>SetTime-KEY_08-digit_6.png</v>
+        <v>SetTime-KEY_02-digit_8.png</v>
       </c>
       <c r="H125" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_6</v>
+        <v>InputEventMap.KEY_8</v>
       </c>
       <c r="I125" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_08: InputEventMap.KEY_6,</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
       <c r="A126" t="s">
         <v>26</v>
       </c>
       <c r="B126" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C126" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D126">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E126" t="str">
         <f t="shared" si="81"/>
-        <v>digit_7</v>
+        <v>digit_9</v>
       </c>
       <c r="F126" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_01</v>
+        <v>KEY_03</v>
       </c>
       <c r="G126" t="str">
         <f t="shared" si="83"/>
-        <v>SetTime-KEY_01-digit_7.png</v>
+        <v>SetTime-KEY_03-digit_9.png</v>
       </c>
       <c r="H126" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_7</v>
+        <v>InputEventMap.KEY_9</v>
       </c>
       <c r="I126" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_7,</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
       <c r="A127" t="s">
         <v>26</v>
       </c>
       <c r="B127" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C127" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D127">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E127" t="str">
         <f t="shared" si="81"/>
-        <v>digit_8</v>
+        <v>back_space</v>
       </c>
       <c r="F127" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_02</v>
+        <v>KEY_09</v>
       </c>
       <c r="G127" t="str">
         <f t="shared" si="83"/>
-        <v>SetTime-KEY_02-digit_8.png</v>
+        <v>SetTime-KEY_09-back_space.png</v>
       </c>
       <c r="H127" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_8</v>
+        <v>InputEventMap.KEY_BACKSPACE</v>
       </c>
       <c r="I127" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_8,</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_BACKSPACE,</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
       <c r="A128" t="s">
         <v>26</v>
       </c>
       <c r="B128" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C128" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D128">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E128" t="str">
         <f t="shared" si="81"/>
-        <v>digit_9</v>
+        <v>enter</v>
       </c>
       <c r="F128" t="str">
         <f t="shared" si="82"/>
-        <v>KEY_03</v>
+        <v>KEY_0E</v>
       </c>
       <c r="G128" t="str">
         <f t="shared" si="83"/>
-        <v>SetTime-KEY_03-digit_9.png</v>
+        <v>SetTime-KEY_0E-enter.png</v>
       </c>
       <c r="H128" t="str">
         <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_9</v>
+        <v>InputEventMap.KEY_ENTER</v>
       </c>
       <c r="I128" t="str">
         <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_03: InputEventMap.KEY_9,</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9">
       <c r="A129" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B129" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="C129" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D129">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E129" t="str">
-        <f t="shared" si="81"/>
-        <v>back_space</v>
-      </c>
-      <c r="F129" t="str">
-        <f t="shared" si="82"/>
-        <v>KEY_05</v>
-      </c>
-      <c r="G129" t="str">
-        <f t="shared" si="83"/>
-        <v>SetTime-KEY_05-back_space.png</v>
-      </c>
-      <c r="H129" t="str">
-        <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_BACKSPACE</v>
-      </c>
-      <c r="I129" t="str">
-        <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_BACKSPACE,</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A130" t="s">
-        <v>26</v>
-      </c>
-      <c r="B130" t="s">
-        <v>74</v>
-      </c>
-      <c r="C130" t="s">
-        <v>147</v>
-      </c>
-      <c r="D130">
-        <v>14</v>
-      </c>
-      <c r="E130" t="str">
-        <f t="shared" si="81"/>
-        <v>enter</v>
-      </c>
-      <c r="F130" t="str">
-        <f t="shared" si="82"/>
-        <v>KEY_0E</v>
-      </c>
-      <c r="G130" t="str">
-        <f t="shared" si="83"/>
-        <v>SetTime-KEY_0E-enter.png</v>
-      </c>
-      <c r="H130" t="str">
-        <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_ENTER</v>
-      </c>
-      <c r="I130" t="str">
-        <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_ENTER,</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A131" t="s">
-        <v>26</v>
-      </c>
-      <c r="B131" t="s">
-        <v>75</v>
-      </c>
-      <c r="C131" t="s">
-        <v>148</v>
-      </c>
-      <c r="D131">
-        <v>9</v>
-      </c>
-      <c r="E131" t="str">
-        <f t="shared" si="81"/>
-        <v>jump_next</v>
-      </c>
-      <c r="F131" t="str">
-        <f t="shared" si="82"/>
-        <v>KEY_09</v>
-      </c>
-      <c r="G131" t="str">
-        <f t="shared" si="83"/>
-        <v>SetTime-KEY_09-jump_next.png</v>
-      </c>
-      <c r="H131" t="str">
-        <f t="shared" si="84"/>
-        <v>InputEventMap.KEY_TAB</v>
-      </c>
-      <c r="I131" t="str">
-        <f t="shared" si="85"/>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_TAB,</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A132" t="s">
-        <v>30</v>
-      </c>
-      <c r="B132" t="s">
-        <v>100</v>
-      </c>
-      <c r="C132" t="s">
-        <v>151</v>
-      </c>
-      <c r="D132">
-        <v>0</v>
-      </c>
-      <c r="E132" t="str">
-        <f t="shared" ref="E132" si="111">LOWER(
+        <f t="shared" ref="E129" si="111">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B132, FIND(" = InputEventMap", B132) - 1),
+      LEFT(B129, FIND(" = InputEventMap", B129) - 1),
       CHAR(160),
       " "
     )
@@ -5644,78 +5536,78 @@
 )</f>
         <v>screen</v>
       </c>
-      <c r="F132" t="str">
-        <f t="shared" ref="F132" si="112">"KEY_" &amp; CHOOSE(
-    D132+1,
+      <c r="F129" t="str">
+        <f t="shared" ref="F129" si="112">"KEY_" &amp; CHOOSE(
+    D129+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_00</v>
       </c>
-      <c r="G132" t="str">
-        <f t="shared" ref="G132" si="113">_xlfn.CONCAT(A132, "-", F132, "-", E132, ".png")</f>
+      <c r="G129" t="str">
+        <f t="shared" ref="G129" si="113">_xlfn.CONCAT(A129, "-", F129, "-", E129, ".png")</f>
         <v>StorageManagement-KEY_00-screen.png</v>
       </c>
-      <c r="H132" t="str">
-        <f t="shared" ref="H132" si="114">MID(B132, FIND("InputEventMap", B132), LEN(B132))</f>
+      <c r="H129" t="str">
+        <f t="shared" ref="H129" si="114">MID(B129, FIND("InputEventMap", B129), LEN(B129))</f>
         <v>InputEventMap.KEY_ASTERISK</v>
       </c>
-      <c r="I132" t="str">
-        <f t="shared" ref="I132" si="115">_xlfn.CONCAT("StreamdeckInput.", F132, ": ", H132, ",")</f>
+      <c r="I129" t="str">
+        <f t="shared" ref="I129" si="115">_xlfn.CONCAT("StreamdeckInput.", F129, ": ", H129, ",")</f>
         <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A133" t="s">
+    <row r="130" spans="1:9">
+      <c r="A130" t="s">
         <v>30</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B130" t="s">
         <v>4</v>
       </c>
-      <c r="C133" t="s">
-        <v>89</v>
-      </c>
-      <c r="D133">
+      <c r="C130" t="s">
+        <v>88</v>
+      </c>
+      <c r="D130">
         <v>4</v>
       </c>
-      <c r="E133" t="str">
+      <c r="E130" t="str">
         <f t="shared" si="81"/>
         <v>help</v>
       </c>
-      <c r="F133" t="str">
+      <c r="F130" t="str">
         <f t="shared" si="82"/>
         <v>KEY_04</v>
       </c>
-      <c r="G133" t="str">
+      <c r="G130" t="str">
         <f t="shared" si="83"/>
         <v>StorageManagement-KEY_04-help.png</v>
       </c>
-      <c r="H133" t="str">
+      <c r="H130" t="str">
         <f t="shared" si="84"/>
         <v>InputEventMap.KEY_ASTERISK</v>
       </c>
-      <c r="I133" t="str">
+      <c r="I130" t="str">
         <f t="shared" si="85"/>
         <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A134" t="s">
+    <row r="131" spans="1:9">
+      <c r="A131" t="s">
         <v>30</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B131" t="s">
         <v>5</v>
       </c>
-      <c r="C134" t="s">
-        <v>90</v>
-      </c>
-      <c r="D134">
+      <c r="C131" t="s">
+        <v>89</v>
+      </c>
+      <c r="D131">
         <v>9</v>
       </c>
-      <c r="E134" t="str">
-        <f t="shared" ref="E134:E149" si="116">LOWER(
+      <c r="E131" t="str">
+        <f t="shared" ref="E131:E146" si="116">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B134, FIND(" = InputEventMap", B134) - 1),
+      LEFT(B131, FIND(" = InputEventMap", B131) - 1),
       CHAR(160),
       " "
     )
@@ -5723,282 +5615,282 @@
 )</f>
         <v>menu</v>
       </c>
-      <c r="F134" t="str">
-        <f t="shared" ref="F134:F149" si="117">"KEY_" &amp; CHOOSE(
-    D134+1,
+      <c r="F131" t="str">
+        <f t="shared" ref="F131:F146" si="117">"KEY_" &amp; CHOOSE(
+    D131+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_09</v>
       </c>
+      <c r="G131" t="str">
+        <f t="shared" ref="G131:G146" si="118">_xlfn.CONCAT(A131, "-", F131, "-", E131, ".png")</f>
+        <v>StorageManagement-KEY_09-menu.png</v>
+      </c>
+      <c r="H131" t="str">
+        <f t="shared" ref="H131:H146" si="119">MID(B131, FIND("InputEventMap", B131), LEN(B131))</f>
+        <v>InputEventMap.KEY_5</v>
+      </c>
+      <c r="I131" t="str">
+        <f t="shared" ref="I131:I146" si="120">_xlfn.CONCAT("StreamdeckInput.", F131, ": ", H131, ",")</f>
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
+      <c r="A132" t="s">
+        <v>30</v>
+      </c>
+      <c r="B132" t="s">
+        <v>75</v>
+      </c>
+      <c r="C132" t="s">
+        <v>150</v>
+      </c>
+      <c r="D132">
+        <v>5</v>
+      </c>
+      <c r="E132" t="str">
+        <f t="shared" si="116"/>
+        <v>disconnect_storage</v>
+      </c>
+      <c r="F132" t="str">
+        <f t="shared" si="117"/>
+        <v>KEY_05</v>
+      </c>
+      <c r="G132" t="str">
+        <f t="shared" si="118"/>
+        <v>StorageManagement-KEY_05-disconnect_storage.png</v>
+      </c>
+      <c r="H132" t="str">
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_0</v>
+      </c>
+      <c r="I132" t="str">
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_0,</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
+      <c r="A133" t="s">
+        <v>30</v>
+      </c>
+      <c r="B133" t="s">
+        <v>76</v>
+      </c>
+      <c r="C133" t="s">
+        <v>92</v>
+      </c>
+      <c r="D133">
+        <v>1</v>
+      </c>
+      <c r="E133" t="str">
+        <f t="shared" si="116"/>
+        <v>detect_rc1</v>
+      </c>
+      <c r="F133" t="str">
+        <f t="shared" si="117"/>
+        <v>KEY_01</v>
+      </c>
+      <c r="G133" t="str">
+        <f t="shared" si="118"/>
+        <v>StorageManagement-KEY_01-detect_rc1.png</v>
+      </c>
+      <c r="H133" t="str">
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_1</v>
+      </c>
+      <c r="I133" t="str">
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_1,</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9">
+      <c r="A134" t="s">
+        <v>30</v>
+      </c>
+      <c r="B134" t="s">
+        <v>77</v>
+      </c>
+      <c r="C134" t="s">
+        <v>92</v>
+      </c>
+      <c r="D134">
+        <v>2</v>
+      </c>
+      <c r="E134" t="str">
+        <f t="shared" si="116"/>
+        <v>detect_rc2</v>
+      </c>
+      <c r="F134" t="str">
+        <f t="shared" si="117"/>
+        <v>KEY_02</v>
+      </c>
       <c r="G134" t="str">
-        <f t="shared" ref="G134:G149" si="118">_xlfn.CONCAT(A134, "-", F134, "-", E134, ".png")</f>
-        <v>StorageManagement-KEY_09-menu.png</v>
+        <f t="shared" si="118"/>
+        <v>StorageManagement-KEY_02-detect_rc2.png</v>
       </c>
       <c r="H134" t="str">
-        <f t="shared" ref="H134:H149" si="119">MID(B134, FIND("InputEventMap", B134), LEN(B134))</f>
-        <v>InputEventMap.KEY_5</v>
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I134" t="str">
-        <f t="shared" ref="I134:I149" si="120">_xlfn.CONCAT("StreamdeckInput.", F134, ": ", H134, ",")</f>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_5,</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_3,</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9">
       <c r="A135" t="s">
         <v>30</v>
       </c>
       <c r="B135" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C135" t="s">
-        <v>152</v>
+        <v>93</v>
       </c>
       <c r="D135">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E135" t="str">
         <f t="shared" si="116"/>
-        <v>disconnect_storage</v>
+        <v>format_rc1</v>
       </c>
       <c r="F135" t="str">
         <f t="shared" si="117"/>
-        <v>KEY_05</v>
+        <v>KEY_06</v>
       </c>
       <c r="G135" t="str">
         <f t="shared" si="118"/>
-        <v>StorageManagement-KEY_05-disconnect_storage.png</v>
+        <v>StorageManagement-KEY_06-format_rc1.png</v>
       </c>
       <c r="H135" t="str">
         <f t="shared" si="119"/>
-        <v>InputEventMap.KEY_0</v>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I135" t="str">
         <f t="shared" si="120"/>
-        <v>StreamdeckInput.KEY_05: InputEventMap.KEY_0,</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9">
       <c r="A136" t="s">
         <v>30</v>
       </c>
       <c r="B136" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C136" t="s">
         <v>93</v>
       </c>
       <c r="D136">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E136" t="str">
         <f t="shared" si="116"/>
-        <v>detect_rc1</v>
+        <v>format_rc2</v>
       </c>
       <c r="F136" t="str">
         <f t="shared" si="117"/>
-        <v>KEY_01</v>
+        <v>KEY_07</v>
       </c>
       <c r="G136" t="str">
         <f t="shared" si="118"/>
-        <v>StorageManagement-KEY_01-detect_rc1.png</v>
+        <v>StorageManagement-KEY_07-format_rc2.png</v>
       </c>
       <c r="H136" t="str">
         <f t="shared" si="119"/>
-        <v>InputEventMap.KEY_1</v>
+        <v>InputEventMap.KEY_6</v>
       </c>
       <c r="I136" t="str">
         <f t="shared" si="120"/>
-        <v>StreamdeckInput.KEY_01: InputEventMap.KEY_1,</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_6,</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9">
       <c r="A137" t="s">
         <v>30</v>
       </c>
       <c r="B137" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C137" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D137">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E137" t="str">
         <f t="shared" si="116"/>
-        <v>detect_rc2</v>
+        <v>clean_rc1</v>
       </c>
       <c r="F137" t="str">
         <f t="shared" si="117"/>
-        <v>KEY_02</v>
+        <v>KEY_0B</v>
       </c>
       <c r="G137" t="str">
         <f t="shared" si="118"/>
-        <v>StorageManagement-KEY_02-detect_rc2.png</v>
+        <v>StorageManagement-KEY_0B-clean_rc1.png</v>
       </c>
       <c r="H137" t="str">
         <f t="shared" si="119"/>
-        <v>InputEventMap.KEY_3</v>
+        <v>InputEventMap.KEY_7</v>
       </c>
       <c r="I137" t="str">
         <f t="shared" si="120"/>
-        <v>StreamdeckInput.KEY_02: InputEventMap.KEY_3,</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_7,</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9">
       <c r="A138" t="s">
         <v>30</v>
       </c>
       <c r="B138" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C138" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D138">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E138" t="str">
         <f t="shared" si="116"/>
-        <v>format_rc1</v>
+        <v>clean_rc2</v>
       </c>
       <c r="F138" t="str">
         <f t="shared" si="117"/>
-        <v>KEY_06</v>
+        <v>KEY_0C</v>
       </c>
       <c r="G138" t="str">
         <f t="shared" si="118"/>
-        <v>StorageManagement-KEY_06-format_rc1.png</v>
+        <v>StorageManagement-KEY_0C-clean_rc2.png</v>
       </c>
       <c r="H138" t="str">
         <f t="shared" si="119"/>
-        <v>InputEventMap.KEY_4</v>
+        <v>InputEventMap.KEY_9</v>
       </c>
       <c r="I138" t="str">
         <f t="shared" si="120"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_4,</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_9,</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9">
       <c r="A139" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="B139" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="C139" t="s">
-        <v>94</v>
+        <v>151</v>
       </c>
       <c r="D139">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E139" t="str">
-        <f t="shared" si="116"/>
-        <v>format_rc2</v>
-      </c>
-      <c r="F139" t="str">
-        <f t="shared" si="117"/>
-        <v>KEY_07</v>
-      </c>
-      <c r="G139" t="str">
-        <f t="shared" si="118"/>
-        <v>StorageManagement-KEY_07-format_rc2.png</v>
-      </c>
-      <c r="H139" t="str">
-        <f t="shared" si="119"/>
-        <v>InputEventMap.KEY_6</v>
-      </c>
-      <c r="I139" t="str">
-        <f t="shared" si="120"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_6,</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A140" t="s">
-        <v>30</v>
-      </c>
-      <c r="B140" t="s">
-        <v>81</v>
-      </c>
-      <c r="C140" t="s">
-        <v>97</v>
-      </c>
-      <c r="D140">
-        <v>11</v>
-      </c>
-      <c r="E140" t="str">
-        <f t="shared" si="116"/>
-        <v>clean_rc1</v>
-      </c>
-      <c r="F140" t="str">
-        <f t="shared" si="117"/>
-        <v>KEY_0B</v>
-      </c>
-      <c r="G140" t="str">
-        <f t="shared" si="118"/>
-        <v>StorageManagement-KEY_0B-clean_rc1.png</v>
-      </c>
-      <c r="H140" t="str">
-        <f t="shared" si="119"/>
-        <v>InputEventMap.KEY_7</v>
-      </c>
-      <c r="I140" t="str">
-        <f t="shared" si="120"/>
-        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_7,</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A141" t="s">
-        <v>30</v>
-      </c>
-      <c r="B141" t="s">
-        <v>82</v>
-      </c>
-      <c r="C141" t="s">
-        <v>97</v>
-      </c>
-      <c r="D141">
-        <v>12</v>
-      </c>
-      <c r="E141" t="str">
-        <f t="shared" si="116"/>
-        <v>clean_rc2</v>
-      </c>
-      <c r="F141" t="str">
-        <f t="shared" si="117"/>
-        <v>KEY_0C</v>
-      </c>
-      <c r="G141" t="str">
-        <f t="shared" si="118"/>
-        <v>StorageManagement-KEY_0C-clean_rc2.png</v>
-      </c>
-      <c r="H141" t="str">
-        <f t="shared" si="119"/>
-        <v>InputEventMap.KEY_9</v>
-      </c>
-      <c r="I141" t="str">
-        <f t="shared" si="120"/>
-        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_9,</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A142" t="s">
-        <v>8</v>
-      </c>
-      <c r="B142" t="s">
-        <v>100</v>
-      </c>
-      <c r="C142" t="s">
-        <v>153</v>
-      </c>
-      <c r="D142">
-        <v>0</v>
-      </c>
-      <c r="E142" t="str">
-        <f t="shared" ref="E142" si="121">LOWER(
+        <f t="shared" ref="E139" si="121">LOWER(
   TRIM(
     SUBSTITUTE(
-      LEFT(B142, FIND(" = InputEventMap", B142) - 1),
+      LEFT(B139, FIND(" = InputEventMap", B139) - 1),
       CHAR(160),
       " "
     )
@@ -6006,266 +5898,266 @@
 )</f>
         <v>screen</v>
       </c>
-      <c r="F142" t="str">
-        <f t="shared" ref="F142" si="122">"KEY_" &amp; CHOOSE(
-    D142+1,
+      <c r="F139" t="str">
+        <f t="shared" ref="F139" si="122">"KEY_" &amp; CHOOSE(
+    D139+1,
     "00","01","02","03","04","05","06","07","08","09","0A","0B","0C","0D","0E"
 )</f>
         <v>KEY_00</v>
       </c>
+      <c r="G139" t="str">
+        <f t="shared" ref="G139" si="123">_xlfn.CONCAT(A139, "-", F139, "-", E139, ".png")</f>
+        <v>System-KEY_00-screen.png</v>
+      </c>
+      <c r="H139" t="str">
+        <f t="shared" ref="H139" si="124">MID(B139, FIND("InputEventMap", B139), LEN(B139))</f>
+        <v>InputEventMap.KEY_ASTERISK</v>
+      </c>
+      <c r="I139" t="str">
+        <f t="shared" ref="I139" si="125">_xlfn.CONCAT("StreamdeckInput.", F139, ": ", H139, ",")</f>
+        <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9">
+      <c r="A140" t="s">
+        <v>8</v>
+      </c>
+      <c r="B140" t="s">
+        <v>4</v>
+      </c>
+      <c r="C140" t="s">
+        <v>88</v>
+      </c>
+      <c r="D140">
+        <v>4</v>
+      </c>
+      <c r="E140" t="str">
+        <f t="shared" si="116"/>
+        <v>help</v>
+      </c>
+      <c r="F140" t="str">
+        <f t="shared" si="117"/>
+        <v>KEY_04</v>
+      </c>
+      <c r="G140" t="str">
+        <f t="shared" si="118"/>
+        <v>System-KEY_04-help.png</v>
+      </c>
+      <c r="H140" t="str">
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_ASTERISK</v>
+      </c>
+      <c r="I140" t="str">
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9">
+      <c r="A141" t="s">
+        <v>8</v>
+      </c>
+      <c r="B141" t="s">
+        <v>82</v>
+      </c>
+      <c r="C141" t="s">
+        <v>97</v>
+      </c>
+      <c r="D141">
+        <v>9</v>
+      </c>
+      <c r="E141" t="str">
+        <f t="shared" si="116"/>
+        <v>select_main</v>
+      </c>
+      <c r="F141" t="str">
+        <f t="shared" si="117"/>
+        <v>KEY_09</v>
+      </c>
+      <c r="G141" t="str">
+        <f t="shared" si="118"/>
+        <v>System-KEY_09-select_main.png</v>
+      </c>
+      <c r="H141" t="str">
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_1</v>
+      </c>
+      <c r="I141" t="str">
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_1,</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9">
+      <c r="A142" t="s">
+        <v>8</v>
+      </c>
+      <c r="B142" t="s">
+        <v>83</v>
+      </c>
+      <c r="C142" t="s">
+        <v>152</v>
+      </c>
+      <c r="D142">
+        <v>6</v>
+      </c>
+      <c r="E142" t="str">
+        <f t="shared" si="116"/>
+        <v>select_language</v>
+      </c>
+      <c r="F142" t="str">
+        <f t="shared" si="117"/>
+        <v>KEY_06</v>
+      </c>
       <c r="G142" t="str">
-        <f t="shared" ref="G142" si="123">_xlfn.CONCAT(A142, "-", F142, "-", E142, ".png")</f>
-        <v>System-KEY_00-screen.png</v>
+        <f t="shared" si="118"/>
+        <v>System-KEY_06-select_language.png</v>
       </c>
       <c r="H142" t="str">
-        <f t="shared" ref="H142" si="124">MID(B142, FIND("InputEventMap", B142), LEN(B142))</f>
-        <v>InputEventMap.KEY_ASTERISK</v>
+        <f t="shared" si="119"/>
+        <v>InputEventMap.KEY_2</v>
       </c>
       <c r="I142" t="str">
-        <f t="shared" ref="I142" si="125">_xlfn.CONCAT("StreamdeckInput.", F142, ": ", H142, ",")</f>
-        <v>StreamdeckInput.KEY_00: InputEventMap.KEY_ASTERISK,</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
+        <f t="shared" si="120"/>
+        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9">
       <c r="A143" t="s">
         <v>8</v>
       </c>
       <c r="B143" t="s">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="C143" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="D143">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E143" t="str">
         <f t="shared" si="116"/>
-        <v>help</v>
+        <v>select_storage</v>
       </c>
       <c r="F143" t="str">
         <f t="shared" si="117"/>
-        <v>KEY_04</v>
+        <v>KEY_07</v>
       </c>
       <c r="G143" t="str">
         <f t="shared" si="118"/>
-        <v>System-KEY_04-help.png</v>
+        <v>System-KEY_07-select_storage.png</v>
       </c>
       <c r="H143" t="str">
         <f t="shared" si="119"/>
-        <v>InputEventMap.KEY_ASTERISK</v>
+        <v>InputEventMap.KEY_3</v>
       </c>
       <c r="I143" t="str">
         <f t="shared" si="120"/>
-        <v>StreamdeckInput.KEY_04: InputEventMap.KEY_ASTERISK,</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9">
       <c r="A144" t="s">
         <v>8</v>
       </c>
       <c r="B144" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C144" t="s">
-        <v>98</v>
+        <v>154</v>
       </c>
       <c r="D144">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E144" t="str">
         <f t="shared" si="116"/>
-        <v>select_main</v>
+        <v>set_date</v>
       </c>
       <c r="F144" t="str">
         <f t="shared" si="117"/>
-        <v>KEY_09</v>
+        <v>KEY_0B</v>
       </c>
       <c r="G144" t="str">
         <f t="shared" si="118"/>
-        <v>System-KEY_09-select_main.png</v>
+        <v>System-KEY_0B-set_date.png</v>
       </c>
       <c r="H144" t="str">
         <f t="shared" si="119"/>
-        <v>InputEventMap.KEY_1</v>
+        <v>InputEventMap.KEY_4</v>
       </c>
       <c r="I144" t="str">
         <f t="shared" si="120"/>
-        <v>StreamdeckInput.KEY_09: InputEventMap.KEY_1,</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_4,</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9">
       <c r="A145" t="s">
         <v>8</v>
       </c>
       <c r="B145" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C145" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D145">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E145" t="str">
         <f t="shared" si="116"/>
-        <v>select_language</v>
+        <v>set_time</v>
       </c>
       <c r="F145" t="str">
         <f t="shared" si="117"/>
-        <v>KEY_06</v>
+        <v>KEY_0C</v>
       </c>
       <c r="G145" t="str">
         <f t="shared" si="118"/>
-        <v>System-KEY_06-select_language.png</v>
+        <v>System-KEY_0C-set_time.png</v>
       </c>
       <c r="H145" t="str">
         <f t="shared" si="119"/>
-        <v>InputEventMap.KEY_2</v>
+        <v>InputEventMap.KEY_6</v>
       </c>
       <c r="I145" t="str">
         <f t="shared" si="120"/>
-        <v>StreamdeckInput.KEY_06: InputEventMap.KEY_2,</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
+        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_6,</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9">
       <c r="A146" t="s">
         <v>8</v>
       </c>
       <c r="B146" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="C146" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
       <c r="D146">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E146" t="str">
         <f t="shared" si="116"/>
-        <v>select_storage</v>
+        <v>stop_system</v>
       </c>
       <c r="F146" t="str">
         <f t="shared" si="117"/>
-        <v>KEY_07</v>
+        <v>KEY_0E</v>
       </c>
       <c r="G146" t="str">
         <f t="shared" si="118"/>
-        <v>System-KEY_07-select_storage.png</v>
+        <v>System-KEY_0E-stop_system.png</v>
       </c>
       <c r="H146" t="str">
         <f t="shared" si="119"/>
-        <v>InputEventMap.KEY_3</v>
+        <v>InputEventMap.KEY_9</v>
       </c>
       <c r="I146" t="str">
         <f t="shared" si="120"/>
-        <v>StreamdeckInput.KEY_07: InputEventMap.KEY_3,</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A147" t="s">
-        <v>8</v>
-      </c>
-      <c r="B147" t="s">
-        <v>86</v>
-      </c>
-      <c r="C147" t="s">
-        <v>156</v>
-      </c>
-      <c r="D147">
-        <v>11</v>
-      </c>
-      <c r="E147" t="str">
-        <f t="shared" si="116"/>
-        <v>set_date</v>
-      </c>
-      <c r="F147" t="str">
-        <f t="shared" si="117"/>
-        <v>KEY_0B</v>
-      </c>
-      <c r="G147" t="str">
-        <f t="shared" si="118"/>
-        <v>System-KEY_0B-set_date.png</v>
-      </c>
-      <c r="H147" t="str">
-        <f t="shared" si="119"/>
-        <v>InputEventMap.KEY_4</v>
-      </c>
-      <c r="I147" t="str">
-        <f t="shared" si="120"/>
-        <v>StreamdeckInput.KEY_0B: InputEventMap.KEY_4,</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A148" t="s">
-        <v>8</v>
-      </c>
-      <c r="B148" t="s">
-        <v>87</v>
-      </c>
-      <c r="C148" t="s">
-        <v>157</v>
-      </c>
-      <c r="D148">
-        <v>12</v>
-      </c>
-      <c r="E148" t="str">
-        <f t="shared" si="116"/>
-        <v>set_time</v>
-      </c>
-      <c r="F148" t="str">
-        <f t="shared" si="117"/>
-        <v>KEY_0C</v>
-      </c>
-      <c r="G148" t="str">
-        <f t="shared" si="118"/>
-        <v>System-KEY_0C-set_time.png</v>
-      </c>
-      <c r="H148" t="str">
-        <f t="shared" si="119"/>
-        <v>InputEventMap.KEY_6</v>
-      </c>
-      <c r="I148" t="str">
-        <f t="shared" si="120"/>
-        <v>StreamdeckInput.KEY_0C: InputEventMap.KEY_6,</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A149" t="s">
-        <v>8</v>
-      </c>
-      <c r="B149" t="s">
-        <v>45</v>
-      </c>
-      <c r="C149" t="s">
-        <v>104</v>
-      </c>
-      <c r="D149">
-        <v>14</v>
-      </c>
-      <c r="E149" t="str">
-        <f t="shared" si="116"/>
-        <v>stop_system</v>
-      </c>
-      <c r="F149" t="str">
-        <f t="shared" si="117"/>
-        <v>KEY_0E</v>
-      </c>
-      <c r="G149" t="str">
-        <f t="shared" si="118"/>
-        <v>System-KEY_0E-stop_system.png</v>
-      </c>
-      <c r="H149" t="str">
-        <f t="shared" si="119"/>
-        <v>InputEventMap.KEY_9</v>
-      </c>
-      <c r="I149" t="str">
-        <f t="shared" si="120"/>
         <v>StreamdeckInput.KEY_0E: InputEventMap.KEY_9,</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I149" xr:uid="{47861C0B-96C3-4FC0-B828-7FD785B358D7}"/>
+  <autoFilter ref="A1:I146" xr:uid="{47861C0B-96C3-4FC0-B828-7FD785B358D7}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>